<commit_message>
CBSLine evaluation with MFS of 176Byte
</commit_message>
<xml_diff>
--- a/src/main/java/org/networkcalculus/dnc/demos/Eval_CBSLine/Eval_CBSLine_Results.xlsx
+++ b/src/main/java/org/networkcalculus/dnc/demos/Eval_CBSLine/Eval_CBSLine_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ForceXX\Documents\Studium\FAU_Informatik_Master\FS5\Masterarbeit\Network_Calculus_in_TSN\DNC\IntelliJ\src\main\java\org\networkcalculus\dnc\demos\Eval_CBSLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD402568-3D85-4EA2-B29A-5D19DD22F457}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D32D6A-D893-4F9E-AFEA-73E15F1A9249}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1824" windowWidth="46080" windowHeight="22152" activeTab="1" xr2:uid="{76093B85-C4EA-4FAC-BB07-8F5ADEBC9C5C}"/>
+    <workbookView xWindow="0" yWindow="2280" windowWidth="46080" windowHeight="22152" activeTab="1" xr2:uid="{76093B85-C4EA-4FAC-BB07-8F5ADEBC9C5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="34">
   <si>
     <t>f1</t>
   </si>
@@ -911,7 +911,7 @@
   <dimension ref="B3:W62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1636,8 +1636,12 @@
         <v>100000000</v>
       </c>
       <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
-      <c r="T35" s="12"/>
+      <c r="S35" s="1">
+        <v>1328.70144</v>
+      </c>
+      <c r="T35" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="U35" s="11"/>
       <c r="V35" s="11"/>
       <c r="W35" s="14"/>
@@ -1741,13 +1745,27 @@
       <c r="M41" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
-      <c r="T41" s="15"/>
+      <c r="N41" s="15">
+        <v>2.051340288E-4</v>
+      </c>
+      <c r="O41" s="15">
+        <v>2.2524702719999999E-4</v>
+      </c>
+      <c r="P41" s="15">
+        <v>2.4536002560000001E-4</v>
+      </c>
+      <c r="Q41" s="15">
+        <v>2.6547302400000002E-4</v>
+      </c>
+      <c r="R41" s="15">
+        <v>2.8558602239999999E-4</v>
+      </c>
+      <c r="S41" s="15">
+        <v>2.5049902080000002E-4</v>
+      </c>
+      <c r="T41" s="15">
+        <v>1.4772991487999999E-3</v>
+      </c>
       <c r="U41" s="11"/>
       <c r="V41" s="15"/>
       <c r="W41" s="14"/>
@@ -1757,13 +1775,27 @@
       <c r="M42" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
-      <c r="S42" s="15"/>
-      <c r="T42" s="15"/>
+      <c r="N42" s="15">
+        <v>1.9264E-4</v>
+      </c>
+      <c r="O42" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="P42" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="Q42" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="R42" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="S42" s="15">
+        <v>1.5152000000000001E-4</v>
+      </c>
+      <c r="T42" s="15">
+        <v>1.1710399999999999E-3</v>
+      </c>
       <c r="U42" s="11"/>
       <c r="V42" s="15"/>
       <c r="W42" s="14"/>
@@ -1775,13 +1807,27 @@
       <c r="M43" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
+      <c r="N43" s="15">
+        <v>2.051340288E-4</v>
+      </c>
+      <c r="O43" s="15">
+        <v>2.2524702719999999E-4</v>
+      </c>
+      <c r="P43" s="15">
+        <v>2.4536002560000001E-4</v>
+      </c>
+      <c r="Q43" s="15">
+        <v>2.6547302400000002E-4</v>
+      </c>
+      <c r="R43" s="15">
+        <v>2.8558602239999999E-4</v>
+      </c>
+      <c r="S43" s="15">
+        <v>2.5049902080000002E-4</v>
+      </c>
+      <c r="T43" s="15">
+        <v>1.4772991487999999E-3</v>
+      </c>
       <c r="U43" s="11"/>
       <c r="V43" s="15"/>
       <c r="W43" s="14"/>
@@ -1791,13 +1837,27 @@
       <c r="M44" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
+      <c r="N44" s="15">
+        <v>1.9264E-4</v>
+      </c>
+      <c r="O44" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="P44" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="Q44" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="R44" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="S44" s="15">
+        <v>1.5152000000000001E-4</v>
+      </c>
+      <c r="T44" s="15">
+        <v>1.1710399999999999E-3</v>
+      </c>
       <c r="U44" s="11"/>
       <c r="V44" s="15"/>
       <c r="W44" s="14"/>
@@ -1813,7 +1873,9 @@
       <c r="Q45" s="15"/>
       <c r="R45" s="15"/>
       <c r="S45" s="15"/>
-      <c r="T45" s="15"/>
+      <c r="T45" s="15">
+        <v>1.0427340288E-3</v>
+      </c>
       <c r="U45" s="11"/>
       <c r="V45" s="15"/>
       <c r="W45" s="14"/>
@@ -1829,7 +1891,9 @@
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
       <c r="S46" s="15"/>
-      <c r="T46" s="15"/>
+      <c r="T46" s="15">
+        <v>1.0427340288E-3</v>
+      </c>
       <c r="U46" s="11"/>
       <c r="V46" s="15"/>
       <c r="W46" s="14"/>
@@ -1845,7 +1909,9 @@
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
       <c r="S47" s="15"/>
-      <c r="T47" s="15"/>
+      <c r="T47" s="15">
+        <v>1.0427340288E-3</v>
+      </c>
       <c r="U47" s="11"/>
       <c r="V47" s="15"/>
       <c r="W47" s="14"/>
@@ -1997,13 +2063,19 @@
       <c r="M55" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
+      <c r="N55" s="15">
+        <v>2.1062446080000001E-4</v>
+      </c>
+      <c r="O55" s="15">
+        <v>3.2178662400000001E-4</v>
+      </c>
       <c r="P55" s="15"/>
       <c r="Q55" s="15"/>
       <c r="R55" s="15"/>
       <c r="S55" s="15"/>
-      <c r="T55" s="15"/>
+      <c r="T55" s="15">
+        <v>5.3241108480000003E-4</v>
+      </c>
       <c r="U55" s="11"/>
       <c r="V55" s="15"/>
       <c r="W55" s="14"/>
@@ -2013,13 +2085,19 @@
       <c r="M56" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N56" s="15"/>
-      <c r="O56" s="15"/>
+      <c r="N56" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="O56" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
       <c r="P56" s="15"/>
       <c r="Q56" s="15"/>
       <c r="R56" s="15"/>
       <c r="S56" s="15"/>
-      <c r="T56" s="15"/>
+      <c r="T56" s="15">
+        <v>3.5935999999999997E-4</v>
+      </c>
       <c r="U56" s="11"/>
       <c r="V56" s="15"/>
       <c r="W56" s="14"/>
@@ -2031,13 +2109,19 @@
       <c r="M57" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="N57" s="15"/>
-      <c r="O57" s="15"/>
+      <c r="N57" s="15">
+        <v>2.1062446080000001E-4</v>
+      </c>
+      <c r="O57" s="15">
+        <v>3.2178662400000001E-4</v>
+      </c>
       <c r="P57" s="15"/>
       <c r="Q57" s="15"/>
       <c r="R57" s="15"/>
       <c r="S57" s="15"/>
-      <c r="T57" s="15"/>
+      <c r="T57" s="15">
+        <v>5.3241108480000003E-4</v>
+      </c>
       <c r="U57" s="11"/>
       <c r="V57" s="15"/>
       <c r="W57" s="14"/>
@@ -2047,13 +2131,19 @@
       <c r="M58" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="N58" s="15"/>
-      <c r="O58" s="15"/>
+      <c r="N58" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="O58" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
       <c r="P58" s="15"/>
       <c r="Q58" s="15"/>
       <c r="R58" s="15"/>
       <c r="S58" s="15"/>
-      <c r="T58" s="15"/>
+      <c r="T58" s="15">
+        <v>3.5935999999999997E-4</v>
+      </c>
       <c r="U58" s="11"/>
       <c r="V58" s="15"/>
       <c r="W58" s="14"/>
@@ -2069,7 +2159,9 @@
       <c r="Q59" s="15"/>
       <c r="R59" s="15"/>
       <c r="S59" s="15"/>
-      <c r="T59" s="15"/>
+      <c r="T59" s="15">
+        <v>3.339844608E-4</v>
+      </c>
       <c r="U59" s="11"/>
       <c r="V59" s="15"/>
       <c r="W59" s="14"/>
@@ -2085,7 +2177,9 @@
       <c r="Q60" s="15"/>
       <c r="R60" s="15"/>
       <c r="S60" s="15"/>
-      <c r="T60" s="15"/>
+      <c r="T60" s="15">
+        <v>3.339844608E-4</v>
+      </c>
       <c r="U60" s="11"/>
       <c r="V60" s="15"/>
       <c r="W60" s="14"/>
@@ -2101,7 +2195,9 @@
       <c r="Q61" s="15"/>
       <c r="R61" s="15"/>
       <c r="S61" s="15"/>
-      <c r="T61" s="15"/>
+      <c r="T61" s="15">
+        <v>3.339844608E-4</v>
+      </c>
       <c r="U61" s="11"/>
       <c r="V61" s="15"/>
       <c r="W61" s="14"/>

</xml_diff>

<commit_message>
CBSLine evaluation with MFS of 264Byte
</commit_message>
<xml_diff>
--- a/src/main/java/org/networkcalculus/dnc/demos/Eval_CBSLine/Eval_CBSLine_Results.xlsx
+++ b/src/main/java/org/networkcalculus/dnc/demos/Eval_CBSLine/Eval_CBSLine_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ForceXX\Documents\Studium\FAU_Informatik_Master\FS5\Masterarbeit\Network_Calculus_in_TSN\DNC\IntelliJ\src\main\java\org\networkcalculus\dnc\demos\Eval_CBSLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D32D6A-D893-4F9E-AFEA-73E15F1A9249}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE60F089-2B81-4F17-81A9-4069557A829F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2280" windowWidth="46080" windowHeight="22152" activeTab="1" xr2:uid="{76093B85-C4EA-4FAC-BB07-8F5ADEBC9C5C}"/>
+    <workbookView xWindow="0" yWindow="2736" windowWidth="46080" windowHeight="22152" activeTab="1" xr2:uid="{76093B85-C4EA-4FAC-BB07-8F5ADEBC9C5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="35">
   <si>
     <t>f1</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>22,528MBIt/s</t>
+  </si>
+  <si>
+    <t>33,792MBIt/s</t>
   </si>
 </sst>
 </file>
@@ -307,7 +310,49 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="42">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
     </dxf>
@@ -465,13 +510,13 @@
   <autoFilter ref="M9:T16" xr:uid="{AFD0FDAD-B567-49C8-A37C-DCEECED05009}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{BE6FA1AF-957C-4302-ABCA-3CED577909FB}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{EABB3472-FB4D-420C-9C6B-D5FBAEE8D4FF}" name="S1" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{362B0664-EECB-41EA-8E6D-BC83B9D56EFC}" name="S2" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{6AAC6F6B-16ED-403D-9C2D-403BD383643D}" name="S3" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{AD2D3DC2-A063-43E3-8F4D-72B5648D83E8}" name="S4" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{1ACA20C8-E74E-4AE0-9617-8D84870DB044}" name="S5" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{5FFF2E6B-00A8-47E0-8FF6-2C25AA61CD2E}" name="S6" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{59937D66-C814-42EC-A281-7F9615B9AC54}" name="Total" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{EABB3472-FB4D-420C-9C6B-D5FBAEE8D4FF}" name="S1" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{362B0664-EECB-41EA-8E6D-BC83B9D56EFC}" name="S2" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{6AAC6F6B-16ED-403D-9C2D-403BD383643D}" name="S3" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{AD2D3DC2-A063-43E3-8F4D-72B5648D83E8}" name="S4" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{1ACA20C8-E74E-4AE0-9617-8D84870DB044}" name="S5" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{5FFF2E6B-00A8-47E0-8FF6-2C25AA61CD2E}" name="S6" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{59937D66-C814-42EC-A281-7F9615B9AC54}" name="Total" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -482,13 +527,13 @@
   <autoFilter ref="M23:T30" xr:uid="{9F3FFC4E-8857-417C-879B-7E46756E6ACB}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{6C7A2137-FE16-4D18-B3E5-47340E52F2D5}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{EDDA7831-D99A-413F-AA04-C00A206D6D34}" name="S1" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{3CB5E796-20A3-4C92-9FC5-590D66DC5593}" name="S2" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{3D106F77-8448-4063-87F7-7B7BE008B2F2}" name="S3" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{A891D787-2819-425A-9CE0-E8145AC0C05B}" name="S4" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{C6263B6C-6BFC-46DD-94D3-5EDB5A4EAF2F}" name="S5" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{AAC57713-C8ED-436C-B744-473CD5CFAB13}" name="S6" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{31F74DD7-5067-4854-B832-9EFA7B4543EA}" name="Total" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{EDDA7831-D99A-413F-AA04-C00A206D6D34}" name="S1" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{3CB5E796-20A3-4C92-9FC5-590D66DC5593}" name="S2" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{3D106F77-8448-4063-87F7-7B7BE008B2F2}" name="S3" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{A891D787-2819-425A-9CE0-E8145AC0C05B}" name="S4" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{C6263B6C-6BFC-46DD-94D3-5EDB5A4EAF2F}" name="S5" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{AAC57713-C8ED-436C-B744-473CD5CFAB13}" name="S6" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{31F74DD7-5067-4854-B832-9EFA7B4543EA}" name="Total" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -499,13 +544,13 @@
   <autoFilter ref="M40:T47" xr:uid="{E16230B5-F45F-4647-925B-5EE18F895F9C}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9D1375EE-0D83-4727-B0F9-FE752E8A0CBC}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{C37D03EB-F7B2-4349-B2CC-726DB4010C90}" name="S1" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{7037993D-3D73-4283-A3B4-93C5B4E6E202}" name="S2" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{7ADA14D4-6575-4C8D-A7EA-C47F389375CE}" name="S3" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{5429F400-2F0F-4356-AC4A-9C65390A88EF}" name="S4" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{65870CF8-359E-4FAC-947D-39633692A667}" name="S5" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{59753DB4-DBE6-466A-BCC2-D1C2D56D1A27}" name="S6" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{51BDBB4F-8359-4885-B4D7-DF406809ECB7}" name="Total" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{C37D03EB-F7B2-4349-B2CC-726DB4010C90}" name="S1" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{7037993D-3D73-4283-A3B4-93C5B4E6E202}" name="S2" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{7ADA14D4-6575-4C8D-A7EA-C47F389375CE}" name="S3" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{5429F400-2F0F-4356-AC4A-9C65390A88EF}" name="S4" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{65870CF8-359E-4FAC-947D-39633692A667}" name="S5" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{59753DB4-DBE6-466A-BCC2-D1C2D56D1A27}" name="S6" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{51BDBB4F-8359-4885-B4D7-DF406809ECB7}" name="Total" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -516,13 +561,47 @@
   <autoFilter ref="M54:T61" xr:uid="{B5EBC119-6892-4EFB-AB7E-F78E33D432A9}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0BB4E427-3492-4DCF-9D08-38551180E6EE}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{625D768D-2EA2-4E64-B741-35AF2819C1F7}" name="S1" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{2FA180EB-2936-481F-B1D1-4C1DA624FA57}" name="S2" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{7EDAFDAC-585A-4749-ABD8-DEBBA52F7B86}" name="S3" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{3E05A679-5166-455F-9DE8-C76697485C01}" name="S4" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{9611ADE2-11EE-403F-8E25-5BF3FD83A7EE}" name="S5" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{4B5CC043-D947-410A-8D8E-B4B1EDA50E93}" name="S6" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{90BF4DC0-8F16-4F8E-AD7A-04145C27A52D}" name="Total" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{625D768D-2EA2-4E64-B741-35AF2819C1F7}" name="S1" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{2FA180EB-2936-481F-B1D1-4C1DA624FA57}" name="S2" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{7EDAFDAC-585A-4749-ABD8-DEBBA52F7B86}" name="S3" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{3E05A679-5166-455F-9DE8-C76697485C01}" name="S4" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{9611ADE2-11EE-403F-8E25-5BF3FD83A7EE}" name="S5" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{4B5CC043-D947-410A-8D8E-B4B1EDA50E93}" name="S6" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{90BF4DC0-8F16-4F8E-AD7A-04145C27A52D}" name="Total" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CA385C79-BAF1-4263-8928-2A2D2D1190C4}" name="Tabelle146" displayName="Tabelle146" ref="M71:T78" totalsRowShown="0">
+  <autoFilter ref="M71:T78" xr:uid="{51782671-9EEB-46B0-812D-DE4D14A213EE}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{AD5E4FB3-F32D-4B93-86CA-C7ECF985973B}" name="Analysis"/>
+    <tableColumn id="2" xr3:uid="{32771DFC-FFFB-479C-8088-AA245ED9B201}" name="S1" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{850259B7-F6FC-40B4-94B0-436FE4A42169}" name="S2" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{D83AC1AB-1A0A-4527-925F-218D72D2227A}" name="S3" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{9AE7B8F5-E983-41B9-B1F4-4FC70710981E}" name="S4" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{BF918F35-6CDD-4DEE-956C-2A3434C345D0}" name="S5" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{8BF14E06-E1BE-45C5-B2AF-D712C65491A2}" name="S6" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{386EE86E-EBB8-4A4D-B17D-421040C58630}" name="Total" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{60894574-2FEA-4B96-9E6D-6C74E2DA7F23}" name="Tabelle1357" displayName="Tabelle1357" ref="M85:T92" totalsRowShown="0">
+  <autoFilter ref="M85:T92" xr:uid="{B8C55D2C-921B-49DD-AC76-772D4A43E64D}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{1B1BABD6-FD5C-41BB-948A-6FC0BCC11D24}" name="Analysis"/>
+    <tableColumn id="2" xr3:uid="{DB6F9D20-C97E-480C-99B2-E87E4A9E1E0E}" name="S1" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{6D579111-6BD1-4C25-A59D-5752C6D1027B}" name="S2" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{971D35F8-9047-4D4E-B3A8-1050E4CBB9F7}" name="S3" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{12EA7A8D-ED74-4686-A548-2A70B019DDD4}" name="S4" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{1FE3C278-2C61-4E80-AD86-3FA5279E30B5}" name="S5" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{EE077AF3-1AB4-421C-B5DC-9511794D8F8E}" name="S6" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{4D81D46E-0FA9-4BFC-8316-8FE6191F7B12}" name="Total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -828,7 +907,7 @@
   <dimension ref="B3:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -861,7 +940,7 @@
       </c>
       <c r="L3" s="4">
         <f>B4*C4*8</f>
-        <v>2816</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
@@ -869,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>176</v>
+        <v>264</v>
       </c>
       <c r="D4" s="1">
         <v>1.25E-4</v>
@@ -885,7 +964,7 @@
       </c>
       <c r="L4" s="5">
         <f>L3/D4</f>
-        <v>22528000</v>
+        <v>33792000</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
@@ -894,7 +973,7 @@
       </c>
       <c r="L5" s="4">
         <f>L3*(1-(L4/E4))</f>
-        <v>2181.6115199999999</v>
+        <v>2796.62592</v>
       </c>
     </row>
   </sheetData>
@@ -908,10 +987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB25049-F719-48DC-B24C-CE81CB877780}">
-  <dimension ref="B3:W62"/>
+  <dimension ref="B3:W93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X34" sqref="X34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="T77" sqref="T77:T78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2216,14 +2295,622 @@
       <c r="V62" s="19"/>
       <c r="W62" s="21"/>
     </row>
+    <row r="65" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L65" s="6"/>
+      <c r="M65" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N65" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O65" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="P65" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q65" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R65" s="7"/>
+      <c r="S65" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="T65" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="U65" s="7"/>
+      <c r="V65" s="7"/>
+      <c r="W65" s="9"/>
+    </row>
+    <row r="66" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L66" s="10"/>
+      <c r="M66" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N66" s="12">
+        <v>2</v>
+      </c>
+      <c r="O66" s="12">
+        <v>88</v>
+      </c>
+      <c r="P66" s="12">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="Q66" s="13">
+        <v>100000000</v>
+      </c>
+      <c r="R66" s="11"/>
+      <c r="S66" s="1">
+        <v>1328.70144</v>
+      </c>
+      <c r="T66" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="U66" s="11"/>
+      <c r="V66" s="11"/>
+      <c r="W66" s="14"/>
+    </row>
+    <row r="67" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L67" s="10"/>
+      <c r="M67" s="11"/>
+      <c r="N67" s="11"/>
+      <c r="O67" s="11"/>
+      <c r="P67" s="11"/>
+      <c r="Q67" s="11"/>
+      <c r="R67" s="11"/>
+      <c r="S67" s="11"/>
+      <c r="T67" s="11"/>
+      <c r="U67" s="11"/>
+      <c r="V67" s="11"/>
+      <c r="W67" s="14"/>
+    </row>
+    <row r="68" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L68" s="10"/>
+      <c r="M68" s="11"/>
+      <c r="N68" s="11"/>
+      <c r="O68" s="11"/>
+      <c r="P68" s="11"/>
+      <c r="Q68" s="11"/>
+      <c r="R68" s="11"/>
+      <c r="S68" s="11"/>
+      <c r="T68" s="11"/>
+      <c r="U68" s="11"/>
+      <c r="V68" s="11"/>
+      <c r="W68" s="14"/>
+    </row>
+    <row r="69" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L69" s="10"/>
+      <c r="M69" s="11"/>
+      <c r="N69" s="11"/>
+      <c r="O69" s="11"/>
+      <c r="P69" s="11"/>
+      <c r="Q69" s="11"/>
+      <c r="R69" s="11"/>
+      <c r="S69" s="11"/>
+      <c r="T69" s="11"/>
+      <c r="U69" s="11"/>
+      <c r="V69" s="11"/>
+      <c r="W69" s="14"/>
+    </row>
+    <row r="70" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L70" s="10"/>
+      <c r="M70" s="11"/>
+      <c r="N70" s="11"/>
+      <c r="O70" s="11"/>
+      <c r="P70" s="11"/>
+      <c r="Q70" s="11"/>
+      <c r="R70" s="11"/>
+      <c r="S70" s="11"/>
+      <c r="T70" s="11"/>
+      <c r="U70" s="11"/>
+      <c r="V70" s="11"/>
+      <c r="W70" s="14"/>
+    </row>
+    <row r="71" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L71" s="10"/>
+      <c r="M71" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N71" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O71" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P71" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q71" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R71" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="S71" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="T71" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="U71" s="11"/>
+      <c r="V71" s="11"/>
+      <c r="W71" s="14"/>
+    </row>
+    <row r="72" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L72" s="10"/>
+      <c r="M72" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N72" s="15">
+        <v>2.1217402879999999E-4</v>
+      </c>
+      <c r="O72" s="15">
+        <v>2.330800128E-4</v>
+      </c>
+      <c r="P72" s="15">
+        <v>2.5398599679999999E-4</v>
+      </c>
+      <c r="Q72" s="15">
+        <v>2.7489198080000001E-4</v>
+      </c>
+      <c r="R72" s="15">
+        <v>2.9579796480000002E-4</v>
+      </c>
+      <c r="S72" s="15">
+        <v>2.5446394880000001E-4</v>
+      </c>
+      <c r="T72" s="15">
+        <v>1.5243939328E-3</v>
+      </c>
+      <c r="U72" s="11"/>
+      <c r="V72" s="15"/>
+      <c r="W72" s="14"/>
+    </row>
+    <row r="73" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L73" s="10"/>
+      <c r="M73" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N73" s="15">
+        <v>1.9968000000000001E-4</v>
+      </c>
+      <c r="O73" s="15">
+        <v>2.20585984E-4</v>
+      </c>
+      <c r="P73" s="15">
+        <v>2.2783999999999999E-4</v>
+      </c>
+      <c r="Q73" s="15">
+        <v>2.2783999999999999E-4</v>
+      </c>
+      <c r="R73" s="15">
+        <v>2.2783999999999999E-4</v>
+      </c>
+      <c r="S73" s="15">
+        <v>1.6559999999999999E-4</v>
+      </c>
+      <c r="T73" s="15">
+        <v>1.269385984E-3</v>
+      </c>
+      <c r="U73" s="11"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="14"/>
+    </row>
+    <row r="74" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L74" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M74" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N74" s="15">
+        <v>2.1217402879999999E-4</v>
+      </c>
+      <c r="O74" s="15">
+        <v>2.330800128E-4</v>
+      </c>
+      <c r="P74" s="15">
+        <v>2.5398599679999999E-4</v>
+      </c>
+      <c r="Q74" s="15">
+        <v>2.7489198080000001E-4</v>
+      </c>
+      <c r="R74" s="15">
+        <v>2.9579796480000002E-4</v>
+      </c>
+      <c r="S74" s="15">
+        <v>2.5446394880000001E-4</v>
+      </c>
+      <c r="T74" s="15">
+        <v>1.5243939328E-3</v>
+      </c>
+      <c r="U74" s="11"/>
+      <c r="V74" s="15"/>
+      <c r="W74" s="14"/>
+    </row>
+    <row r="75" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L75" s="10"/>
+      <c r="M75" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N75" s="15"/>
+      <c r="O75" s="15"/>
+      <c r="P75" s="15"/>
+      <c r="Q75" s="15"/>
+      <c r="R75" s="15"/>
+      <c r="S75" s="15"/>
+      <c r="T75" s="15">
+        <v>1.269385984E-3</v>
+      </c>
+      <c r="U75" s="11"/>
+      <c r="V75" s="15"/>
+      <c r="W75" s="14"/>
+    </row>
+    <row r="76" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L76" s="10"/>
+      <c r="M76" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N76" s="15"/>
+      <c r="O76" s="15"/>
+      <c r="P76" s="15"/>
+      <c r="Q76" s="15"/>
+      <c r="R76" s="15"/>
+      <c r="S76" s="15"/>
+      <c r="T76" s="15">
+        <v>1.0779340287999999E-3</v>
+      </c>
+      <c r="U76" s="11"/>
+      <c r="V76" s="15"/>
+      <c r="W76" s="14"/>
+    </row>
+    <row r="77" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L77" s="10"/>
+      <c r="M77" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N77" s="15"/>
+      <c r="O77" s="15"/>
+      <c r="P77" s="15"/>
+      <c r="Q77" s="15"/>
+      <c r="R77" s="15"/>
+      <c r="S77" s="15"/>
+      <c r="T77" s="15">
+        <v>1.0779340287999999E-3</v>
+      </c>
+      <c r="U77" s="11"/>
+      <c r="V77" s="15"/>
+      <c r="W77" s="14"/>
+    </row>
+    <row r="78" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L78" s="10"/>
+      <c r="M78" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N78" s="15"/>
+      <c r="O78" s="15"/>
+      <c r="P78" s="15"/>
+      <c r="Q78" s="15"/>
+      <c r="R78" s="15"/>
+      <c r="S78" s="15"/>
+      <c r="T78" s="15">
+        <v>1.0779340287999999E-3</v>
+      </c>
+      <c r="U78" s="11"/>
+      <c r="V78" s="15"/>
+      <c r="W78" s="14"/>
+    </row>
+    <row r="79" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L79" s="10"/>
+      <c r="M79" s="11"/>
+      <c r="N79" s="11"/>
+      <c r="O79" s="11"/>
+      <c r="P79" s="11"/>
+      <c r="Q79" s="11"/>
+      <c r="R79" s="11"/>
+      <c r="S79" s="11"/>
+      <c r="T79" s="11"/>
+      <c r="U79" s="11"/>
+      <c r="V79" s="11"/>
+      <c r="W79" s="14"/>
+    </row>
+    <row r="80" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L80" s="10"/>
+      <c r="M80" s="11"/>
+      <c r="N80" s="11"/>
+      <c r="O80" s="11"/>
+      <c r="P80" s="11"/>
+      <c r="Q80" s="11"/>
+      <c r="R80" s="11"/>
+      <c r="S80" s="11"/>
+      <c r="T80" s="11"/>
+      <c r="U80" s="11"/>
+      <c r="V80" s="11"/>
+      <c r="W80" s="14"/>
+    </row>
+    <row r="81" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L81" s="10"/>
+      <c r="M81" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N81" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="O81" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P81" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q81" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="R81" s="11"/>
+      <c r="S81" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="T81" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="U81" s="11"/>
+      <c r="V81" s="11"/>
+      <c r="W81" s="14"/>
+    </row>
+    <row r="82" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L82" s="10"/>
+      <c r="M82" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N82" s="12">
+        <v>2</v>
+      </c>
+      <c r="O82" s="12">
+        <v>264</v>
+      </c>
+      <c r="P82" s="12">
+        <v>1.25E-4</v>
+      </c>
+      <c r="Q82" s="13">
+        <v>100000000</v>
+      </c>
+      <c r="R82" s="11"/>
+      <c r="S82" s="22">
+        <v>2796.62592</v>
+      </c>
+      <c r="T82" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="U82" s="11"/>
+      <c r="V82" s="11"/>
+      <c r="W82" s="14"/>
+    </row>
+    <row r="83" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L83" s="10"/>
+      <c r="M83" s="11"/>
+      <c r="N83" s="11"/>
+      <c r="O83" s="11"/>
+      <c r="P83" s="11"/>
+      <c r="Q83" s="11"/>
+      <c r="R83" s="11"/>
+      <c r="S83" s="11"/>
+      <c r="T83" s="11"/>
+      <c r="U83" s="11"/>
+      <c r="V83" s="11"/>
+      <c r="W83" s="14"/>
+    </row>
+    <row r="84" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L84" s="10"/>
+      <c r="M84" s="11"/>
+      <c r="N84" s="11"/>
+      <c r="O84" s="11"/>
+      <c r="P84" s="11"/>
+      <c r="Q84" s="11"/>
+      <c r="R84" s="11"/>
+      <c r="S84" s="11"/>
+      <c r="T84" s="11"/>
+      <c r="U84" s="11"/>
+      <c r="V84" s="11"/>
+      <c r="W84" s="14"/>
+    </row>
+    <row r="85" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L85" s="10"/>
+      <c r="M85" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N85" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O85" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P85" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q85" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R85" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="S85" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="T85" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="U85" s="11"/>
+      <c r="V85" s="11"/>
+      <c r="W85" s="14"/>
+    </row>
+    <row r="86" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L86" s="10"/>
+      <c r="M86" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N86" s="15">
+        <v>2.3522503679999999E-4</v>
+      </c>
+      <c r="O86" s="15">
+        <v>4.0196828159999999E-4</v>
+      </c>
+      <c r="P86" s="15"/>
+      <c r="Q86" s="15"/>
+      <c r="R86" s="15"/>
+      <c r="S86" s="15"/>
+      <c r="T86" s="15">
+        <v>6.3719331840000003E-4</v>
+      </c>
+      <c r="U86" s="11"/>
+      <c r="V86" s="15"/>
+      <c r="W86" s="14"/>
+    </row>
+    <row r="87" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L87" s="10"/>
+      <c r="M87" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N87" s="15">
+        <v>2.0783999999999999E-4</v>
+      </c>
+      <c r="O87" s="15">
+        <v>2.0783999999999999E-4</v>
+      </c>
+      <c r="P87" s="15"/>
+      <c r="Q87" s="15"/>
+      <c r="R87" s="15"/>
+      <c r="S87" s="15"/>
+      <c r="T87" s="15">
+        <v>4.1567999999999998E-4</v>
+      </c>
+      <c r="U87" s="11"/>
+      <c r="V87" s="15"/>
+      <c r="W87" s="14"/>
+    </row>
+    <row r="88" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L88" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="M88" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N88" s="15">
+        <v>2.3522503679999999E-4</v>
+      </c>
+      <c r="O88" s="15">
+        <v>3.9455999999999899E-4</v>
+      </c>
+      <c r="P88" s="15"/>
+      <c r="Q88" s="15"/>
+      <c r="R88" s="15"/>
+      <c r="S88" s="15"/>
+      <c r="T88" s="15">
+        <v>6.2978503680000001E-4</v>
+      </c>
+      <c r="U88" s="11"/>
+      <c r="V88" s="15"/>
+      <c r="W88" s="14"/>
+    </row>
+    <row r="89" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L89" s="10"/>
+      <c r="M89" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N89" s="15">
+        <v>2.0783999999999999E-4</v>
+      </c>
+      <c r="O89" s="15">
+        <v>2.0783999999999999E-4</v>
+      </c>
+      <c r="P89" s="15"/>
+      <c r="Q89" s="15"/>
+      <c r="R89" s="15"/>
+      <c r="S89" s="15"/>
+      <c r="T89" s="15">
+        <v>4.1567999999999998E-4</v>
+      </c>
+      <c r="U89" s="11"/>
+      <c r="V89" s="15"/>
+      <c r="W89" s="14"/>
+    </row>
+    <row r="90" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L90" s="10"/>
+      <c r="M90" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N90" s="15"/>
+      <c r="O90" s="15"/>
+      <c r="P90" s="15"/>
+      <c r="Q90" s="15"/>
+      <c r="R90" s="15"/>
+      <c r="S90" s="15"/>
+      <c r="T90" s="15">
+        <v>3.5858503679999997E-4</v>
+      </c>
+      <c r="U90" s="11"/>
+      <c r="V90" s="15"/>
+      <c r="W90" s="14"/>
+    </row>
+    <row r="91" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L91" s="10"/>
+      <c r="M91" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N91" s="15"/>
+      <c r="O91" s="15"/>
+      <c r="P91" s="15"/>
+      <c r="Q91" s="15"/>
+      <c r="R91" s="15"/>
+      <c r="S91" s="15"/>
+      <c r="T91" s="15">
+        <v>3.5858503679999997E-4</v>
+      </c>
+      <c r="U91" s="11"/>
+      <c r="V91" s="15"/>
+      <c r="W91" s="14"/>
+    </row>
+    <row r="92" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L92" s="10"/>
+      <c r="M92" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N92" s="15"/>
+      <c r="O92" s="15"/>
+      <c r="P92" s="15"/>
+      <c r="Q92" s="15"/>
+      <c r="R92" s="15"/>
+      <c r="S92" s="15"/>
+      <c r="T92" s="15">
+        <v>3.5858503679999997E-4</v>
+      </c>
+      <c r="U92" s="11"/>
+      <c r="V92" s="15"/>
+      <c r="W92" s="14"/>
+    </row>
+    <row r="93" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L93" s="18"/>
+      <c r="M93" s="19"/>
+      <c r="N93" s="19"/>
+      <c r="O93" s="19"/>
+      <c r="P93" s="19"/>
+      <c r="Q93" s="19"/>
+      <c r="R93" s="19"/>
+      <c r="S93" s="19"/>
+      <c r="T93" s="19"/>
+      <c r="U93" s="19"/>
+      <c r="V93" s="19"/>
+      <c r="W93" s="21"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CBSLine evaluation with MFS of 512Byte
</commit_message>
<xml_diff>
--- a/src/main/java/org/networkcalculus/dnc/demos/Eval_CBSLine/Eval_CBSLine_Results.xlsx
+++ b/src/main/java/org/networkcalculus/dnc/demos/Eval_CBSLine/Eval_CBSLine_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ForceXX\Documents\Studium\FAU_Informatik_Master\FS5\Masterarbeit\Network_Calculus_in_TSN\DNC\IntelliJ\src\main\java\org\networkcalculus\dnc\demos\Eval_CBSLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE60F089-2B81-4F17-81A9-4069557A829F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE109720-B8B8-4500-8C31-B8D54B3A16A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2736" windowWidth="46080" windowHeight="22152" activeTab="1" xr2:uid="{76093B85-C4EA-4FAC-BB07-8F5ADEBC9C5C}"/>
+    <workbookView xWindow="0" yWindow="3192" windowWidth="46080" windowHeight="22152" activeTab="1" xr2:uid="{76093B85-C4EA-4FAC-BB07-8F5ADEBC9C5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="36">
   <si>
     <t>f1</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>33,792MBIt/s</t>
+  </si>
+  <si>
+    <t>65,536MBit/s</t>
   </si>
 </sst>
 </file>
@@ -310,7 +313,49 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="56">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
     </dxf>
@@ -510,13 +555,13 @@
   <autoFilter ref="M9:T16" xr:uid="{AFD0FDAD-B567-49C8-A37C-DCEECED05009}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{BE6FA1AF-957C-4302-ABCA-3CED577909FB}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{EABB3472-FB4D-420C-9C6B-D5FBAEE8D4FF}" name="S1" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{362B0664-EECB-41EA-8E6D-BC83B9D56EFC}" name="S2" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{6AAC6F6B-16ED-403D-9C2D-403BD383643D}" name="S3" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{AD2D3DC2-A063-43E3-8F4D-72B5648D83E8}" name="S4" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{1ACA20C8-E74E-4AE0-9617-8D84870DB044}" name="S5" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{5FFF2E6B-00A8-47E0-8FF6-2C25AA61CD2E}" name="S6" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{59937D66-C814-42EC-A281-7F9615B9AC54}" name="Total" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{EABB3472-FB4D-420C-9C6B-D5FBAEE8D4FF}" name="S1" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{362B0664-EECB-41EA-8E6D-BC83B9D56EFC}" name="S2" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{6AAC6F6B-16ED-403D-9C2D-403BD383643D}" name="S3" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{AD2D3DC2-A063-43E3-8F4D-72B5648D83E8}" name="S4" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{1ACA20C8-E74E-4AE0-9617-8D84870DB044}" name="S5" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{5FFF2E6B-00A8-47E0-8FF6-2C25AA61CD2E}" name="S6" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{59937D66-C814-42EC-A281-7F9615B9AC54}" name="Total" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -527,13 +572,13 @@
   <autoFilter ref="M23:T30" xr:uid="{9F3FFC4E-8857-417C-879B-7E46756E6ACB}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{6C7A2137-FE16-4D18-B3E5-47340E52F2D5}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{EDDA7831-D99A-413F-AA04-C00A206D6D34}" name="S1" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{3CB5E796-20A3-4C92-9FC5-590D66DC5593}" name="S2" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{3D106F77-8448-4063-87F7-7B7BE008B2F2}" name="S3" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{A891D787-2819-425A-9CE0-E8145AC0C05B}" name="S4" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{C6263B6C-6BFC-46DD-94D3-5EDB5A4EAF2F}" name="S5" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{AAC57713-C8ED-436C-B744-473CD5CFAB13}" name="S6" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{31F74DD7-5067-4854-B832-9EFA7B4543EA}" name="Total" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{EDDA7831-D99A-413F-AA04-C00A206D6D34}" name="S1" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{3CB5E796-20A3-4C92-9FC5-590D66DC5593}" name="S2" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{3D106F77-8448-4063-87F7-7B7BE008B2F2}" name="S3" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{A891D787-2819-425A-9CE0-E8145AC0C05B}" name="S4" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{C6263B6C-6BFC-46DD-94D3-5EDB5A4EAF2F}" name="S5" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{AAC57713-C8ED-436C-B744-473CD5CFAB13}" name="S6" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{31F74DD7-5067-4854-B832-9EFA7B4543EA}" name="Total" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -544,13 +589,13 @@
   <autoFilter ref="M40:T47" xr:uid="{E16230B5-F45F-4647-925B-5EE18F895F9C}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9D1375EE-0D83-4727-B0F9-FE752E8A0CBC}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{C37D03EB-F7B2-4349-B2CC-726DB4010C90}" name="S1" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{7037993D-3D73-4283-A3B4-93C5B4E6E202}" name="S2" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{7ADA14D4-6575-4C8D-A7EA-C47F389375CE}" name="S3" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{5429F400-2F0F-4356-AC4A-9C65390A88EF}" name="S4" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{65870CF8-359E-4FAC-947D-39633692A667}" name="S5" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{59753DB4-DBE6-466A-BCC2-D1C2D56D1A27}" name="S6" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{51BDBB4F-8359-4885-B4D7-DF406809ECB7}" name="Total" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{C37D03EB-F7B2-4349-B2CC-726DB4010C90}" name="S1" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{7037993D-3D73-4283-A3B4-93C5B4E6E202}" name="S2" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{7ADA14D4-6575-4C8D-A7EA-C47F389375CE}" name="S3" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{5429F400-2F0F-4356-AC4A-9C65390A88EF}" name="S4" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{65870CF8-359E-4FAC-947D-39633692A667}" name="S5" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{59753DB4-DBE6-466A-BCC2-D1C2D56D1A27}" name="S6" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{51BDBB4F-8359-4885-B4D7-DF406809ECB7}" name="Total" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -561,13 +606,13 @@
   <autoFilter ref="M54:T61" xr:uid="{B5EBC119-6892-4EFB-AB7E-F78E33D432A9}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0BB4E427-3492-4DCF-9D08-38551180E6EE}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{625D768D-2EA2-4E64-B741-35AF2819C1F7}" name="S1" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{2FA180EB-2936-481F-B1D1-4C1DA624FA57}" name="S2" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{7EDAFDAC-585A-4749-ABD8-DEBBA52F7B86}" name="S3" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{3E05A679-5166-455F-9DE8-C76697485C01}" name="S4" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{9611ADE2-11EE-403F-8E25-5BF3FD83A7EE}" name="S5" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{4B5CC043-D947-410A-8D8E-B4B1EDA50E93}" name="S6" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{90BF4DC0-8F16-4F8E-AD7A-04145C27A52D}" name="Total" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{625D768D-2EA2-4E64-B741-35AF2819C1F7}" name="S1" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{2FA180EB-2936-481F-B1D1-4C1DA624FA57}" name="S2" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{7EDAFDAC-585A-4749-ABD8-DEBBA52F7B86}" name="S3" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{3E05A679-5166-455F-9DE8-C76697485C01}" name="S4" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{9611ADE2-11EE-403F-8E25-5BF3FD83A7EE}" name="S5" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{4B5CC043-D947-410A-8D8E-B4B1EDA50E93}" name="S6" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{90BF4DC0-8F16-4F8E-AD7A-04145C27A52D}" name="Total" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -578,13 +623,13 @@
   <autoFilter ref="M71:T78" xr:uid="{51782671-9EEB-46B0-812D-DE4D14A213EE}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{AD5E4FB3-F32D-4B93-86CA-C7ECF985973B}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{32771DFC-FFFB-479C-8088-AA245ED9B201}" name="S1" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{850259B7-F6FC-40B4-94B0-436FE4A42169}" name="S2" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{D83AC1AB-1A0A-4527-925F-218D72D2227A}" name="S3" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{9AE7B8F5-E983-41B9-B1F4-4FC70710981E}" name="S4" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{BF918F35-6CDD-4DEE-956C-2A3434C345D0}" name="S5" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{8BF14E06-E1BE-45C5-B2AF-D712C65491A2}" name="S6" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{386EE86E-EBB8-4A4D-B17D-421040C58630}" name="Total" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{32771DFC-FFFB-479C-8088-AA245ED9B201}" name="S1" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{850259B7-F6FC-40B4-94B0-436FE4A42169}" name="S2" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{D83AC1AB-1A0A-4527-925F-218D72D2227A}" name="S3" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{9AE7B8F5-E983-41B9-B1F4-4FC70710981E}" name="S4" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{BF918F35-6CDD-4DEE-956C-2A3434C345D0}" name="S5" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{8BF14E06-E1BE-45C5-B2AF-D712C65491A2}" name="S6" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{386EE86E-EBB8-4A4D-B17D-421040C58630}" name="Total" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -595,13 +640,47 @@
   <autoFilter ref="M85:T92" xr:uid="{B8C55D2C-921B-49DD-AC76-772D4A43E64D}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{1B1BABD6-FD5C-41BB-948A-6FC0BCC11D24}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{DB6F9D20-C97E-480C-99B2-E87E4A9E1E0E}" name="S1" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{6D579111-6BD1-4C25-A59D-5752C6D1027B}" name="S2" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{971D35F8-9047-4D4E-B3A8-1050E4CBB9F7}" name="S3" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{12EA7A8D-ED74-4686-A548-2A70B019DDD4}" name="S4" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{1FE3C278-2C61-4E80-AD86-3FA5279E30B5}" name="S5" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{EE077AF3-1AB4-421C-B5DC-9511794D8F8E}" name="S6" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{4D81D46E-0FA9-4BFC-8316-8FE6191F7B12}" name="Total" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{DB6F9D20-C97E-480C-99B2-E87E4A9E1E0E}" name="S1" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{6D579111-6BD1-4C25-A59D-5752C6D1027B}" name="S2" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{971D35F8-9047-4D4E-B3A8-1050E4CBB9F7}" name="S3" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{12EA7A8D-ED74-4686-A548-2A70B019DDD4}" name="S4" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{1FE3C278-2C61-4E80-AD86-3FA5279E30B5}" name="S5" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{EE077AF3-1AB4-421C-B5DC-9511794D8F8E}" name="S6" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{4D81D46E-0FA9-4BFC-8316-8FE6191F7B12}" name="Total" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D0CE2A10-3FBF-4612-B421-725452D05BEB}" name="Tabelle1468" displayName="Tabelle1468" ref="M102:T109" totalsRowShown="0">
+  <autoFilter ref="M102:T109" xr:uid="{3B58D87F-510B-43F0-BC7D-8EF14E94029E}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{E6C46FA4-813C-4003-A6A1-34967D676206}" name="Analysis"/>
+    <tableColumn id="2" xr3:uid="{C1B5C27C-40D8-4CE6-8300-D32B61DBD03E}" name="S1" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{822EBEC2-E9F3-433C-9D06-01D83E51B4EC}" name="S2" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{7E24F410-F931-4EB2-B8F2-71F614752416}" name="S3" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{6F4DDE75-12D5-4E09-BD4C-B84DBE3A1613}" name="S4" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{D1A7BB02-6526-44E4-BAC4-F951ACEB49E0}" name="S5" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{CA43AF65-8F45-41AF-809C-76D07CBDCA7B}" name="S6" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{AA305A43-F356-44F9-B1BE-8A8539A588B2}" name="Total" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9E3095CD-2D75-4900-AE69-F559B8E8D3BD}" name="Tabelle13579" displayName="Tabelle13579" ref="M116:T123" totalsRowShown="0">
+  <autoFilter ref="M116:T123" xr:uid="{BBD41544-5CF6-451E-B19F-AA4B349E0FF5}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{F68E10CC-FD59-48C5-91A8-4F747980D2B8}" name="Analysis"/>
+    <tableColumn id="2" xr3:uid="{091DCD40-AFF4-4A35-A51B-5CE995B27C5B}" name="S1" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{32F634D5-1211-4A7C-8411-0DC8BF7C0116}" name="S2" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{BE2DA717-3CEA-4B45-9D01-B2AF2CFBA155}" name="S3" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{820A1FC2-AB1F-424D-8760-928CAC5CEC89}" name="S4" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{7CDBF264-CA71-4555-AD13-B4F0B0EFF5CB}" name="S5" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{FD7873DE-5A47-42D5-BE83-3AC049767285}" name="S6" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{514BF621-1FB2-46A5-A883-5F156AE64F89}" name="Total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -907,7 +986,7 @@
   <dimension ref="B3:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,7 +1019,7 @@
       </c>
       <c r="L3" s="4">
         <f>B4*C4*8</f>
-        <v>4224</v>
+        <v>12480</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
@@ -948,7 +1027,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>264</v>
+        <v>780</v>
       </c>
       <c r="D4" s="1">
         <v>1.25E-4</v>
@@ -964,7 +1043,7 @@
       </c>
       <c r="L4" s="5">
         <f>L3/D4</f>
-        <v>33792000</v>
+        <v>99840000</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
@@ -973,7 +1052,7 @@
       </c>
       <c r="L5" s="4">
         <f>L3*(1-(L4/E4))</f>
-        <v>2796.62592</v>
+        <v>19.968000000000572</v>
       </c>
     </row>
   </sheetData>
@@ -987,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB25049-F719-48DC-B24C-CE81CB877780}">
-  <dimension ref="B3:W93"/>
+  <dimension ref="B3:W124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="T77" sqref="T77:T78"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2901,16 +2980,624 @@
       <c r="V93" s="19"/>
       <c r="W93" s="21"/>
     </row>
+    <row r="96" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L96" s="6"/>
+      <c r="M96" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N96" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O96" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="P96" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q96" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R96" s="7"/>
+      <c r="S96" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="T96" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="U96" s="7"/>
+      <c r="V96" s="7"/>
+      <c r="W96" s="9"/>
+    </row>
+    <row r="97" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L97" s="10"/>
+      <c r="M97" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N97" s="12">
+        <v>2</v>
+      </c>
+      <c r="O97" s="12">
+        <v>88</v>
+      </c>
+      <c r="P97" s="12">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="Q97" s="13">
+        <v>100000000</v>
+      </c>
+      <c r="R97" s="11"/>
+      <c r="S97" s="1">
+        <v>1328.70144</v>
+      </c>
+      <c r="T97" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="U97" s="11"/>
+      <c r="V97" s="11"/>
+      <c r="W97" s="14"/>
+    </row>
+    <row r="98" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L98" s="10"/>
+      <c r="M98" s="11"/>
+      <c r="N98" s="11"/>
+      <c r="O98" s="11"/>
+      <c r="P98" s="11"/>
+      <c r="Q98" s="11"/>
+      <c r="R98" s="11"/>
+      <c r="S98" s="11"/>
+      <c r="T98" s="11"/>
+      <c r="U98" s="11"/>
+      <c r="V98" s="11"/>
+      <c r="W98" s="14"/>
+    </row>
+    <row r="99" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L99" s="10"/>
+      <c r="M99" s="11"/>
+      <c r="N99" s="11"/>
+      <c r="O99" s="11"/>
+      <c r="P99" s="11"/>
+      <c r="Q99" s="11"/>
+      <c r="R99" s="11"/>
+      <c r="S99" s="11"/>
+      <c r="T99" s="11"/>
+      <c r="U99" s="11"/>
+      <c r="V99" s="11"/>
+      <c r="W99" s="14"/>
+    </row>
+    <row r="100" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L100" s="10"/>
+      <c r="M100" s="11"/>
+      <c r="N100" s="11"/>
+      <c r="O100" s="11"/>
+      <c r="P100" s="11"/>
+      <c r="Q100" s="11"/>
+      <c r="R100" s="11"/>
+      <c r="S100" s="11"/>
+      <c r="T100" s="11"/>
+      <c r="U100" s="11"/>
+      <c r="V100" s="11"/>
+      <c r="W100" s="14"/>
+    </row>
+    <row r="101" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L101" s="10"/>
+      <c r="M101" s="11"/>
+      <c r="N101" s="11"/>
+      <c r="O101" s="11"/>
+      <c r="P101" s="11"/>
+      <c r="Q101" s="11"/>
+      <c r="R101" s="11"/>
+      <c r="S101" s="11"/>
+      <c r="T101" s="11"/>
+      <c r="U101" s="11"/>
+      <c r="V101" s="11"/>
+      <c r="W101" s="14"/>
+    </row>
+    <row r="102" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L102" s="10"/>
+      <c r="M102" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N102" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O102" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P102" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q102" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R102" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="S102" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="T102" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="U102" s="11"/>
+      <c r="V102" s="11"/>
+      <c r="W102" s="14"/>
+    </row>
+    <row r="103" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L103" s="10"/>
+      <c r="M103" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N103" s="15">
+        <v>2.3201402879999999E-4</v>
+      </c>
+      <c r="O103" s="15">
+        <v>2.5515479040000001E-4</v>
+      </c>
+      <c r="P103" s="15">
+        <v>2.7829555199999998E-4</v>
+      </c>
+      <c r="Q103" s="15">
+        <v>3.014363136E-4</v>
+      </c>
+      <c r="R103" s="15">
+        <v>3.2457707519999997E-4</v>
+      </c>
+      <c r="S103" s="15">
+        <v>2.656378368E-4</v>
+      </c>
+      <c r="T103" s="15">
+        <v>1.6571155968000001E-3</v>
+      </c>
+      <c r="U103" s="11"/>
+      <c r="V103" s="15"/>
+      <c r="W103" s="14"/>
+    </row>
+    <row r="104" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L104" s="10"/>
+      <c r="M104" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N104" s="15">
+        <v>2.1952000000000001E-4</v>
+      </c>
+      <c r="O104" s="15">
+        <v>2.4266076160000001E-4</v>
+      </c>
+      <c r="P104" s="15">
+        <v>2.6580152320000001E-4</v>
+      </c>
+      <c r="Q104" s="15">
+        <v>2.8736000000000001E-4</v>
+      </c>
+      <c r="R104" s="15">
+        <v>2.8736000000000001E-4</v>
+      </c>
+      <c r="S104" s="15">
+        <v>2.0528000000000001E-4</v>
+      </c>
+      <c r="T104" s="15">
+        <v>1.5079822847999999E-3</v>
+      </c>
+      <c r="U104" s="11"/>
+      <c r="V104" s="15"/>
+      <c r="W104" s="14"/>
+    </row>
+    <row r="105" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L105" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M105" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N105" s="15"/>
+      <c r="O105" s="15"/>
+      <c r="P105" s="15"/>
+      <c r="Q105" s="15"/>
+      <c r="R105" s="15"/>
+      <c r="S105" s="15"/>
+      <c r="T105" s="15">
+        <v>1.6571155968000001E-3</v>
+      </c>
+      <c r="U105" s="11"/>
+      <c r="V105" s="15"/>
+      <c r="W105" s="14"/>
+    </row>
+    <row r="106" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L106" s="10"/>
+      <c r="M106" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N106" s="15">
+        <v>2.1952000000000001E-4</v>
+      </c>
+      <c r="O106" s="15">
+        <v>2.4266076160000001E-4</v>
+      </c>
+      <c r="P106" s="15">
+        <v>2.6580152320000001E-4</v>
+      </c>
+      <c r="Q106" s="15">
+        <v>2.8736000000000001E-4</v>
+      </c>
+      <c r="R106" s="15">
+        <v>2.8736000000000001E-4</v>
+      </c>
+      <c r="S106" s="15">
+        <v>2.0528000000000001E-4</v>
+      </c>
+      <c r="T106" s="15">
+        <v>1.5079822847999999E-3</v>
+      </c>
+      <c r="U106" s="11"/>
+      <c r="V106" s="15"/>
+      <c r="W106" s="14"/>
+    </row>
+    <row r="107" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L107" s="10"/>
+      <c r="M107" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N107" s="15"/>
+      <c r="O107" s="15"/>
+      <c r="P107" s="15"/>
+      <c r="Q107" s="15"/>
+      <c r="R107" s="15"/>
+      <c r="S107" s="15"/>
+      <c r="T107" s="15">
+        <v>1.1771340288E-3</v>
+      </c>
+      <c r="U107" s="11"/>
+      <c r="V107" s="15"/>
+      <c r="W107" s="14"/>
+    </row>
+    <row r="108" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L108" s="10"/>
+      <c r="M108" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N108" s="15"/>
+      <c r="O108" s="15"/>
+      <c r="P108" s="15"/>
+      <c r="Q108" s="15"/>
+      <c r="R108" s="15"/>
+      <c r="S108" s="15"/>
+      <c r="T108" s="15">
+        <v>1.1771340288E-3</v>
+      </c>
+      <c r="U108" s="11"/>
+      <c r="V108" s="15"/>
+      <c r="W108" s="14"/>
+    </row>
+    <row r="109" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L109" s="10"/>
+      <c r="M109" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N109" s="15"/>
+      <c r="O109" s="15"/>
+      <c r="P109" s="15"/>
+      <c r="Q109" s="15"/>
+      <c r="R109" s="15"/>
+      <c r="S109" s="15"/>
+      <c r="T109" s="15">
+        <v>1.1771340288E-3</v>
+      </c>
+      <c r="U109" s="11"/>
+      <c r="V109" s="15"/>
+      <c r="W109" s="14"/>
+    </row>
+    <row r="110" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L110" s="10"/>
+      <c r="M110" s="11"/>
+      <c r="N110" s="11"/>
+      <c r="O110" s="11"/>
+      <c r="P110" s="11"/>
+      <c r="Q110" s="11"/>
+      <c r="R110" s="11"/>
+      <c r="S110" s="11"/>
+      <c r="T110" s="11"/>
+      <c r="U110" s="11"/>
+      <c r="V110" s="11"/>
+      <c r="W110" s="14"/>
+    </row>
+    <row r="111" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L111" s="10"/>
+      <c r="M111" s="11"/>
+      <c r="N111" s="11"/>
+      <c r="O111" s="11"/>
+      <c r="P111" s="11"/>
+      <c r="Q111" s="11"/>
+      <c r="R111" s="11"/>
+      <c r="S111" s="11"/>
+      <c r="T111" s="11"/>
+      <c r="U111" s="11"/>
+      <c r="V111" s="11"/>
+      <c r="W111" s="14"/>
+    </row>
+    <row r="112" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L112" s="10"/>
+      <c r="M112" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N112" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="O112" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P112" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q112" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="R112" s="11"/>
+      <c r="S112" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="T112" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="U112" s="11"/>
+      <c r="V112" s="11"/>
+      <c r="W112" s="14"/>
+    </row>
+    <row r="113" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L113" s="10"/>
+      <c r="M113" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N113" s="12">
+        <v>2</v>
+      </c>
+      <c r="O113" s="12">
+        <v>512</v>
+      </c>
+      <c r="P113" s="12">
+        <v>1.25E-4</v>
+      </c>
+      <c r="Q113" s="13">
+        <v>100000000</v>
+      </c>
+      <c r="R113" s="11"/>
+      <c r="S113" s="22">
+        <v>2823.2908799000002</v>
+      </c>
+      <c r="T113" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="U113" s="11"/>
+      <c r="V113" s="11"/>
+      <c r="W113" s="14"/>
+    </row>
+    <row r="114" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L114" s="10"/>
+      <c r="M114" s="11"/>
+      <c r="N114" s="11"/>
+      <c r="O114" s="11"/>
+      <c r="P114" s="11"/>
+      <c r="Q114" s="11"/>
+      <c r="R114" s="11"/>
+      <c r="S114" s="11"/>
+      <c r="T114" s="11"/>
+      <c r="U114" s="11"/>
+      <c r="V114" s="11"/>
+      <c r="W114" s="14"/>
+    </row>
+    <row r="115" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L115" s="10"/>
+      <c r="M115" s="11"/>
+      <c r="N115" s="11"/>
+      <c r="O115" s="11"/>
+      <c r="P115" s="11"/>
+      <c r="Q115" s="11"/>
+      <c r="R115" s="11"/>
+      <c r="S115" s="11"/>
+      <c r="T115" s="11"/>
+      <c r="U115" s="11"/>
+      <c r="V115" s="11"/>
+      <c r="W115" s="14"/>
+    </row>
+    <row r="116" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L116" s="10"/>
+      <c r="M116" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N116" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O116" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P116" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q116" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R116" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="S116" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="T116" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="U116" s="11"/>
+      <c r="V116" s="11"/>
+      <c r="W116" s="14"/>
+    </row>
+    <row r="117" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L117" s="10"/>
+      <c r="M117" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N117" s="15">
+        <v>2.3629163519999901E-4</v>
+      </c>
+      <c r="O117" s="15">
+        <v>5.5967247360000003E-4</v>
+      </c>
+      <c r="P117" s="15"/>
+      <c r="Q117" s="15"/>
+      <c r="R117" s="15"/>
+      <c r="S117" s="15"/>
+      <c r="T117" s="15">
+        <v>7.9596410879999996E-4</v>
+      </c>
+      <c r="U117" s="11"/>
+      <c r="V117" s="15"/>
+      <c r="W117" s="14"/>
+    </row>
+    <row r="118" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L118" s="10"/>
+      <c r="M118" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N118" s="15">
+        <v>2.3629163519999901E-4</v>
+      </c>
+      <c r="O118" s="15">
+        <v>2.8719999999999999E-4</v>
+      </c>
+      <c r="P118" s="15"/>
+      <c r="Q118" s="15"/>
+      <c r="R118" s="15"/>
+      <c r="S118" s="15"/>
+      <c r="T118" s="15">
+        <v>5.2349163519999997E-4</v>
+      </c>
+      <c r="U118" s="11"/>
+      <c r="V118" s="15"/>
+      <c r="W118" s="14"/>
+    </row>
+    <row r="119" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L119" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="M119" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N119" s="15">
+        <v>2.3629163519999901E-4</v>
+      </c>
+      <c r="O119" s="15">
+        <v>5.3344000000000004E-4</v>
+      </c>
+      <c r="P119" s="15"/>
+      <c r="Q119" s="15"/>
+      <c r="R119" s="15"/>
+      <c r="S119" s="15"/>
+      <c r="T119" s="15">
+        <v>7.6973163519999997E-4</v>
+      </c>
+      <c r="U119" s="11"/>
+      <c r="V119" s="15"/>
+      <c r="W119" s="14"/>
+    </row>
+    <row r="120" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L120" s="10"/>
+      <c r="M120" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N120" s="15">
+        <v>2.3629163519999901E-4</v>
+      </c>
+      <c r="O120" s="15">
+        <v>2.8719999999999999E-4</v>
+      </c>
+      <c r="P120" s="15"/>
+      <c r="Q120" s="15"/>
+      <c r="R120" s="15"/>
+      <c r="S120" s="15"/>
+      <c r="T120" s="15">
+        <v>5.2349163519999997E-4</v>
+      </c>
+      <c r="U120" s="11"/>
+      <c r="V120" s="15"/>
+      <c r="W120" s="14"/>
+    </row>
+    <row r="121" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L121" s="10"/>
+      <c r="M121" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N121" s="15"/>
+      <c r="O121" s="15"/>
+      <c r="P121" s="15"/>
+      <c r="Q121" s="15"/>
+      <c r="R121" s="15"/>
+      <c r="S121" s="15"/>
+      <c r="T121" s="15">
+        <v>3.5965163520000002E-4</v>
+      </c>
+      <c r="U121" s="11"/>
+      <c r="V121" s="15"/>
+      <c r="W121" s="14"/>
+    </row>
+    <row r="122" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L122" s="10"/>
+      <c r="M122" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N122" s="15"/>
+      <c r="O122" s="15"/>
+      <c r="P122" s="15"/>
+      <c r="Q122" s="15"/>
+      <c r="R122" s="15"/>
+      <c r="S122" s="15"/>
+      <c r="T122" s="15">
+        <v>3.5965163520000002E-4</v>
+      </c>
+      <c r="U122" s="11"/>
+      <c r="V122" s="15"/>
+      <c r="W122" s="14"/>
+    </row>
+    <row r="123" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L123" s="10"/>
+      <c r="M123" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N123" s="15"/>
+      <c r="O123" s="15"/>
+      <c r="P123" s="15"/>
+      <c r="Q123" s="15"/>
+      <c r="R123" s="15"/>
+      <c r="S123" s="15"/>
+      <c r="T123" s="15">
+        <v>3.5965163520000002E-4</v>
+      </c>
+      <c r="U123" s="11"/>
+      <c r="V123" s="15"/>
+      <c r="W123" s="14"/>
+    </row>
+    <row r="124" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L124" s="18"/>
+      <c r="M124" s="19"/>
+      <c r="N124" s="19"/>
+      <c r="O124" s="19"/>
+      <c r="P124" s="19"/>
+      <c r="Q124" s="19"/>
+      <c r="R124" s="19"/>
+      <c r="S124" s="19"/>
+      <c r="T124" s="19"/>
+      <c r="U124" s="19"/>
+      <c r="V124" s="19"/>
+      <c r="W124" s="21"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="6">
+  <tableParts count="8">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CBSLine evaluation with MFS of 780Byte
</commit_message>
<xml_diff>
--- a/src/main/java/org/networkcalculus/dnc/demos/Eval_CBSLine/Eval_CBSLine_Results.xlsx
+++ b/src/main/java/org/networkcalculus/dnc/demos/Eval_CBSLine/Eval_CBSLine_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ForceXX\Documents\Studium\FAU_Informatik_Master\FS5\Masterarbeit\Network_Calculus_in_TSN\DNC\IntelliJ\src\main\java\org\networkcalculus\dnc\demos\Eval_CBSLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE109720-B8B8-4500-8C31-B8D54B3A16A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83D647F-EFE6-4468-9530-44933C0A399A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3192" windowWidth="46080" windowHeight="22152" activeTab="1" xr2:uid="{76093B85-C4EA-4FAC-BB07-8F5ADEBC9C5C}"/>
+    <workbookView xWindow="0" yWindow="3648" windowWidth="46080" windowHeight="22152" activeTab="1" xr2:uid="{76093B85-C4EA-4FAC-BB07-8F5ADEBC9C5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="37">
   <si>
     <t>f1</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>65,536MBit/s</t>
+  </si>
+  <si>
+    <t>99,84MBit/s</t>
   </si>
 </sst>
 </file>
@@ -260,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -309,11 +312,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="70">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
     </dxf>
@@ -555,13 +601,30 @@
   <autoFilter ref="M9:T16" xr:uid="{AFD0FDAD-B567-49C8-A37C-DCEECED05009}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{BE6FA1AF-957C-4302-ABCA-3CED577909FB}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{EABB3472-FB4D-420C-9C6B-D5FBAEE8D4FF}" name="S1" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{362B0664-EECB-41EA-8E6D-BC83B9D56EFC}" name="S2" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{6AAC6F6B-16ED-403D-9C2D-403BD383643D}" name="S3" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{AD2D3DC2-A063-43E3-8F4D-72B5648D83E8}" name="S4" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{1ACA20C8-E74E-4AE0-9617-8D84870DB044}" name="S5" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{5FFF2E6B-00A8-47E0-8FF6-2C25AA61CD2E}" name="S6" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{59937D66-C814-42EC-A281-7F9615B9AC54}" name="Total" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{EABB3472-FB4D-420C-9C6B-D5FBAEE8D4FF}" name="S1" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{362B0664-EECB-41EA-8E6D-BC83B9D56EFC}" name="S2" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{6AAC6F6B-16ED-403D-9C2D-403BD383643D}" name="S3" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{AD2D3DC2-A063-43E3-8F4D-72B5648D83E8}" name="S4" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{1ACA20C8-E74E-4AE0-9617-8D84870DB044}" name="S5" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{5FFF2E6B-00A8-47E0-8FF6-2C25AA61CD2E}" name="S6" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{59937D66-C814-42EC-A281-7F9615B9AC54}" name="Total" dataDxfId="63"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{958BE0E6-6C6F-4596-BACE-B5052141E776}" name="Tabelle1357911" displayName="Tabelle1357911" ref="M147:T154" totalsRowShown="0">
+  <autoFilter ref="M147:T154" xr:uid="{2891661D-836E-47DB-BD40-F3A27A090E4F}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{5ED748F3-0EF7-490E-9255-D93E2E8A38B3}" name="Analysis"/>
+    <tableColumn id="2" xr3:uid="{A96E6DCE-0CD4-444C-AC15-B039A4AD73D3}" name="S1" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{A38F3CDE-3B3B-46A2-8F23-68228377ED85}" name="S2" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{8B8B1AD0-037F-4F96-A7E6-AD0731A1A674}" name="S3" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{C2CC595E-C7DA-4A76-917C-24B06D46A036}" name="S4" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{68190FF9-32AD-4425-9D62-C708869AA72B}" name="S5" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{FA329009-A789-402C-A1BE-8BA2289036EA}" name="S6" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{F099B37D-2BC9-4533-80BD-70060862C629}" name="Total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -572,13 +635,13 @@
   <autoFilter ref="M23:T30" xr:uid="{9F3FFC4E-8857-417C-879B-7E46756E6ACB}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{6C7A2137-FE16-4D18-B3E5-47340E52F2D5}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{EDDA7831-D99A-413F-AA04-C00A206D6D34}" name="S1" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{3CB5E796-20A3-4C92-9FC5-590D66DC5593}" name="S2" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{3D106F77-8448-4063-87F7-7B7BE008B2F2}" name="S3" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{A891D787-2819-425A-9CE0-E8145AC0C05B}" name="S4" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{C6263B6C-6BFC-46DD-94D3-5EDB5A4EAF2F}" name="S5" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{AAC57713-C8ED-436C-B744-473CD5CFAB13}" name="S6" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{31F74DD7-5067-4854-B832-9EFA7B4543EA}" name="Total" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{EDDA7831-D99A-413F-AA04-C00A206D6D34}" name="S1" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{3CB5E796-20A3-4C92-9FC5-590D66DC5593}" name="S2" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{3D106F77-8448-4063-87F7-7B7BE008B2F2}" name="S3" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{A891D787-2819-425A-9CE0-E8145AC0C05B}" name="S4" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{C6263B6C-6BFC-46DD-94D3-5EDB5A4EAF2F}" name="S5" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{AAC57713-C8ED-436C-B744-473CD5CFAB13}" name="S6" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{31F74DD7-5067-4854-B832-9EFA7B4543EA}" name="Total" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -589,13 +652,13 @@
   <autoFilter ref="M40:T47" xr:uid="{E16230B5-F45F-4647-925B-5EE18F895F9C}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9D1375EE-0D83-4727-B0F9-FE752E8A0CBC}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{C37D03EB-F7B2-4349-B2CC-726DB4010C90}" name="S1" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{7037993D-3D73-4283-A3B4-93C5B4E6E202}" name="S2" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{7ADA14D4-6575-4C8D-A7EA-C47F389375CE}" name="S3" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{5429F400-2F0F-4356-AC4A-9C65390A88EF}" name="S4" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{65870CF8-359E-4FAC-947D-39633692A667}" name="S5" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{59753DB4-DBE6-466A-BCC2-D1C2D56D1A27}" name="S6" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{51BDBB4F-8359-4885-B4D7-DF406809ECB7}" name="Total" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{C37D03EB-F7B2-4349-B2CC-726DB4010C90}" name="S1" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{7037993D-3D73-4283-A3B4-93C5B4E6E202}" name="S2" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{7ADA14D4-6575-4C8D-A7EA-C47F389375CE}" name="S3" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{5429F400-2F0F-4356-AC4A-9C65390A88EF}" name="S4" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{65870CF8-359E-4FAC-947D-39633692A667}" name="S5" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{59753DB4-DBE6-466A-BCC2-D1C2D56D1A27}" name="S6" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{51BDBB4F-8359-4885-B4D7-DF406809ECB7}" name="Total" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -606,13 +669,13 @@
   <autoFilter ref="M54:T61" xr:uid="{B5EBC119-6892-4EFB-AB7E-F78E33D432A9}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0BB4E427-3492-4DCF-9D08-38551180E6EE}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{625D768D-2EA2-4E64-B741-35AF2819C1F7}" name="S1" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{2FA180EB-2936-481F-B1D1-4C1DA624FA57}" name="S2" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{7EDAFDAC-585A-4749-ABD8-DEBBA52F7B86}" name="S3" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{3E05A679-5166-455F-9DE8-C76697485C01}" name="S4" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{9611ADE2-11EE-403F-8E25-5BF3FD83A7EE}" name="S5" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{4B5CC043-D947-410A-8D8E-B4B1EDA50E93}" name="S6" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{90BF4DC0-8F16-4F8E-AD7A-04145C27A52D}" name="Total" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{625D768D-2EA2-4E64-B741-35AF2819C1F7}" name="S1" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{2FA180EB-2936-481F-B1D1-4C1DA624FA57}" name="S2" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{7EDAFDAC-585A-4749-ABD8-DEBBA52F7B86}" name="S3" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{3E05A679-5166-455F-9DE8-C76697485C01}" name="S4" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{9611ADE2-11EE-403F-8E25-5BF3FD83A7EE}" name="S5" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{4B5CC043-D947-410A-8D8E-B4B1EDA50E93}" name="S6" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{90BF4DC0-8F16-4F8E-AD7A-04145C27A52D}" name="Total" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -623,13 +686,13 @@
   <autoFilter ref="M71:T78" xr:uid="{51782671-9EEB-46B0-812D-DE4D14A213EE}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{AD5E4FB3-F32D-4B93-86CA-C7ECF985973B}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{32771DFC-FFFB-479C-8088-AA245ED9B201}" name="S1" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{850259B7-F6FC-40B4-94B0-436FE4A42169}" name="S2" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{D83AC1AB-1A0A-4527-925F-218D72D2227A}" name="S3" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{9AE7B8F5-E983-41B9-B1F4-4FC70710981E}" name="S4" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{BF918F35-6CDD-4DEE-956C-2A3434C345D0}" name="S5" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{8BF14E06-E1BE-45C5-B2AF-D712C65491A2}" name="S6" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{386EE86E-EBB8-4A4D-B17D-421040C58630}" name="Total" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{32771DFC-FFFB-479C-8088-AA245ED9B201}" name="S1" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{850259B7-F6FC-40B4-94B0-436FE4A42169}" name="S2" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{D83AC1AB-1A0A-4527-925F-218D72D2227A}" name="S3" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{9AE7B8F5-E983-41B9-B1F4-4FC70710981E}" name="S4" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{BF918F35-6CDD-4DEE-956C-2A3434C345D0}" name="S5" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{8BF14E06-E1BE-45C5-B2AF-D712C65491A2}" name="S6" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{386EE86E-EBB8-4A4D-B17D-421040C58630}" name="Total" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -640,13 +703,13 @@
   <autoFilter ref="M85:T92" xr:uid="{B8C55D2C-921B-49DD-AC76-772D4A43E64D}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{1B1BABD6-FD5C-41BB-948A-6FC0BCC11D24}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{DB6F9D20-C97E-480C-99B2-E87E4A9E1E0E}" name="S1" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{6D579111-6BD1-4C25-A59D-5752C6D1027B}" name="S2" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{971D35F8-9047-4D4E-B3A8-1050E4CBB9F7}" name="S3" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{12EA7A8D-ED74-4686-A548-2A70B019DDD4}" name="S4" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{1FE3C278-2C61-4E80-AD86-3FA5279E30B5}" name="S5" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{EE077AF3-1AB4-421C-B5DC-9511794D8F8E}" name="S6" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{4D81D46E-0FA9-4BFC-8316-8FE6191F7B12}" name="Total" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{DB6F9D20-C97E-480C-99B2-E87E4A9E1E0E}" name="S1" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{6D579111-6BD1-4C25-A59D-5752C6D1027B}" name="S2" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{971D35F8-9047-4D4E-B3A8-1050E4CBB9F7}" name="S3" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{12EA7A8D-ED74-4686-A548-2A70B019DDD4}" name="S4" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{1FE3C278-2C61-4E80-AD86-3FA5279E30B5}" name="S5" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{EE077AF3-1AB4-421C-B5DC-9511794D8F8E}" name="S6" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{4D81D46E-0FA9-4BFC-8316-8FE6191F7B12}" name="Total" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -657,13 +720,13 @@
   <autoFilter ref="M102:T109" xr:uid="{3B58D87F-510B-43F0-BC7D-8EF14E94029E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E6C46FA4-813C-4003-A6A1-34967D676206}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{C1B5C27C-40D8-4CE6-8300-D32B61DBD03E}" name="S1" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{822EBEC2-E9F3-433C-9D06-01D83E51B4EC}" name="S2" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{7E24F410-F931-4EB2-B8F2-71F614752416}" name="S3" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{6F4DDE75-12D5-4E09-BD4C-B84DBE3A1613}" name="S4" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{D1A7BB02-6526-44E4-BAC4-F951ACEB49E0}" name="S5" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{CA43AF65-8F45-41AF-809C-76D07CBDCA7B}" name="S6" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{AA305A43-F356-44F9-B1BE-8A8539A588B2}" name="Total" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{C1B5C27C-40D8-4CE6-8300-D32B61DBD03E}" name="S1" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{822EBEC2-E9F3-433C-9D06-01D83E51B4EC}" name="S2" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{7E24F410-F931-4EB2-B8F2-71F614752416}" name="S3" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{6F4DDE75-12D5-4E09-BD4C-B84DBE3A1613}" name="S4" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{D1A7BB02-6526-44E4-BAC4-F951ACEB49E0}" name="S5" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{CA43AF65-8F45-41AF-809C-76D07CBDCA7B}" name="S6" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{AA305A43-F356-44F9-B1BE-8A8539A588B2}" name="Total" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -674,13 +737,30 @@
   <autoFilter ref="M116:T123" xr:uid="{BBD41544-5CF6-451E-B19F-AA4B349E0FF5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F68E10CC-FD59-48C5-91A8-4F747980D2B8}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{091DCD40-AFF4-4A35-A51B-5CE995B27C5B}" name="S1" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{32F634D5-1211-4A7C-8411-0DC8BF7C0116}" name="S2" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{BE2DA717-3CEA-4B45-9D01-B2AF2CFBA155}" name="S3" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{820A1FC2-AB1F-424D-8760-928CAC5CEC89}" name="S4" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{7CDBF264-CA71-4555-AD13-B4F0B0EFF5CB}" name="S5" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{FD7873DE-5A47-42D5-BE83-3AC049767285}" name="S6" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{514BF621-1FB2-46A5-A883-5F156AE64F89}" name="Total" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{091DCD40-AFF4-4A35-A51B-5CE995B27C5B}" name="S1" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{32F634D5-1211-4A7C-8411-0DC8BF7C0116}" name="S2" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{BE2DA717-3CEA-4B45-9D01-B2AF2CFBA155}" name="S3" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{820A1FC2-AB1F-424D-8760-928CAC5CEC89}" name="S4" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{7CDBF264-CA71-4555-AD13-B4F0B0EFF5CB}" name="S5" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{FD7873DE-5A47-42D5-BE83-3AC049767285}" name="S6" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{514BF621-1FB2-46A5-A883-5F156AE64F89}" name="Total" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{04AFCDBD-3784-45BA-AA96-4CC754756FF3}" name="Tabelle146810" displayName="Tabelle146810" ref="M133:T140" totalsRowShown="0">
+  <autoFilter ref="M133:T140" xr:uid="{FB41092D-F5FF-4971-9DDD-C9E03FD01631}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{6647CD1D-0845-4A23-9836-FBC960574DA7}" name="Analysis"/>
+    <tableColumn id="2" xr3:uid="{5BD82A11-F2EA-4903-B53D-DD982E06A315}" name="S1" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{424AE262-E0C8-44A2-B28D-3F028CA6231F}" name="S2" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{D576FA30-995E-46FE-8DB0-5798DAE28331}" name="S3" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{B630E084-8616-40E7-A93B-DA34C763EADC}" name="S4" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{04C38EE3-C04A-4AE3-B01D-D5CC7EEF4DE2}" name="S5" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{68C4544A-4832-4B5A-9EE3-E132B259AACC}" name="S6" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{71294977-C366-4F0A-B7E5-972975477A7D}" name="Total" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -986,7 +1066,7 @@
   <dimension ref="B3:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1066,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB25049-F719-48DC-B24C-CE81CB877780}">
-  <dimension ref="B3:W124"/>
+  <dimension ref="B3:W155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,7 +1159,6 @@
     <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="20" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="12:23" x14ac:dyDescent="0.3">
@@ -3586,10 +3665,628 @@
       <c r="V124" s="19"/>
       <c r="W124" s="21"/>
     </row>
+    <row r="127" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L127" s="6"/>
+      <c r="M127" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N127" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O127" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="P127" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q127" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R127" s="7"/>
+      <c r="S127" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="T127" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="U127" s="7"/>
+      <c r="V127" s="7"/>
+      <c r="W127" s="9"/>
+    </row>
+    <row r="128" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L128" s="10"/>
+      <c r="M128" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N128" s="12">
+        <v>2</v>
+      </c>
+      <c r="O128" s="12">
+        <v>88</v>
+      </c>
+      <c r="P128" s="12">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="Q128" s="13">
+        <v>100000000</v>
+      </c>
+      <c r="R128" s="11"/>
+      <c r="S128" s="1">
+        <v>1328.70144</v>
+      </c>
+      <c r="T128" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="U128" s="11"/>
+      <c r="V128" s="11"/>
+      <c r="W128" s="14"/>
+    </row>
+    <row r="129" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L129" s="10"/>
+      <c r="M129" s="11"/>
+      <c r="N129" s="11"/>
+      <c r="O129" s="11"/>
+      <c r="P129" s="11"/>
+      <c r="Q129" s="11"/>
+      <c r="R129" s="11"/>
+      <c r="S129" s="11"/>
+      <c r="T129" s="11"/>
+      <c r="U129" s="11"/>
+      <c r="V129" s="11"/>
+      <c r="W129" s="14"/>
+    </row>
+    <row r="130" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L130" s="10"/>
+      <c r="M130" s="11"/>
+      <c r="N130" s="11"/>
+      <c r="O130" s="11"/>
+      <c r="P130" s="11"/>
+      <c r="Q130" s="11"/>
+      <c r="R130" s="11"/>
+      <c r="S130" s="11"/>
+      <c r="T130" s="11"/>
+      <c r="U130" s="11"/>
+      <c r="V130" s="11"/>
+      <c r="W130" s="14"/>
+    </row>
+    <row r="131" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L131" s="10"/>
+      <c r="M131" s="11"/>
+      <c r="N131" s="11"/>
+      <c r="O131" s="11"/>
+      <c r="P131" s="11"/>
+      <c r="Q131" s="11"/>
+      <c r="R131" s="11"/>
+      <c r="S131" s="11"/>
+      <c r="T131" s="11"/>
+      <c r="U131" s="11"/>
+      <c r="V131" s="11"/>
+      <c r="W131" s="14"/>
+    </row>
+    <row r="132" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L132" s="10"/>
+      <c r="M132" s="11"/>
+      <c r="N132" s="11"/>
+      <c r="O132" s="11"/>
+      <c r="P132" s="11"/>
+      <c r="Q132" s="11"/>
+      <c r="R132" s="11"/>
+      <c r="S132" s="11"/>
+      <c r="T132" s="11"/>
+      <c r="U132" s="11"/>
+      <c r="V132" s="11"/>
+      <c r="W132" s="14"/>
+    </row>
+    <row r="133" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L133" s="10"/>
+      <c r="M133" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N133" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O133" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P133" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q133" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R133" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="S133" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="T133" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="U133" s="11"/>
+      <c r="V133" s="11"/>
+      <c r="W133" s="14"/>
+    </row>
+    <row r="134" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L134" s="10"/>
+      <c r="M134" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N134" s="15">
+        <v>2.534540288E-4</v>
+      </c>
+      <c r="O134" s="15">
+        <v>2.7900979199999899E-4</v>
+      </c>
+      <c r="P134" s="15">
+        <v>3.0456555519999998E-4</v>
+      </c>
+      <c r="Q134" s="15">
+        <v>3.301213184E-4</v>
+      </c>
+      <c r="R134" s="15">
+        <v>3.5567708159999899E-4</v>
+      </c>
+      <c r="S134" s="15">
+        <v>2.7771284479999997E-4</v>
+      </c>
+      <c r="T134" s="15">
+        <v>1.8005406207999999E-3</v>
+      </c>
+      <c r="U134" s="11"/>
+      <c r="V134" s="15"/>
+      <c r="W134" s="14"/>
+    </row>
+    <row r="135" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L135" s="10"/>
+      <c r="M135" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N135" s="15">
+        <v>2.4096E-4</v>
+      </c>
+      <c r="O135" s="15">
+        <v>2.6651576319999999E-4</v>
+      </c>
+      <c r="P135" s="15">
+        <v>2.9207152640000001E-4</v>
+      </c>
+      <c r="Q135" s="15">
+        <v>3.1762728959999997E-4</v>
+      </c>
+      <c r="R135" s="15">
+        <v>3.4318305279999999E-4</v>
+      </c>
+      <c r="S135" s="15">
+        <v>2.4815999999999998E-4</v>
+      </c>
+      <c r="T135" s="15">
+        <v>1.708517632E-3</v>
+      </c>
+      <c r="U135" s="11"/>
+      <c r="V135" s="15"/>
+      <c r="W135" s="14"/>
+    </row>
+    <row r="136" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L136" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M136" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N136" s="15">
+        <v>2.534540288E-4</v>
+      </c>
+      <c r="O136" s="15">
+        <v>2.7900979199999899E-4</v>
+      </c>
+      <c r="P136" s="15">
+        <v>3.0456555519999998E-4</v>
+      </c>
+      <c r="Q136" s="15">
+        <v>3.301213184E-4</v>
+      </c>
+      <c r="R136" s="15">
+        <v>3.5567708159999899E-4</v>
+      </c>
+      <c r="S136" s="15">
+        <v>2.7771284479999997E-4</v>
+      </c>
+      <c r="T136" s="15">
+        <v>1.8005406207999999E-3</v>
+      </c>
+      <c r="U136" s="11"/>
+      <c r="V136" s="15"/>
+      <c r="W136" s="14"/>
+    </row>
+    <row r="137" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L137" s="10"/>
+      <c r="M137" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N137" s="15">
+        <v>2.4096E-4</v>
+      </c>
+      <c r="O137" s="15">
+        <v>2.6651576319999999E-4</v>
+      </c>
+      <c r="P137" s="15">
+        <v>2.9207152640000001E-4</v>
+      </c>
+      <c r="Q137" s="15">
+        <v>3.1762728959999997E-4</v>
+      </c>
+      <c r="R137" s="15">
+        <v>3.4318305279999999E-4</v>
+      </c>
+      <c r="S137" s="15">
+        <v>2.4815999999999998E-4</v>
+      </c>
+      <c r="T137" s="15">
+        <v>1.708517632E-3</v>
+      </c>
+      <c r="U137" s="11"/>
+      <c r="V137" s="15"/>
+      <c r="W137" s="14"/>
+    </row>
+    <row r="138" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L138" s="10"/>
+      <c r="M138" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N138" s="15"/>
+      <c r="O138" s="15"/>
+      <c r="P138" s="15"/>
+      <c r="Q138" s="15"/>
+      <c r="R138" s="15"/>
+      <c r="S138" s="15"/>
+      <c r="T138" s="15">
+        <v>1.2843340288E-3</v>
+      </c>
+      <c r="U138" s="11"/>
+      <c r="V138" s="15"/>
+      <c r="W138" s="14"/>
+    </row>
+    <row r="139" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L139" s="10"/>
+      <c r="M139" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N139" s="15"/>
+      <c r="O139" s="15"/>
+      <c r="P139" s="15"/>
+      <c r="Q139" s="15"/>
+      <c r="R139" s="15"/>
+      <c r="S139" s="15"/>
+      <c r="T139" s="15">
+        <v>1.2843340288E-3</v>
+      </c>
+      <c r="U139" s="11"/>
+      <c r="V139" s="15"/>
+      <c r="W139" s="14"/>
+    </row>
+    <row r="140" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L140" s="10"/>
+      <c r="M140" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N140" s="15"/>
+      <c r="O140" s="15"/>
+      <c r="P140" s="15"/>
+      <c r="Q140" s="15"/>
+      <c r="R140" s="15"/>
+      <c r="S140" s="15"/>
+      <c r="T140" s="15">
+        <v>1.2843340288E-3</v>
+      </c>
+      <c r="U140" s="11"/>
+      <c r="V140" s="15"/>
+      <c r="W140" s="14"/>
+    </row>
+    <row r="141" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L141" s="10"/>
+      <c r="M141" s="11"/>
+      <c r="N141" s="11"/>
+      <c r="O141" s="11"/>
+      <c r="P141" s="11"/>
+      <c r="Q141" s="11"/>
+      <c r="R141" s="11"/>
+      <c r="S141" s="11"/>
+      <c r="T141" s="11"/>
+      <c r="U141" s="11"/>
+      <c r="V141" s="11"/>
+      <c r="W141" s="14"/>
+    </row>
+    <row r="142" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L142" s="10"/>
+      <c r="M142" s="11"/>
+      <c r="N142" s="11"/>
+      <c r="O142" s="11"/>
+      <c r="P142" s="11"/>
+      <c r="Q142" s="11"/>
+      <c r="R142" s="11"/>
+      <c r="S142" s="11"/>
+      <c r="T142" s="11"/>
+      <c r="U142" s="11"/>
+      <c r="V142" s="11"/>
+      <c r="W142" s="14"/>
+    </row>
+    <row r="143" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L143" s="10"/>
+      <c r="M143" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N143" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="O143" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P143" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q143" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="R143" s="11"/>
+      <c r="S143" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="T143" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="U143" s="11"/>
+      <c r="V143" s="11"/>
+      <c r="W143" s="14"/>
+    </row>
+    <row r="144" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L144" s="10"/>
+      <c r="M144" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N144" s="12">
+        <v>2</v>
+      </c>
+      <c r="O144" s="12">
+        <v>780</v>
+      </c>
+      <c r="P144" s="12">
+        <v>1.25E-4</v>
+      </c>
+      <c r="Q144" s="13">
+        <v>100000000</v>
+      </c>
+      <c r="R144" s="11"/>
+      <c r="S144" s="22">
+        <v>19.968000000000501</v>
+      </c>
+      <c r="T144" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="U144" s="11"/>
+      <c r="V144" s="11"/>
+      <c r="W144" s="14"/>
+    </row>
+    <row r="145" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L145" s="10"/>
+      <c r="M145" s="11"/>
+      <c r="N145" s="11"/>
+      <c r="O145" s="11"/>
+      <c r="P145" s="11"/>
+      <c r="Q145" s="11"/>
+      <c r="R145" s="11"/>
+      <c r="S145" s="11"/>
+      <c r="T145" s="11"/>
+      <c r="U145" s="11"/>
+      <c r="V145" s="11"/>
+      <c r="W145" s="14"/>
+    </row>
+    <row r="146" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L146" s="10"/>
+      <c r="M146" s="11"/>
+      <c r="N146" s="11"/>
+      <c r="O146" s="11"/>
+      <c r="P146" s="11"/>
+      <c r="Q146" s="11"/>
+      <c r="R146" s="11"/>
+      <c r="S146" s="11"/>
+      <c r="T146" s="11"/>
+      <c r="U146" s="11"/>
+      <c r="V146" s="11"/>
+      <c r="W146" s="14"/>
+    </row>
+    <row r="147" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L147" s="10"/>
+      <c r="M147" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N147" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O147" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P147" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q147" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R147" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="S147" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="T147" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="U147" s="11"/>
+      <c r="V147" s="11"/>
+      <c r="W147" s="14"/>
+    </row>
+    <row r="148" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L148" s="10"/>
+      <c r="M148" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N148" s="24">
+        <v>1.2415872E-4</v>
+      </c>
+      <c r="O148" s="24">
+        <v>6.1680921599999996E-4</v>
+      </c>
+      <c r="P148" s="24"/>
+      <c r="Q148" s="24"/>
+      <c r="R148" s="24"/>
+      <c r="S148" s="24"/>
+      <c r="T148" s="24">
+        <v>7.4096793599999998E-4</v>
+      </c>
+      <c r="U148" s="11"/>
+      <c r="V148" s="15"/>
+      <c r="W148" s="14"/>
+    </row>
+    <row r="149" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L149" s="10"/>
+      <c r="M149" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N149" s="15">
+        <v>1.2415872E-4</v>
+      </c>
+      <c r="O149" s="15">
+        <v>3.7295999999999998E-4</v>
+      </c>
+      <c r="P149" s="15"/>
+      <c r="Q149" s="15"/>
+      <c r="R149" s="15"/>
+      <c r="S149" s="15"/>
+      <c r="T149" s="15">
+        <v>4.9711872E-4</v>
+      </c>
+      <c r="U149" s="11"/>
+      <c r="V149" s="15"/>
+      <c r="W149" s="14"/>
+    </row>
+    <row r="150" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L150" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="M150" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N150" s="24">
+        <v>1.2415872E-4</v>
+      </c>
+      <c r="O150" s="24">
+        <v>6.1680921599999996E-4</v>
+      </c>
+      <c r="P150" s="24"/>
+      <c r="Q150" s="24"/>
+      <c r="R150" s="24"/>
+      <c r="S150" s="24"/>
+      <c r="T150" s="24">
+        <v>7.4096793599999998E-4</v>
+      </c>
+      <c r="U150" s="11"/>
+      <c r="V150" s="15"/>
+      <c r="W150" s="14"/>
+    </row>
+    <row r="151" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L151" s="10"/>
+      <c r="M151" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N151" s="15">
+        <v>1.2415872E-4</v>
+      </c>
+      <c r="O151" s="15">
+        <v>3.7295999999999998E-4</v>
+      </c>
+      <c r="P151" s="15"/>
+      <c r="Q151" s="15"/>
+      <c r="R151" s="15"/>
+      <c r="S151" s="15"/>
+      <c r="T151" s="15">
+        <v>4.9711872E-4</v>
+      </c>
+      <c r="U151" s="11"/>
+      <c r="V151" s="15"/>
+      <c r="W151" s="14"/>
+    </row>
+    <row r="152" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L152" s="10"/>
+      <c r="M152" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N152" s="15"/>
+      <c r="O152" s="15"/>
+      <c r="P152" s="15"/>
+      <c r="Q152" s="15"/>
+      <c r="R152" s="15"/>
+      <c r="S152" s="15"/>
+      <c r="T152" s="15">
+        <v>2.4751872000000001E-4</v>
+      </c>
+      <c r="U152" s="11"/>
+      <c r="V152" s="15"/>
+      <c r="W152" s="14"/>
+    </row>
+    <row r="153" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L153" s="10"/>
+      <c r="M153" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N153" s="15"/>
+      <c r="O153" s="15"/>
+      <c r="P153" s="15"/>
+      <c r="Q153" s="15"/>
+      <c r="R153" s="15"/>
+      <c r="S153" s="15"/>
+      <c r="T153" s="15">
+        <v>2.4751872000000001E-4</v>
+      </c>
+      <c r="U153" s="11"/>
+      <c r="V153" s="15"/>
+      <c r="W153" s="14"/>
+    </row>
+    <row r="154" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L154" s="10"/>
+      <c r="M154" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N154" s="15"/>
+      <c r="O154" s="15"/>
+      <c r="P154" s="15"/>
+      <c r="Q154" s="15"/>
+      <c r="R154" s="15"/>
+      <c r="S154" s="15"/>
+      <c r="T154" s="15">
+        <v>2.4751872000000001E-4</v>
+      </c>
+      <c r="U154" s="11"/>
+      <c r="V154" s="15"/>
+      <c r="W154" s="14"/>
+    </row>
+    <row r="155" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="L155" s="18"/>
+      <c r="M155" s="19"/>
+      <c r="N155" s="19"/>
+      <c r="O155" s="19"/>
+      <c r="P155" s="19"/>
+      <c r="Q155" s="19"/>
+      <c r="R155" s="19"/>
+      <c r="S155" s="19"/>
+      <c r="T155" s="19"/>
+      <c r="U155" s="19"/>
+      <c r="V155" s="19"/>
+      <c r="W155" s="21"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="8">
+  <tableParts count="10">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -3598,6 +4295,8 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Renamed CBSLine BurstIncrease eval files. Started with Prio1 BurstIncrease
</commit_message>
<xml_diff>
--- a/src/main/java/org/networkcalculus/dnc/demos/Eval_CBSLine/Eval_CBSLine_Results.xlsx
+++ b/src/main/java/org/networkcalculus/dnc/demos/Eval_CBSLine/Eval_CBSLine_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ForceXX\Documents\Studium\FAU_Informatik_Master\FS5\Masterarbeit\Network_Calculus_in_TSN\DNC\IntelliJ\src\main\java\org\networkcalculus\dnc\demos\Eval_CBSLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83D647F-EFE6-4468-9530-44933C0A399A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C245A1-97FA-45B3-9C91-8645004C97BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3648" windowWidth="46080" windowHeight="22152" activeTab="1" xr2:uid="{76093B85-C4EA-4FAC-BB07-8F5ADEBC9C5C}"/>
+    <workbookView xWindow="0" yWindow="4104" windowWidth="46080" windowHeight="22152" activeTab="1" xr2:uid="{76093B85-C4EA-4FAC-BB07-8F5ADEBC9C5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="38">
   <si>
     <t>f1</t>
   </si>
@@ -138,6 +138,9 @@
   <si>
     <t>99,84MBit/s</t>
   </si>
+  <si>
+    <t>11,264MBit/s</t>
+  </si>
 </sst>
 </file>
 
@@ -163,12 +166,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -263,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -309,15 +318,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="98">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
     </dxf>
@@ -601,13 +700,13 @@
   <autoFilter ref="M9:T16" xr:uid="{AFD0FDAD-B567-49C8-A37C-DCEECED05009}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{BE6FA1AF-957C-4302-ABCA-3CED577909FB}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{EABB3472-FB4D-420C-9C6B-D5FBAEE8D4FF}" name="S1" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{362B0664-EECB-41EA-8E6D-BC83B9D56EFC}" name="S2" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{6AAC6F6B-16ED-403D-9C2D-403BD383643D}" name="S3" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{AD2D3DC2-A063-43E3-8F4D-72B5648D83E8}" name="S4" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{1ACA20C8-E74E-4AE0-9617-8D84870DB044}" name="S5" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{5FFF2E6B-00A8-47E0-8FF6-2C25AA61CD2E}" name="S6" dataDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{59937D66-C814-42EC-A281-7F9615B9AC54}" name="Total" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{EABB3472-FB4D-420C-9C6B-D5FBAEE8D4FF}" name="S1" dataDxfId="97"/>
+    <tableColumn id="3" xr3:uid="{362B0664-EECB-41EA-8E6D-BC83B9D56EFC}" name="S2" dataDxfId="96"/>
+    <tableColumn id="4" xr3:uid="{6AAC6F6B-16ED-403D-9C2D-403BD383643D}" name="S3" dataDxfId="95"/>
+    <tableColumn id="5" xr3:uid="{AD2D3DC2-A063-43E3-8F4D-72B5648D83E8}" name="S4" dataDxfId="94"/>
+    <tableColumn id="6" xr3:uid="{1ACA20C8-E74E-4AE0-9617-8D84870DB044}" name="S5" dataDxfId="93"/>
+    <tableColumn id="7" xr3:uid="{5FFF2E6B-00A8-47E0-8FF6-2C25AA61CD2E}" name="S6" dataDxfId="92"/>
+    <tableColumn id="8" xr3:uid="{59937D66-C814-42EC-A281-7F9615B9AC54}" name="Total" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -618,13 +717,81 @@
   <autoFilter ref="M147:T154" xr:uid="{2891661D-836E-47DB-BD40-F3A27A090E4F}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5ED748F3-0EF7-490E-9255-D93E2E8A38B3}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{A96E6DCE-0CD4-444C-AC15-B039A4AD73D3}" name="S1" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{A38F3CDE-3B3B-46A2-8F23-68228377ED85}" name="S2" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{8B8B1AD0-037F-4F96-A7E6-AD0731A1A674}" name="S3" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{C2CC595E-C7DA-4A76-917C-24B06D46A036}" name="S4" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{68190FF9-32AD-4425-9D62-C708869AA72B}" name="S5" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{FA329009-A789-402C-A1BE-8BA2289036EA}" name="S6" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{F099B37D-2BC9-4533-80BD-70060862C629}" name="Total" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{A96E6DCE-0CD4-444C-AC15-B039A4AD73D3}" name="S1" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{A38F3CDE-3B3B-46A2-8F23-68228377ED85}" name="S2" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{8B8B1AD0-037F-4F96-A7E6-AD0731A1A674}" name="S3" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{C2CC595E-C7DA-4A76-917C-24B06D46A036}" name="S4" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{68190FF9-32AD-4425-9D62-C708869AA72B}" name="S5" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{FA329009-A789-402C-A1BE-8BA2289036EA}" name="S6" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{F099B37D-2BC9-4533-80BD-70060862C629}" name="Total" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F0458A1D-68C6-46EE-B8B9-425E706558EE}" name="Tabelle1412" displayName="Tabelle1412" ref="AA9:AH16" totalsRowShown="0">
+  <autoFilter ref="AA9:AH16" xr:uid="{20E3359C-A163-4D07-9B73-3FE6F5470B48}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{9D844AAF-0CDD-4431-955C-97AB5934E28C}" name="Analysis"/>
+    <tableColumn id="2" xr3:uid="{C6418D28-1657-4D0C-9B1B-EFDBC441468D}" name="S1" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{5AD084BF-33BD-4934-ABFB-0D84D5716194}" name="S2" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{53F5A0F2-3C27-49EF-B38F-8AB6AFFF4585}" name="S3" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{AEFCE6A1-82A7-4762-8A87-8D7EE290BEF8}" name="S4" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{C005E345-92BC-4E8E-9ACC-1B22BB62D299}" name="S5" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{1CCACC3C-ED33-4844-B76F-F79AE1FC676C}" name="S6" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{5ED8CE44-AA0C-409B-812F-F763BC573AE3}" name="Total" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{35CD6D15-06F8-4A52-BE3F-977C7AF22E28}" name="Tabelle13513" displayName="Tabelle13513" ref="AA23:AH30" totalsRowShown="0">
+  <autoFilter ref="AA23:AH30" xr:uid="{6B2C2460-94FC-4FB2-B838-01558F80A0D9}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{42188820-7181-4146-8D9B-483A6841AD2B}" name="Analysis"/>
+    <tableColumn id="2" xr3:uid="{F875B116-BDC1-4F83-909D-624F36B983BA}" name="S1" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{683F8336-33FB-490C-927E-9EF0BB58C272}" name="S2" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{9B94A0E2-3731-4ECB-93CE-EA29BF8F0FB8}" name="S3" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{43398B5B-74D8-401A-A3DB-BBE6A00516D1}" name="S4" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{28F6192D-A9EF-4A04-987C-F9B382230D36}" name="S5" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{57B2B5DA-BD8D-44B0-A99C-DDC5309B66C8}" name="S6" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{EE9281C4-C299-4F06-9DE0-BAC560DC340D}" name="Total" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{71676B0B-6A14-4E9C-8EE0-D5A9083FAAE3}" name="Tabelle141214" displayName="Tabelle141214" ref="AA40:AH47" totalsRowShown="0">
+  <autoFilter ref="AA40:AH47" xr:uid="{9014955E-1965-4C9A-A9DC-52D322018E9C}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{85E8EEDB-E008-4D1E-84BA-7DAFD9B3B91A}" name="Analysis"/>
+    <tableColumn id="2" xr3:uid="{9BAD68DC-D763-4EE6-8E7F-CF3BCBB288AB}" name="S1" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{F326866F-0A2F-4DAE-B81A-22A042D880AB}" name="S2" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{C91B65B3-A7A1-443E-8824-F147FE1A78D3}" name="S3" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{75D3802F-681F-4C3E-A022-2A048AF821C2}" name="S4" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{EBB82DA4-8866-4F55-9021-87127839AD21}" name="S5" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{72E3FD25-D43A-4384-9CC5-2793827655E1}" name="S6" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{340E3E17-7D6E-477A-BCA8-6436048088BC}" name="Total" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{8360EEB6-154D-40AD-A1AA-9E6933F0D1C5}" name="Tabelle1351315" displayName="Tabelle1351315" ref="AA54:AH61" totalsRowShown="0">
+  <autoFilter ref="AA54:AH61" xr:uid="{86B4AE62-98EF-4BDD-A78A-F87936C846E5}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{FF1A5694-D41B-4A7A-AA69-CBB5EE0C4B7B}" name="Analysis"/>
+    <tableColumn id="2" xr3:uid="{0C4C9F88-B7DD-4351-8C71-782E9D04C6F2}" name="S1" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{D7790C6F-74E4-4EBC-B244-F62780858E7C}" name="S2" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{32DA1EDD-693D-4ABB-A925-5FFE72CED6F5}" name="S3" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{5C9EA794-90CA-4009-980D-8CB10E63E5B4}" name="S4" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{2547B789-108B-4EB1-902A-4248C1F2E3AC}" name="S5" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{A6B77A2A-9DAA-492F-9584-428DCF062F04}" name="S6" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{CADDCCE0-1DD5-4109-9FA0-A0D19ECD12A9}" name="Total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -635,13 +802,13 @@
   <autoFilter ref="M23:T30" xr:uid="{9F3FFC4E-8857-417C-879B-7E46756E6ACB}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{6C7A2137-FE16-4D18-B3E5-47340E52F2D5}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{EDDA7831-D99A-413F-AA04-C00A206D6D34}" name="S1" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{3CB5E796-20A3-4C92-9FC5-590D66DC5593}" name="S2" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{3D106F77-8448-4063-87F7-7B7BE008B2F2}" name="S3" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{A891D787-2819-425A-9CE0-E8145AC0C05B}" name="S4" dataDxfId="59"/>
-    <tableColumn id="6" xr3:uid="{C6263B6C-6BFC-46DD-94D3-5EDB5A4EAF2F}" name="S5" dataDxfId="58"/>
-    <tableColumn id="7" xr3:uid="{AAC57713-C8ED-436C-B744-473CD5CFAB13}" name="S6" dataDxfId="57"/>
-    <tableColumn id="8" xr3:uid="{31F74DD7-5067-4854-B832-9EFA7B4543EA}" name="Total" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{EDDA7831-D99A-413F-AA04-C00A206D6D34}" name="S1" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{3CB5E796-20A3-4C92-9FC5-590D66DC5593}" name="S2" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{3D106F77-8448-4063-87F7-7B7BE008B2F2}" name="S3" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{A891D787-2819-425A-9CE0-E8145AC0C05B}" name="S4" dataDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{C6263B6C-6BFC-46DD-94D3-5EDB5A4EAF2F}" name="S5" dataDxfId="86"/>
+    <tableColumn id="7" xr3:uid="{AAC57713-C8ED-436C-B744-473CD5CFAB13}" name="S6" dataDxfId="85"/>
+    <tableColumn id="8" xr3:uid="{31F74DD7-5067-4854-B832-9EFA7B4543EA}" name="Total" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -652,13 +819,13 @@
   <autoFilter ref="M40:T47" xr:uid="{E16230B5-F45F-4647-925B-5EE18F895F9C}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9D1375EE-0D83-4727-B0F9-FE752E8A0CBC}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{C37D03EB-F7B2-4349-B2CC-726DB4010C90}" name="S1" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{7037993D-3D73-4283-A3B4-93C5B4E6E202}" name="S2" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{7ADA14D4-6575-4C8D-A7EA-C47F389375CE}" name="S3" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{5429F400-2F0F-4356-AC4A-9C65390A88EF}" name="S4" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{65870CF8-359E-4FAC-947D-39633692A667}" name="S5" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{59753DB4-DBE6-466A-BCC2-D1C2D56D1A27}" name="S6" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{51BDBB4F-8359-4885-B4D7-DF406809ECB7}" name="Total" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{C37D03EB-F7B2-4349-B2CC-726DB4010C90}" name="S1" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{7037993D-3D73-4283-A3B4-93C5B4E6E202}" name="S2" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{7ADA14D4-6575-4C8D-A7EA-C47F389375CE}" name="S3" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{5429F400-2F0F-4356-AC4A-9C65390A88EF}" name="S4" dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{65870CF8-359E-4FAC-947D-39633692A667}" name="S5" dataDxfId="79"/>
+    <tableColumn id="7" xr3:uid="{59753DB4-DBE6-466A-BCC2-D1C2D56D1A27}" name="S6" dataDxfId="78"/>
+    <tableColumn id="8" xr3:uid="{51BDBB4F-8359-4885-B4D7-DF406809ECB7}" name="Total" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -669,13 +836,13 @@
   <autoFilter ref="M54:T61" xr:uid="{B5EBC119-6892-4EFB-AB7E-F78E33D432A9}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0BB4E427-3492-4DCF-9D08-38551180E6EE}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{625D768D-2EA2-4E64-B741-35AF2819C1F7}" name="S1" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{2FA180EB-2936-481F-B1D1-4C1DA624FA57}" name="S2" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{7EDAFDAC-585A-4749-ABD8-DEBBA52F7B86}" name="S3" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{3E05A679-5166-455F-9DE8-C76697485C01}" name="S4" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{9611ADE2-11EE-403F-8E25-5BF3FD83A7EE}" name="S5" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{4B5CC043-D947-410A-8D8E-B4B1EDA50E93}" name="S6" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{90BF4DC0-8F16-4F8E-AD7A-04145C27A52D}" name="Total" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{625D768D-2EA2-4E64-B741-35AF2819C1F7}" name="S1" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{2FA180EB-2936-481F-B1D1-4C1DA624FA57}" name="S2" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{7EDAFDAC-585A-4749-ABD8-DEBBA52F7B86}" name="S3" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{3E05A679-5166-455F-9DE8-C76697485C01}" name="S4" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{9611ADE2-11EE-403F-8E25-5BF3FD83A7EE}" name="S5" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{4B5CC043-D947-410A-8D8E-B4B1EDA50E93}" name="S6" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{90BF4DC0-8F16-4F8E-AD7A-04145C27A52D}" name="Total" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -686,13 +853,13 @@
   <autoFilter ref="M71:T78" xr:uid="{51782671-9EEB-46B0-812D-DE4D14A213EE}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{AD5E4FB3-F32D-4B93-86CA-C7ECF985973B}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{32771DFC-FFFB-479C-8088-AA245ED9B201}" name="S1" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{850259B7-F6FC-40B4-94B0-436FE4A42169}" name="S2" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{D83AC1AB-1A0A-4527-925F-218D72D2227A}" name="S3" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{9AE7B8F5-E983-41B9-B1F4-4FC70710981E}" name="S4" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{BF918F35-6CDD-4DEE-956C-2A3434C345D0}" name="S5" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{8BF14E06-E1BE-45C5-B2AF-D712C65491A2}" name="S6" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{386EE86E-EBB8-4A4D-B17D-421040C58630}" name="Total" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{32771DFC-FFFB-479C-8088-AA245ED9B201}" name="S1" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{850259B7-F6FC-40B4-94B0-436FE4A42169}" name="S2" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{D83AC1AB-1A0A-4527-925F-218D72D2227A}" name="S3" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{9AE7B8F5-E983-41B9-B1F4-4FC70710981E}" name="S4" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{BF918F35-6CDD-4DEE-956C-2A3434C345D0}" name="S5" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{8BF14E06-E1BE-45C5-B2AF-D712C65491A2}" name="S6" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{386EE86E-EBB8-4A4D-B17D-421040C58630}" name="Total" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -703,13 +870,13 @@
   <autoFilter ref="M85:T92" xr:uid="{B8C55D2C-921B-49DD-AC76-772D4A43E64D}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{1B1BABD6-FD5C-41BB-948A-6FC0BCC11D24}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{DB6F9D20-C97E-480C-99B2-E87E4A9E1E0E}" name="S1" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{6D579111-6BD1-4C25-A59D-5752C6D1027B}" name="S2" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{971D35F8-9047-4D4E-B3A8-1050E4CBB9F7}" name="S3" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{12EA7A8D-ED74-4686-A548-2A70B019DDD4}" name="S4" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{1FE3C278-2C61-4E80-AD86-3FA5279E30B5}" name="S5" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{EE077AF3-1AB4-421C-B5DC-9511794D8F8E}" name="S6" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{4D81D46E-0FA9-4BFC-8316-8FE6191F7B12}" name="Total" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{DB6F9D20-C97E-480C-99B2-E87E4A9E1E0E}" name="S1" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{6D579111-6BD1-4C25-A59D-5752C6D1027B}" name="S2" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{971D35F8-9047-4D4E-B3A8-1050E4CBB9F7}" name="S3" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{12EA7A8D-ED74-4686-A548-2A70B019DDD4}" name="S4" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{1FE3C278-2C61-4E80-AD86-3FA5279E30B5}" name="S5" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{EE077AF3-1AB4-421C-B5DC-9511794D8F8E}" name="S6" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{4D81D46E-0FA9-4BFC-8316-8FE6191F7B12}" name="Total" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -720,13 +887,13 @@
   <autoFilter ref="M102:T109" xr:uid="{3B58D87F-510B-43F0-BC7D-8EF14E94029E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E6C46FA4-813C-4003-A6A1-34967D676206}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{C1B5C27C-40D8-4CE6-8300-D32B61DBD03E}" name="S1" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{822EBEC2-E9F3-433C-9D06-01D83E51B4EC}" name="S2" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{7E24F410-F931-4EB2-B8F2-71F614752416}" name="S3" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{6F4DDE75-12D5-4E09-BD4C-B84DBE3A1613}" name="S4" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{D1A7BB02-6526-44E4-BAC4-F951ACEB49E0}" name="S5" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{CA43AF65-8F45-41AF-809C-76D07CBDCA7B}" name="S6" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{AA305A43-F356-44F9-B1BE-8A8539A588B2}" name="Total" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{C1B5C27C-40D8-4CE6-8300-D32B61DBD03E}" name="S1" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{822EBEC2-E9F3-433C-9D06-01D83E51B4EC}" name="S2" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{7E24F410-F931-4EB2-B8F2-71F614752416}" name="S3" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{6F4DDE75-12D5-4E09-BD4C-B84DBE3A1613}" name="S4" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{D1A7BB02-6526-44E4-BAC4-F951ACEB49E0}" name="S5" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{CA43AF65-8F45-41AF-809C-76D07CBDCA7B}" name="S6" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{AA305A43-F356-44F9-B1BE-8A8539A588B2}" name="Total" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -737,13 +904,13 @@
   <autoFilter ref="M116:T123" xr:uid="{BBD41544-5CF6-451E-B19F-AA4B349E0FF5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F68E10CC-FD59-48C5-91A8-4F747980D2B8}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{091DCD40-AFF4-4A35-A51B-5CE995B27C5B}" name="S1" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{32F634D5-1211-4A7C-8411-0DC8BF7C0116}" name="S2" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{BE2DA717-3CEA-4B45-9D01-B2AF2CFBA155}" name="S3" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{820A1FC2-AB1F-424D-8760-928CAC5CEC89}" name="S4" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{7CDBF264-CA71-4555-AD13-B4F0B0EFF5CB}" name="S5" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{FD7873DE-5A47-42D5-BE83-3AC049767285}" name="S6" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{514BF621-1FB2-46A5-A883-5F156AE64F89}" name="Total" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{091DCD40-AFF4-4A35-A51B-5CE995B27C5B}" name="S1" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{32F634D5-1211-4A7C-8411-0DC8BF7C0116}" name="S2" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{BE2DA717-3CEA-4B45-9D01-B2AF2CFBA155}" name="S3" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{820A1FC2-AB1F-424D-8760-928CAC5CEC89}" name="S4" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{7CDBF264-CA71-4555-AD13-B4F0B0EFF5CB}" name="S5" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{FD7873DE-5A47-42D5-BE83-3AC049767285}" name="S6" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{514BF621-1FB2-46A5-A883-5F156AE64F89}" name="Total" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -754,13 +921,13 @@
   <autoFilter ref="M133:T140" xr:uid="{FB41092D-F5FF-4971-9DDD-C9E03FD01631}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{6647CD1D-0845-4A23-9836-FBC960574DA7}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{5BD82A11-F2EA-4903-B53D-DD982E06A315}" name="S1" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{424AE262-E0C8-44A2-B28D-3F028CA6231F}" name="S2" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{D576FA30-995E-46FE-8DB0-5798DAE28331}" name="S3" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{B630E084-8616-40E7-A93B-DA34C763EADC}" name="S4" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{04C38EE3-C04A-4AE3-B01D-D5CC7EEF4DE2}" name="S5" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{68C4544A-4832-4B5A-9EE3-E132B259AACC}" name="S6" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{71294977-C366-4F0A-B7E5-972975477A7D}" name="Total" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{5BD82A11-F2EA-4903-B53D-DD982E06A315}" name="S1" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{424AE262-E0C8-44A2-B28D-3F028CA6231F}" name="S2" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{D576FA30-995E-46FE-8DB0-5798DAE28331}" name="S3" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{B630E084-8616-40E7-A93B-DA34C763EADC}" name="S4" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{04C38EE3-C04A-4AE3-B01D-D5CC7EEF4DE2}" name="S5" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{68C4544A-4832-4B5A-9EE3-E132B259AACC}" name="S6" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{71294977-C366-4F0A-B7E5-972975477A7D}" name="Total" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1089,17 +1256,17 @@
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
       <c r="K3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="4">
         <f>B4*C4*8</f>
-        <v>12480</v>
+        <v>2816</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
@@ -1107,10 +1274,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>780</v>
+        <v>176</v>
       </c>
       <c r="D4" s="1">
-        <v>1.25E-4</v>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="E4" s="3">
         <v>100000000</v>
@@ -1123,7 +1290,7 @@
       </c>
       <c r="L4" s="5">
         <f>L3/D4</f>
-        <v>99840000</v>
+        <v>11264000</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
@@ -1132,7 +1299,7 @@
       </c>
       <c r="L5" s="4">
         <f>L3*(1-(L4/E4))</f>
-        <v>19.968000000000572</v>
+        <v>2498.8057600000002</v>
       </c>
     </row>
   </sheetData>
@@ -1146,22 +1313,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB25049-F719-48DC-B24C-CE81CB877780}">
-  <dimension ref="B3:W155"/>
+  <dimension ref="B3:AK155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="S10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AL26" sqref="AL26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="20" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="20" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="34" width="23.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="12:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L3" s="6"/>
       <c r="M3" s="7" t="s">
         <v>26</v>
@@ -1188,8 +1358,34 @@
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
       <c r="W3" s="9"/>
-    </row>
-    <row r="4" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
+      <c r="AK3" s="9"/>
+    </row>
+    <row r="4" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L4" s="10"/>
       <c r="M4" s="11" t="s">
         <v>27</v>
@@ -1216,8 +1412,34 @@
       <c r="U4" s="11"/>
       <c r="V4" s="11"/>
       <c r="W4" s="14"/>
-    </row>
-    <row r="5" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB4" s="12">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="25">
+        <v>88</v>
+      </c>
+      <c r="AD4" s="12">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="AE4" s="13">
+        <v>100000000</v>
+      </c>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="26">
+        <v>1328.70144</v>
+      </c>
+      <c r="AH4" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI4" s="11"/>
+      <c r="AJ4" s="11"/>
+      <c r="AK4" s="14"/>
+    </row>
+    <row r="5" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L5" s="10"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
@@ -1230,8 +1452,20 @@
       <c r="U5" s="11"/>
       <c r="V5" s="11"/>
       <c r="W5" s="14"/>
-    </row>
-    <row r="6" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="11"/>
+      <c r="AI5" s="11"/>
+      <c r="AJ5" s="11"/>
+      <c r="AK5" s="14"/>
+    </row>
+    <row r="6" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L6" s="10"/>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
@@ -1244,8 +1478,20 @@
       <c r="U6" s="11"/>
       <c r="V6" s="11"/>
       <c r="W6" s="14"/>
-    </row>
-    <row r="7" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="14"/>
+    </row>
+    <row r="7" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L7" s="10"/>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
@@ -1258,8 +1504,20 @@
       <c r="U7" s="11"/>
       <c r="V7" s="11"/>
       <c r="W7" s="14"/>
-    </row>
-    <row r="8" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="11"/>
+      <c r="AH7" s="11"/>
+      <c r="AI7" s="11"/>
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="14"/>
+    </row>
+    <row r="8" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L8" s="10"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
@@ -1272,8 +1530,20 @@
       <c r="U8" s="11"/>
       <c r="V8" s="11"/>
       <c r="W8" s="14"/>
-    </row>
-    <row r="9" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="11"/>
+      <c r="AJ8" s="11"/>
+      <c r="AK8" s="14"/>
+    </row>
+    <row r="9" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L9" s="10"/>
       <c r="M9" s="11" t="s">
         <v>15</v>
@@ -1302,8 +1572,36 @@
       <c r="U9" s="11"/>
       <c r="V9" s="11"/>
       <c r="W9" s="14"/>
-    </row>
-    <row r="10" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI9" s="11"/>
+      <c r="AJ9" s="11"/>
+      <c r="AK9" s="14"/>
+    </row>
+    <row r="10" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L10" s="10"/>
       <c r="M10" s="11" t="s">
         <v>16</v>
@@ -1335,8 +1633,36 @@
         <v>1.4302043647999999E-3</v>
       </c>
       <c r="W10" s="14"/>
-    </row>
-    <row r="11" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB10" s="15">
+        <v>2.051340288E-4</v>
+      </c>
+      <c r="AC10" s="15">
+        <v>2.2524702719999999E-4</v>
+      </c>
+      <c r="AD10" s="15">
+        <v>2.4536002560000001E-4</v>
+      </c>
+      <c r="AE10" s="15">
+        <v>2.6547302400000002E-4</v>
+      </c>
+      <c r="AF10" s="15">
+        <v>2.8558602239999999E-4</v>
+      </c>
+      <c r="AG10" s="15">
+        <v>2.5049902080000002E-4</v>
+      </c>
+      <c r="AH10" s="15">
+        <v>1.4772991487999999E-3</v>
+      </c>
+      <c r="AI10" s="11"/>
+      <c r="AJ10" s="15"/>
+      <c r="AK10" s="14"/>
+    </row>
+    <row r="11" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L11" s="10"/>
       <c r="M11" s="11" t="s">
         <v>17</v>
@@ -1368,8 +1694,36 @@
         <v>1.06544E-3</v>
       </c>
       <c r="W11" s="14"/>
-    </row>
-    <row r="12" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB11" s="15">
+        <v>1.9264E-4</v>
+      </c>
+      <c r="AC11" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AD11" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AE11" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AF11" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AG11" s="15">
+        <v>1.5152000000000001E-4</v>
+      </c>
+      <c r="AH11" s="15">
+        <v>1.1710399999999999E-3</v>
+      </c>
+      <c r="AI11" s="11"/>
+      <c r="AJ11" s="15"/>
+      <c r="AK11" s="14"/>
+    </row>
+    <row r="12" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L12" s="16" t="s">
         <v>24</v>
       </c>
@@ -1403,8 +1757,38 @@
         <v>1.4302043647999999E-3</v>
       </c>
       <c r="W12" s="14"/>
-    </row>
-    <row r="13" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB12" s="15">
+        <v>2.051340288E-4</v>
+      </c>
+      <c r="AC12" s="15">
+        <v>2.2524702719999999E-4</v>
+      </c>
+      <c r="AD12" s="15">
+        <v>2.4536002560000001E-4</v>
+      </c>
+      <c r="AE12" s="15">
+        <v>2.6547302400000002E-4</v>
+      </c>
+      <c r="AF12" s="15">
+        <v>2.8558602239999999E-4</v>
+      </c>
+      <c r="AG12" s="15">
+        <v>2.5049902080000002E-4</v>
+      </c>
+      <c r="AH12" s="15">
+        <v>1.4772991487999999E-3</v>
+      </c>
+      <c r="AI12" s="11"/>
+      <c r="AJ12" s="15"/>
+      <c r="AK12" s="14"/>
+    </row>
+    <row r="13" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L13" s="10"/>
       <c r="M13" s="11" t="s">
         <v>19</v>
@@ -1436,8 +1820,36 @@
         <v>1.1136E-3</v>
       </c>
       <c r="W13" s="14"/>
-    </row>
-    <row r="14" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB13" s="15">
+        <v>1.9264E-4</v>
+      </c>
+      <c r="AC13" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AD13" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AE13" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AF13" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AG13" s="15">
+        <v>1.5152000000000001E-4</v>
+      </c>
+      <c r="AH13" s="15">
+        <v>1.1710399999999999E-3</v>
+      </c>
+      <c r="AI13" s="11"/>
+      <c r="AJ13" s="15"/>
+      <c r="AK13" s="14"/>
+    </row>
+    <row r="14" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L14" s="10"/>
       <c r="M14" s="11" t="s">
         <v>20</v>
@@ -1457,8 +1869,24 @@
         <v>0</v>
       </c>
       <c r="W14" s="14"/>
-    </row>
-    <row r="15" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
+      <c r="AF14" s="15"/>
+      <c r="AG14" s="15"/>
+      <c r="AH14" s="15">
+        <v>1.0427340288E-3</v>
+      </c>
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="15"/>
+      <c r="AK14" s="14"/>
+    </row>
+    <row r="15" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L15" s="10"/>
       <c r="M15" s="11" t="s">
         <v>21</v>
@@ -1478,8 +1906,24 @@
         <v>0</v>
       </c>
       <c r="W15" s="14"/>
-    </row>
-    <row r="16" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="15"/>
+      <c r="AF15" s="15"/>
+      <c r="AG15" s="15"/>
+      <c r="AH15" s="15">
+        <v>1.0427340288E-3</v>
+      </c>
+      <c r="AI15" s="11"/>
+      <c r="AJ15" s="15"/>
+      <c r="AK15" s="14"/>
+    </row>
+    <row r="16" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L16" s="10"/>
       <c r="M16" s="11" t="s">
         <v>22</v>
@@ -1499,8 +1943,24 @@
         <v>0</v>
       </c>
       <c r="W16" s="14"/>
-    </row>
-    <row r="17" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
+      <c r="AD16" s="15"/>
+      <c r="AE16" s="15"/>
+      <c r="AF16" s="15"/>
+      <c r="AG16" s="15"/>
+      <c r="AH16" s="15">
+        <v>1.0427340288E-3</v>
+      </c>
+      <c r="AI16" s="11"/>
+      <c r="AJ16" s="15"/>
+      <c r="AK16" s="14"/>
+    </row>
+    <row r="17" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L17" s="10"/>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
@@ -1513,8 +1973,20 @@
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
       <c r="W17" s="14"/>
-    </row>
-    <row r="18" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="11"/>
+      <c r="AE17" s="11"/>
+      <c r="AF17" s="11"/>
+      <c r="AG17" s="11"/>
+      <c r="AH17" s="11"/>
+      <c r="AI17" s="11"/>
+      <c r="AJ17" s="11"/>
+      <c r="AK17" s="14"/>
+    </row>
+    <row r="18" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L18" s="10"/>
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
@@ -1527,8 +1999,20 @@
       <c r="U18" s="11"/>
       <c r="V18" s="11"/>
       <c r="W18" s="14"/>
-    </row>
-    <row r="19" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="11"/>
+      <c r="AG18" s="11"/>
+      <c r="AH18" s="11"/>
+      <c r="AI18" s="11"/>
+      <c r="AJ18" s="11"/>
+      <c r="AK18" s="14"/>
+    </row>
+    <row r="19" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L19" s="10"/>
       <c r="M19" s="11" t="s">
         <v>25</v>
@@ -1555,8 +2039,34 @@
       <c r="U19" s="11"/>
       <c r="V19" s="11"/>
       <c r="W19" s="14"/>
-    </row>
-    <row r="20" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB19" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC19" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD19" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE19" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF19" s="11"/>
+      <c r="AG19" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH19" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI19" s="11"/>
+      <c r="AJ19" s="11"/>
+      <c r="AK19" s="14"/>
+    </row>
+    <row r="20" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L20" s="10"/>
       <c r="M20" s="11" t="s">
         <v>28</v>
@@ -1564,7 +2074,7 @@
       <c r="N20" s="12">
         <v>2</v>
       </c>
-      <c r="O20" s="12">
+      <c r="O20" s="25">
         <v>88</v>
       </c>
       <c r="P20" s="12">
@@ -1574,17 +2084,43 @@
         <v>100000000</v>
       </c>
       <c r="R20" s="11"/>
-      <c r="S20" s="1">
+      <c r="S20" s="26">
         <v>1249.4028800000001</v>
       </c>
-      <c r="T20" s="12" t="s">
+      <c r="T20" s="25" t="s">
         <v>31</v>
       </c>
       <c r="U20" s="11"/>
       <c r="V20" s="11"/>
       <c r="W20" s="14"/>
-    </row>
-    <row r="21" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB20" s="12">
+        <v>2</v>
+      </c>
+      <c r="AC20" s="12">
+        <v>176</v>
+      </c>
+      <c r="AD20" s="12">
+        <v>1.25E-4</v>
+      </c>
+      <c r="AE20" s="13">
+        <v>100000000</v>
+      </c>
+      <c r="AF20" s="11"/>
+      <c r="AG20" s="22">
+        <v>2181.6115199999999</v>
+      </c>
+      <c r="AH20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI20" s="11"/>
+      <c r="AJ20" s="11"/>
+      <c r="AK20" s="14"/>
+    </row>
+    <row r="21" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L21" s="10"/>
       <c r="M21" s="11"/>
       <c r="N21" s="11"/>
@@ -1597,8 +2133,20 @@
       <c r="U21" s="11"/>
       <c r="V21" s="11"/>
       <c r="W21" s="14"/>
-    </row>
-    <row r="22" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="11"/>
+      <c r="AF21" s="11"/>
+      <c r="AG21" s="11"/>
+      <c r="AH21" s="11"/>
+      <c r="AI21" s="11"/>
+      <c r="AJ21" s="11"/>
+      <c r="AK21" s="14"/>
+    </row>
+    <row r="22" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L22" s="10"/>
       <c r="M22" s="11"/>
       <c r="N22" s="11"/>
@@ -1611,8 +2159,20 @@
       <c r="U22" s="11"/>
       <c r="V22" s="11"/>
       <c r="W22" s="14"/>
-    </row>
-    <row r="23" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11"/>
+      <c r="AE22" s="11"/>
+      <c r="AF22" s="11"/>
+      <c r="AG22" s="11"/>
+      <c r="AH22" s="11"/>
+      <c r="AI22" s="11"/>
+      <c r="AJ22" s="11"/>
+      <c r="AK22" s="14"/>
+    </row>
+    <row r="23" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L23" s="10"/>
       <c r="M23" s="11" t="s">
         <v>15</v>
@@ -1641,8 +2201,36 @@
       <c r="U23" s="11"/>
       <c r="V23" s="11"/>
       <c r="W23" s="14"/>
-    </row>
-    <row r="24" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB23" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD23" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH23" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI23" s="11"/>
+      <c r="AJ23" s="11"/>
+      <c r="AK23" s="14"/>
+    </row>
+    <row r="24" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L24" s="10"/>
       <c r="M24" s="11" t="s">
         <v>16</v>
@@ -1666,8 +2254,28 @@
         <v>4.0225331199999999E-4</v>
       </c>
       <c r="W24" s="14"/>
-    </row>
-    <row r="25" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z24" s="10"/>
+      <c r="AA24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB24" s="15">
+        <v>2.1062446080000001E-4</v>
+      </c>
+      <c r="AC24" s="15">
+        <v>3.2178662400000001E-4</v>
+      </c>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="15"/>
+      <c r="AF24" s="15"/>
+      <c r="AG24" s="15"/>
+      <c r="AH24" s="15">
+        <v>5.3241108480000003E-4</v>
+      </c>
+      <c r="AI24" s="11"/>
+      <c r="AJ24" s="15"/>
+      <c r="AK24" s="14"/>
+    </row>
+    <row r="25" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L25" s="10"/>
       <c r="M25" s="11" t="s">
         <v>17</v>
@@ -1691,8 +2299,28 @@
         <v>3.0304000000000003E-4</v>
       </c>
       <c r="W25" s="14"/>
-    </row>
-    <row r="26" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB25" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="AC25" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="AD25" s="15"/>
+      <c r="AE25" s="15"/>
+      <c r="AF25" s="15"/>
+      <c r="AG25" s="15"/>
+      <c r="AH25" s="15">
+        <v>3.5935999999999997E-4</v>
+      </c>
+      <c r="AI25" s="11"/>
+      <c r="AJ25" s="15"/>
+      <c r="AK25" s="14"/>
+    </row>
+    <row r="26" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L26" s="16" t="s">
         <v>0</v>
       </c>
@@ -1718,8 +2346,30 @@
         <v>4.0225331199999999E-4</v>
       </c>
       <c r="W26" s="14"/>
-    </row>
-    <row r="27" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z26" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB26" s="15">
+        <v>2.1062446080000001E-4</v>
+      </c>
+      <c r="AC26" s="15">
+        <v>3.2178662400000001E-4</v>
+      </c>
+      <c r="AD26" s="15"/>
+      <c r="AE26" s="15"/>
+      <c r="AF26" s="15"/>
+      <c r="AG26" s="15"/>
+      <c r="AH26" s="15">
+        <v>5.3241108480000003E-4</v>
+      </c>
+      <c r="AI26" s="11"/>
+      <c r="AJ26" s="15"/>
+      <c r="AK26" s="14"/>
+    </row>
+    <row r="27" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L27" s="10"/>
       <c r="M27" s="11" t="s">
         <v>19</v>
@@ -1743,8 +2393,28 @@
         <v>3.0304000000000003E-4</v>
       </c>
       <c r="W27" s="14"/>
-    </row>
-    <row r="28" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z27" s="10"/>
+      <c r="AA27" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB27" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="AC27" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="AD27" s="15"/>
+      <c r="AE27" s="15"/>
+      <c r="AF27" s="15"/>
+      <c r="AG27" s="15"/>
+      <c r="AH27" s="15">
+        <v>3.5935999999999997E-4</v>
+      </c>
+      <c r="AI27" s="11"/>
+      <c r="AJ27" s="15"/>
+      <c r="AK27" s="14"/>
+    </row>
+    <row r="28" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L28" s="10"/>
       <c r="M28" s="11" t="s">
         <v>20</v>
@@ -1764,8 +2434,24 @@
         <v>0</v>
       </c>
       <c r="W28" s="14"/>
-    </row>
-    <row r="29" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z28" s="10"/>
+      <c r="AA28" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB28" s="15"/>
+      <c r="AC28" s="15"/>
+      <c r="AD28" s="15"/>
+      <c r="AE28" s="15"/>
+      <c r="AF28" s="15"/>
+      <c r="AG28" s="15"/>
+      <c r="AH28" s="15">
+        <v>3.339844608E-4</v>
+      </c>
+      <c r="AI28" s="11"/>
+      <c r="AJ28" s="15"/>
+      <c r="AK28" s="14"/>
+    </row>
+    <row r="29" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L29" s="10"/>
       <c r="M29" s="11" t="s">
         <v>21</v>
@@ -1785,8 +2471,24 @@
         <v>0</v>
       </c>
       <c r="W29" s="14"/>
-    </row>
-    <row r="30" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z29" s="10"/>
+      <c r="AA29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB29" s="15"/>
+      <c r="AC29" s="15"/>
+      <c r="AD29" s="15"/>
+      <c r="AE29" s="15"/>
+      <c r="AF29" s="15"/>
+      <c r="AG29" s="15"/>
+      <c r="AH29" s="15">
+        <v>3.339844608E-4</v>
+      </c>
+      <c r="AI29" s="11"/>
+      <c r="AJ29" s="15"/>
+      <c r="AK29" s="14"/>
+    </row>
+    <row r="30" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L30" s="10"/>
       <c r="M30" s="11" t="s">
         <v>22</v>
@@ -1806,8 +2508,24 @@
         <v>0</v>
       </c>
       <c r="W30" s="14"/>
-    </row>
-    <row r="31" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB30" s="15"/>
+      <c r="AC30" s="15"/>
+      <c r="AD30" s="15"/>
+      <c r="AE30" s="15"/>
+      <c r="AF30" s="15"/>
+      <c r="AG30" s="15"/>
+      <c r="AH30" s="15">
+        <v>3.339844608E-4</v>
+      </c>
+      <c r="AI30" s="11"/>
+      <c r="AJ30" s="15"/>
+      <c r="AK30" s="14"/>
+    </row>
+    <row r="31" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L31" s="18"/>
       <c r="M31" s="19"/>
       <c r="N31" s="20"/>
@@ -1820,14 +2538,26 @@
       <c r="U31" s="19"/>
       <c r="V31" s="19"/>
       <c r="W31" s="21"/>
-    </row>
-    <row r="32" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z31" s="18"/>
+      <c r="AA31" s="19"/>
+      <c r="AB31" s="19"/>
+      <c r="AC31" s="19"/>
+      <c r="AD31" s="19"/>
+      <c r="AE31" s="19"/>
+      <c r="AF31" s="19"/>
+      <c r="AG31" s="19"/>
+      <c r="AH31" s="19"/>
+      <c r="AI31" s="19"/>
+      <c r="AJ31" s="19"/>
+      <c r="AK31" s="21"/>
+    </row>
+    <row r="32" spans="12:37" x14ac:dyDescent="0.3">
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="3"/>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L34" s="6"/>
       <c r="M34" s="7" t="s">
         <v>26</v>
@@ -1854,8 +2584,34 @@
       <c r="U34" s="7"/>
       <c r="V34" s="7"/>
       <c r="W34" s="9"/>
-    </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z34" s="6"/>
+      <c r="AA34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB34" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD34" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF34" s="7"/>
+      <c r="AG34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH34" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI34" s="7"/>
+      <c r="AJ34" s="7"/>
+      <c r="AK34" s="9"/>
+    </row>
+    <row r="35" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L35" s="10"/>
       <c r="M35" s="11" t="s">
         <v>27</v>
@@ -1882,8 +2638,34 @@
       <c r="U35" s="11"/>
       <c r="V35" s="11"/>
       <c r="W35" s="14"/>
-    </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z35" s="10"/>
+      <c r="AA35" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB35" s="12">
+        <v>2</v>
+      </c>
+      <c r="AC35" s="25">
+        <v>176</v>
+      </c>
+      <c r="AD35" s="12">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="AE35" s="13">
+        <v>100000000</v>
+      </c>
+      <c r="AF35" s="11"/>
+      <c r="AG35" s="26">
+        <v>2498.8057600000002</v>
+      </c>
+      <c r="AH35" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI35" s="11"/>
+      <c r="AJ35" s="11"/>
+      <c r="AK35" s="14"/>
+    </row>
+    <row r="36" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1900,8 +2682,20 @@
       <c r="U36" s="11"/>
       <c r="V36" s="11"/>
       <c r="W36" s="14"/>
-    </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z36" s="10"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11"/>
+      <c r="AC36" s="11"/>
+      <c r="AD36" s="11"/>
+      <c r="AE36" s="11"/>
+      <c r="AF36" s="11"/>
+      <c r="AG36" s="11"/>
+      <c r="AH36" s="11"/>
+      <c r="AI36" s="11"/>
+      <c r="AJ36" s="11"/>
+      <c r="AK36" s="14"/>
+    </row>
+    <row r="37" spans="2:37" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1918,8 +2712,20 @@
       <c r="U37" s="11"/>
       <c r="V37" s="11"/>
       <c r="W37" s="14"/>
-    </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z37" s="10"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="11"/>
+      <c r="AC37" s="11"/>
+      <c r="AD37" s="11"/>
+      <c r="AE37" s="11"/>
+      <c r="AF37" s="11"/>
+      <c r="AG37" s="11"/>
+      <c r="AH37" s="11"/>
+      <c r="AI37" s="11"/>
+      <c r="AJ37" s="11"/>
+      <c r="AK37" s="14"/>
+    </row>
+    <row r="38" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L38" s="10"/>
       <c r="M38" s="11"/>
       <c r="N38" s="11"/>
@@ -1932,8 +2738,20 @@
       <c r="U38" s="11"/>
       <c r="V38" s="11"/>
       <c r="W38" s="14"/>
-    </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z38" s="10"/>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="11"/>
+      <c r="AC38" s="11"/>
+      <c r="AD38" s="11"/>
+      <c r="AE38" s="11"/>
+      <c r="AF38" s="11"/>
+      <c r="AG38" s="11"/>
+      <c r="AH38" s="11"/>
+      <c r="AI38" s="11"/>
+      <c r="AJ38" s="11"/>
+      <c r="AK38" s="14"/>
+    </row>
+    <row r="39" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L39" s="10"/>
       <c r="M39" s="11"/>
       <c r="N39" s="11"/>
@@ -1946,8 +2764,20 @@
       <c r="U39" s="11"/>
       <c r="V39" s="11"/>
       <c r="W39" s="14"/>
-    </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z39" s="10"/>
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="11"/>
+      <c r="AC39" s="11"/>
+      <c r="AD39" s="11"/>
+      <c r="AE39" s="11"/>
+      <c r="AF39" s="11"/>
+      <c r="AG39" s="11"/>
+      <c r="AH39" s="11"/>
+      <c r="AI39" s="11"/>
+      <c r="AJ39" s="11"/>
+      <c r="AK39" s="14"/>
+    </row>
+    <row r="40" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L40" s="10"/>
       <c r="M40" s="11" t="s">
         <v>15</v>
@@ -1976,8 +2806,36 @@
       <c r="U40" s="11"/>
       <c r="V40" s="11"/>
       <c r="W40" s="14"/>
-    </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z40" s="10"/>
+      <c r="AA40" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB40" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC40" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD40" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE40" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF40" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG40" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH40" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI40" s="11"/>
+      <c r="AJ40" s="11"/>
+      <c r="AK40" s="14"/>
+    </row>
+    <row r="41" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L41" s="10"/>
       <c r="M41" s="11" t="s">
         <v>16</v>
@@ -2006,8 +2864,36 @@
       <c r="U41" s="11"/>
       <c r="V41" s="15"/>
       <c r="W41" s="14"/>
-    </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z41" s="10"/>
+      <c r="AA41" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB41" s="15">
+        <v>2.2853611520000001E-4</v>
+      </c>
+      <c r="AC41" s="15">
+        <v>2.6876211200000001E-4</v>
+      </c>
+      <c r="AD41" s="15">
+        <v>3.0898810879999999E-4</v>
+      </c>
+      <c r="AE41" s="15">
+        <v>3.4921410560000002E-4</v>
+      </c>
+      <c r="AF41" s="15">
+        <v>3.894401024E-4</v>
+      </c>
+      <c r="AG41" s="15">
+        <v>3.744660992E-4</v>
+      </c>
+      <c r="AH41" s="15">
+        <v>1.9194066432E-3</v>
+      </c>
+      <c r="AI41" s="11"/>
+      <c r="AJ41" s="15"/>
+      <c r="AK41" s="14"/>
+    </row>
+    <row r="42" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L42" s="10"/>
       <c r="M42" s="11" t="s">
         <v>17</v>
@@ -2036,8 +2922,36 @@
       <c r="U42" s="11"/>
       <c r="V42" s="15"/>
       <c r="W42" s="14"/>
-    </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z42" s="10"/>
+      <c r="AA42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB42" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AC42" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AD42" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AE42" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AF42" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AG42" s="15">
+        <v>1.5152000000000001E-4</v>
+      </c>
+      <c r="AH42" s="15">
+        <v>1.18512E-3</v>
+      </c>
+      <c r="AI42" s="11"/>
+      <c r="AJ42" s="15"/>
+      <c r="AK42" s="14"/>
+    </row>
+    <row r="43" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L43" s="16" t="s">
         <v>24</v>
       </c>
@@ -2068,8 +2982,38 @@
       <c r="U43" s="11"/>
       <c r="V43" s="15"/>
       <c r="W43" s="14"/>
-    </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z43" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA43" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB43" s="15">
+        <v>2.2853611520000001E-4</v>
+      </c>
+      <c r="AC43" s="15">
+        <v>2.6876211200000001E-4</v>
+      </c>
+      <c r="AD43" s="15">
+        <v>3.0898810879999999E-4</v>
+      </c>
+      <c r="AE43" s="15">
+        <v>3.4921410560000002E-4</v>
+      </c>
+      <c r="AF43" s="15">
+        <v>3.894401024E-4</v>
+      </c>
+      <c r="AG43" s="15">
+        <v>3.4415999999999998E-4</v>
+      </c>
+      <c r="AH43" s="15">
+        <v>1.8891005439999899E-3</v>
+      </c>
+      <c r="AI43" s="11"/>
+      <c r="AJ43" s="15"/>
+      <c r="AK43" s="14"/>
+    </row>
+    <row r="44" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L44" s="10"/>
       <c r="M44" s="11" t="s">
         <v>19</v>
@@ -2098,8 +3042,36 @@
       <c r="U44" s="11"/>
       <c r="V44" s="15"/>
       <c r="W44" s="14"/>
-    </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z44" s="10"/>
+      <c r="AA44" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB44" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AC44" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AD44" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AE44" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AF44" s="15">
+        <v>2.0672E-4</v>
+      </c>
+      <c r="AG44" s="15">
+        <v>1.5152000000000001E-4</v>
+      </c>
+      <c r="AH44" s="15">
+        <v>1.18512E-3</v>
+      </c>
+      <c r="AI44" s="11"/>
+      <c r="AJ44" s="15"/>
+      <c r="AK44" s="14"/>
+    </row>
+    <row r="45" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L45" s="10"/>
       <c r="M45" s="11" t="s">
         <v>20</v>
@@ -2116,8 +3088,24 @@
       <c r="U45" s="11"/>
       <c r="V45" s="15"/>
       <c r="W45" s="14"/>
-    </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z45" s="10"/>
+      <c r="AA45" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB45" s="15"/>
+      <c r="AC45" s="15"/>
+      <c r="AD45" s="15"/>
+      <c r="AE45" s="15"/>
+      <c r="AF45" s="15"/>
+      <c r="AG45" s="15"/>
+      <c r="AH45" s="15">
+        <v>1.0661361152E-3</v>
+      </c>
+      <c r="AI45" s="11"/>
+      <c r="AJ45" s="15"/>
+      <c r="AK45" s="14"/>
+    </row>
+    <row r="46" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L46" s="10"/>
       <c r="M46" s="11" t="s">
         <v>21</v>
@@ -2134,8 +3122,24 @@
       <c r="U46" s="11"/>
       <c r="V46" s="15"/>
       <c r="W46" s="14"/>
-    </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z46" s="10"/>
+      <c r="AA46" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB46" s="15"/>
+      <c r="AC46" s="15"/>
+      <c r="AD46" s="15"/>
+      <c r="AE46" s="15"/>
+      <c r="AF46" s="15"/>
+      <c r="AG46" s="15"/>
+      <c r="AH46" s="15">
+        <v>1.0661361152E-3</v>
+      </c>
+      <c r="AI46" s="11"/>
+      <c r="AJ46" s="15"/>
+      <c r="AK46" s="14"/>
+    </row>
+    <row r="47" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L47" s="10"/>
       <c r="M47" s="11" t="s">
         <v>22</v>
@@ -2152,8 +3156,24 @@
       <c r="U47" s="11"/>
       <c r="V47" s="15"/>
       <c r="W47" s="14"/>
-    </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="Z47" s="10"/>
+      <c r="AA47" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB47" s="15"/>
+      <c r="AC47" s="15"/>
+      <c r="AD47" s="15"/>
+      <c r="AE47" s="15"/>
+      <c r="AF47" s="15"/>
+      <c r="AG47" s="15"/>
+      <c r="AH47" s="15">
+        <v>1.0661361152E-3</v>
+      </c>
+      <c r="AI47" s="11"/>
+      <c r="AJ47" s="15"/>
+      <c r="AK47" s="14"/>
+    </row>
+    <row r="48" spans="2:37" x14ac:dyDescent="0.3">
       <c r="L48" s="10"/>
       <c r="M48" s="11"/>
       <c r="N48" s="11"/>
@@ -2166,8 +3186,20 @@
       <c r="U48" s="11"/>
       <c r="V48" s="11"/>
       <c r="W48" s="14"/>
-    </row>
-    <row r="49" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z48" s="10"/>
+      <c r="AA48" s="11"/>
+      <c r="AB48" s="11"/>
+      <c r="AC48" s="11"/>
+      <c r="AD48" s="11"/>
+      <c r="AE48" s="11"/>
+      <c r="AF48" s="11"/>
+      <c r="AG48" s="11"/>
+      <c r="AH48" s="11"/>
+      <c r="AI48" s="11"/>
+      <c r="AJ48" s="11"/>
+      <c r="AK48" s="14"/>
+    </row>
+    <row r="49" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L49" s="10"/>
       <c r="M49" s="11"/>
       <c r="N49" s="11"/>
@@ -2180,8 +3212,20 @@
       <c r="U49" s="11"/>
       <c r="V49" s="11"/>
       <c r="W49" s="14"/>
-    </row>
-    <row r="50" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z49" s="10"/>
+      <c r="AA49" s="11"/>
+      <c r="AB49" s="11"/>
+      <c r="AC49" s="11"/>
+      <c r="AD49" s="11"/>
+      <c r="AE49" s="11"/>
+      <c r="AF49" s="11"/>
+      <c r="AG49" s="11"/>
+      <c r="AH49" s="11"/>
+      <c r="AI49" s="11"/>
+      <c r="AJ49" s="11"/>
+      <c r="AK49" s="14"/>
+    </row>
+    <row r="50" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L50" s="10"/>
       <c r="M50" s="11" t="s">
         <v>25</v>
@@ -2208,8 +3252,34 @@
       <c r="U50" s="11"/>
       <c r="V50" s="11"/>
       <c r="W50" s="14"/>
-    </row>
-    <row r="51" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z50" s="10"/>
+      <c r="AA50" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB50" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC50" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD50" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE50" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF50" s="11"/>
+      <c r="AG50" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH50" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI50" s="11"/>
+      <c r="AJ50" s="11"/>
+      <c r="AK50" s="14"/>
+    </row>
+    <row r="51" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L51" s="10"/>
       <c r="M51" s="11" t="s">
         <v>28</v>
@@ -2217,7 +3287,7 @@
       <c r="N51" s="12">
         <v>2</v>
       </c>
-      <c r="O51" s="12">
+      <c r="O51" s="25">
         <v>176</v>
       </c>
       <c r="P51" s="12">
@@ -2227,17 +3297,43 @@
         <v>100000000</v>
       </c>
       <c r="R51" s="11"/>
-      <c r="S51" s="22">
+      <c r="S51" s="25">
         <v>2181.6115199999999</v>
       </c>
-      <c r="T51" s="12" t="s">
+      <c r="T51" s="25" t="s">
         <v>33</v>
       </c>
       <c r="U51" s="11"/>
       <c r="V51" s="11"/>
       <c r="W51" s="14"/>
-    </row>
-    <row r="52" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z51" s="10"/>
+      <c r="AA51" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB51" s="12">
+        <v>2</v>
+      </c>
+      <c r="AC51" s="12">
+        <v>176</v>
+      </c>
+      <c r="AD51" s="12">
+        <v>1.25E-4</v>
+      </c>
+      <c r="AE51" s="13">
+        <v>100000000</v>
+      </c>
+      <c r="AF51" s="11"/>
+      <c r="AG51" s="22">
+        <v>2181.6115199999999</v>
+      </c>
+      <c r="AH51" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI51" s="11"/>
+      <c r="AJ51" s="11"/>
+      <c r="AK51" s="14"/>
+    </row>
+    <row r="52" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L52" s="10"/>
       <c r="M52" s="11"/>
       <c r="N52" s="11"/>
@@ -2250,8 +3346,20 @@
       <c r="U52" s="11"/>
       <c r="V52" s="11"/>
       <c r="W52" s="14"/>
-    </row>
-    <row r="53" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z52" s="10"/>
+      <c r="AA52" s="11"/>
+      <c r="AB52" s="11"/>
+      <c r="AC52" s="11"/>
+      <c r="AD52" s="11"/>
+      <c r="AE52" s="11"/>
+      <c r="AF52" s="11"/>
+      <c r="AG52" s="11"/>
+      <c r="AH52" s="11"/>
+      <c r="AI52" s="11"/>
+      <c r="AJ52" s="11"/>
+      <c r="AK52" s="14"/>
+    </row>
+    <row r="53" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L53" s="10"/>
       <c r="M53" s="11"/>
       <c r="N53" s="11"/>
@@ -2264,8 +3372,20 @@
       <c r="U53" s="11"/>
       <c r="V53" s="11"/>
       <c r="W53" s="14"/>
-    </row>
-    <row r="54" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z53" s="10"/>
+      <c r="AA53" s="11"/>
+      <c r="AB53" s="11"/>
+      <c r="AC53" s="11"/>
+      <c r="AD53" s="11"/>
+      <c r="AE53" s="11"/>
+      <c r="AF53" s="11"/>
+      <c r="AG53" s="11"/>
+      <c r="AH53" s="11"/>
+      <c r="AI53" s="11"/>
+      <c r="AJ53" s="11"/>
+      <c r="AK53" s="14"/>
+    </row>
+    <row r="54" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L54" s="10"/>
       <c r="M54" s="11" t="s">
         <v>15</v>
@@ -2294,8 +3414,36 @@
       <c r="U54" s="11"/>
       <c r="V54" s="11"/>
       <c r="W54" s="14"/>
-    </row>
-    <row r="55" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z54" s="10"/>
+      <c r="AA54" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB54" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC54" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD54" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE54" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF54" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG54" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH54" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI54" s="11"/>
+      <c r="AJ54" s="11"/>
+      <c r="AK54" s="14"/>
+    </row>
+    <row r="55" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L55" s="10"/>
       <c r="M55" s="11" t="s">
         <v>16</v>
@@ -2316,8 +3464,28 @@
       <c r="U55" s="11"/>
       <c r="V55" s="15"/>
       <c r="W55" s="14"/>
-    </row>
-    <row r="56" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z55" s="10"/>
+      <c r="AA55" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB55" s="15">
+        <v>2.1062446080000001E-4</v>
+      </c>
+      <c r="AC55" s="15">
+        <v>3.2178662400000001E-4</v>
+      </c>
+      <c r="AD55" s="15"/>
+      <c r="AE55" s="15"/>
+      <c r="AF55" s="15"/>
+      <c r="AG55" s="15"/>
+      <c r="AH55" s="15">
+        <v>5.3241108480000003E-4</v>
+      </c>
+      <c r="AI55" s="11"/>
+      <c r="AJ55" s="15"/>
+      <c r="AK55" s="14"/>
+    </row>
+    <row r="56" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L56" s="10"/>
       <c r="M56" s="11" t="s">
         <v>17</v>
@@ -2338,8 +3506,28 @@
       <c r="U56" s="11"/>
       <c r="V56" s="15"/>
       <c r="W56" s="14"/>
-    </row>
-    <row r="57" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z56" s="10"/>
+      <c r="AA56" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB56" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="AC56" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="AD56" s="15"/>
+      <c r="AE56" s="15"/>
+      <c r="AF56" s="15"/>
+      <c r="AG56" s="15"/>
+      <c r="AH56" s="15">
+        <v>3.5935999999999997E-4</v>
+      </c>
+      <c r="AI56" s="11"/>
+      <c r="AJ56" s="15"/>
+      <c r="AK56" s="14"/>
+    </row>
+    <row r="57" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L57" s="16" t="s">
         <v>0</v>
       </c>
@@ -2362,8 +3550,30 @@
       <c r="U57" s="11"/>
       <c r="V57" s="15"/>
       <c r="W57" s="14"/>
-    </row>
-    <row r="58" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z57" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA57" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB57" s="15">
+        <v>2.1062446080000001E-4</v>
+      </c>
+      <c r="AC57" s="15">
+        <v>3.2178662400000001E-4</v>
+      </c>
+      <c r="AD57" s="15"/>
+      <c r="AE57" s="15"/>
+      <c r="AF57" s="15"/>
+      <c r="AG57" s="15"/>
+      <c r="AH57" s="15">
+        <v>5.3241108480000003E-4</v>
+      </c>
+      <c r="AI57" s="11"/>
+      <c r="AJ57" s="15"/>
+      <c r="AK57" s="14"/>
+    </row>
+    <row r="58" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L58" s="10"/>
       <c r="M58" s="11" t="s">
         <v>19</v>
@@ -2384,8 +3594,28 @@
       <c r="U58" s="11"/>
       <c r="V58" s="15"/>
       <c r="W58" s="14"/>
-    </row>
-    <row r="59" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z58" s="10"/>
+      <c r="AA58" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB58" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="AC58" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="AD58" s="15"/>
+      <c r="AE58" s="15"/>
+      <c r="AF58" s="15"/>
+      <c r="AG58" s="15"/>
+      <c r="AH58" s="15">
+        <v>3.5935999999999997E-4</v>
+      </c>
+      <c r="AI58" s="11"/>
+      <c r="AJ58" s="15"/>
+      <c r="AK58" s="14"/>
+    </row>
+    <row r="59" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L59" s="10"/>
       <c r="M59" s="11" t="s">
         <v>20</v>
@@ -2402,8 +3632,24 @@
       <c r="U59" s="11"/>
       <c r="V59" s="15"/>
       <c r="W59" s="14"/>
-    </row>
-    <row r="60" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z59" s="10"/>
+      <c r="AA59" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB59" s="15"/>
+      <c r="AC59" s="15"/>
+      <c r="AD59" s="15"/>
+      <c r="AE59" s="15"/>
+      <c r="AF59" s="15"/>
+      <c r="AG59" s="15"/>
+      <c r="AH59" s="15">
+        <v>3.339844608E-4</v>
+      </c>
+      <c r="AI59" s="11"/>
+      <c r="AJ59" s="15"/>
+      <c r="AK59" s="14"/>
+    </row>
+    <row r="60" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L60" s="10"/>
       <c r="M60" s="11" t="s">
         <v>21</v>
@@ -2420,8 +3666,24 @@
       <c r="U60" s="11"/>
       <c r="V60" s="15"/>
       <c r="W60" s="14"/>
-    </row>
-    <row r="61" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z60" s="10"/>
+      <c r="AA60" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB60" s="15"/>
+      <c r="AC60" s="15"/>
+      <c r="AD60" s="15"/>
+      <c r="AE60" s="15"/>
+      <c r="AF60" s="15"/>
+      <c r="AG60" s="15"/>
+      <c r="AH60" s="15">
+        <v>3.339844608E-4</v>
+      </c>
+      <c r="AI60" s="11"/>
+      <c r="AJ60" s="15"/>
+      <c r="AK60" s="14"/>
+    </row>
+    <row r="61" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L61" s="10"/>
       <c r="M61" s="11" t="s">
         <v>22</v>
@@ -2438,8 +3700,24 @@
       <c r="U61" s="11"/>
       <c r="V61" s="15"/>
       <c r="W61" s="14"/>
-    </row>
-    <row r="62" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z61" s="10"/>
+      <c r="AA61" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB61" s="15"/>
+      <c r="AC61" s="15"/>
+      <c r="AD61" s="15"/>
+      <c r="AE61" s="15"/>
+      <c r="AF61" s="15"/>
+      <c r="AG61" s="15"/>
+      <c r="AH61" s="15">
+        <v>3.339844608E-4</v>
+      </c>
+      <c r="AI61" s="11"/>
+      <c r="AJ61" s="15"/>
+      <c r="AK61" s="14"/>
+    </row>
+    <row r="62" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L62" s="18"/>
       <c r="M62" s="19"/>
       <c r="N62" s="19"/>
@@ -2452,6 +3730,18 @@
       <c r="U62" s="19"/>
       <c r="V62" s="19"/>
       <c r="W62" s="21"/>
+      <c r="Z62" s="18"/>
+      <c r="AA62" s="19"/>
+      <c r="AB62" s="19"/>
+      <c r="AC62" s="19"/>
+      <c r="AD62" s="19"/>
+      <c r="AE62" s="19"/>
+      <c r="AF62" s="19"/>
+      <c r="AG62" s="19"/>
+      <c r="AH62" s="19"/>
+      <c r="AI62" s="19"/>
+      <c r="AJ62" s="19"/>
+      <c r="AK62" s="21"/>
     </row>
     <row r="65" spans="12:23" x14ac:dyDescent="0.3">
       <c r="L65" s="6"/>
@@ -2823,7 +4113,7 @@
       <c r="N82" s="12">
         <v>2</v>
       </c>
-      <c r="O82" s="12">
+      <c r="O82" s="25">
         <v>264</v>
       </c>
       <c r="P82" s="12">
@@ -2833,10 +4123,10 @@
         <v>100000000</v>
       </c>
       <c r="R82" s="11"/>
-      <c r="S82" s="22">
+      <c r="S82" s="25">
         <v>2796.62592</v>
       </c>
-      <c r="T82" s="12" t="s">
+      <c r="T82" s="25" t="s">
         <v>34</v>
       </c>
       <c r="U82" s="11"/>
@@ -3429,7 +4719,7 @@
       <c r="N113" s="12">
         <v>2</v>
       </c>
-      <c r="O113" s="12">
+      <c r="O113" s="25">
         <v>512</v>
       </c>
       <c r="P113" s="12">
@@ -3439,10 +4729,10 @@
         <v>100000000</v>
       </c>
       <c r="R113" s="11"/>
-      <c r="S113" s="22">
+      <c r="S113" s="25">
         <v>2823.2908799000002</v>
       </c>
-      <c r="T113" s="12" t="s">
+      <c r="T113" s="25" t="s">
         <v>35</v>
       </c>
       <c r="U113" s="11"/>
@@ -4047,7 +5337,7 @@
       <c r="N144" s="12">
         <v>2</v>
       </c>
-      <c r="O144" s="12">
+      <c r="O144" s="25">
         <v>780</v>
       </c>
       <c r="P144" s="12">
@@ -4057,10 +5347,10 @@
         <v>100000000</v>
       </c>
       <c r="R144" s="11"/>
-      <c r="S144" s="22">
+      <c r="S144" s="25">
         <v>19.968000000000501</v>
       </c>
-      <c r="T144" s="12" t="s">
+      <c r="T144" s="25" t="s">
         <v>36</v>
       </c>
       <c r="U144" s="11"/>
@@ -4130,17 +5420,17 @@
       <c r="M148" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="N148" s="24">
+      <c r="N148" s="23">
         <v>1.2415872E-4</v>
       </c>
-      <c r="O148" s="24">
+      <c r="O148" s="23">
         <v>6.1680921599999996E-4</v>
       </c>
-      <c r="P148" s="24"/>
-      <c r="Q148" s="24"/>
-      <c r="R148" s="24"/>
-      <c r="S148" s="24"/>
-      <c r="T148" s="24">
+      <c r="P148" s="23"/>
+      <c r="Q148" s="23"/>
+      <c r="R148" s="23"/>
+      <c r="S148" s="23"/>
+      <c r="T148" s="23">
         <v>7.4096793599999998E-4</v>
       </c>
       <c r="U148" s="11"/>
@@ -4176,17 +5466,17 @@
       <c r="M150" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="N150" s="24">
+      <c r="N150" s="23">
         <v>1.2415872E-4</v>
       </c>
-      <c r="O150" s="24">
+      <c r="O150" s="23">
         <v>6.1680921599999996E-4</v>
       </c>
-      <c r="P150" s="24"/>
-      <c r="Q150" s="24"/>
-      <c r="R150" s="24"/>
-      <c r="S150" s="24"/>
-      <c r="T150" s="24">
+      <c r="P150" s="23"/>
+      <c r="Q150" s="23"/>
+      <c r="R150" s="23"/>
+      <c r="S150" s="23"/>
+      <c r="T150" s="23">
         <v>7.4096793599999998E-4</v>
       </c>
       <c r="U150" s="11"/>
@@ -4286,7 +5576,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="10">
+  <tableParts count="14">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -4297,6 +5587,10 @@
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CBSLine evaluation Prio 1 with MFS of 264Byte
</commit_message>
<xml_diff>
--- a/src/main/java/org/networkcalculus/dnc/demos/Eval_CBSLine/Eval_CBSLine_Results.xlsx
+++ b/src/main/java/org/networkcalculus/dnc/demos/Eval_CBSLine/Eval_CBSLine_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ForceXX\Documents\Studium\FAU_Informatik_Master\FS5\Masterarbeit\Network_Calculus_in_TSN\DNC\IntelliJ\src\main\java\org\networkcalculus\dnc\demos\Eval_CBSLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C245A1-97FA-45B3-9C91-8645004C97BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C3950F-458E-45A8-8C95-66E11C7611F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4104" windowWidth="46080" windowHeight="22152" activeTab="1" xr2:uid="{76093B85-C4EA-4FAC-BB07-8F5ADEBC9C5C}"/>
+    <workbookView xWindow="0" yWindow="5016" windowWidth="46080" windowHeight="22152" activeTab="1" xr2:uid="{76093B85-C4EA-4FAC-BB07-8F5ADEBC9C5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="39">
   <si>
     <t>f1</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>11,264MBit/s</t>
+  </si>
+  <si>
+    <t>16,896MBit/s</t>
   </si>
 </sst>
 </file>
@@ -319,20 +322,62 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="112">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00000000000000000000"/>
     </dxf>
@@ -700,13 +745,13 @@
   <autoFilter ref="M9:T16" xr:uid="{AFD0FDAD-B567-49C8-A37C-DCEECED05009}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{BE6FA1AF-957C-4302-ABCA-3CED577909FB}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{EABB3472-FB4D-420C-9C6B-D5FBAEE8D4FF}" name="S1" dataDxfId="97"/>
-    <tableColumn id="3" xr3:uid="{362B0664-EECB-41EA-8E6D-BC83B9D56EFC}" name="S2" dataDxfId="96"/>
-    <tableColumn id="4" xr3:uid="{6AAC6F6B-16ED-403D-9C2D-403BD383643D}" name="S3" dataDxfId="95"/>
-    <tableColumn id="5" xr3:uid="{AD2D3DC2-A063-43E3-8F4D-72B5648D83E8}" name="S4" dataDxfId="94"/>
-    <tableColumn id="6" xr3:uid="{1ACA20C8-E74E-4AE0-9617-8D84870DB044}" name="S5" dataDxfId="93"/>
-    <tableColumn id="7" xr3:uid="{5FFF2E6B-00A8-47E0-8FF6-2C25AA61CD2E}" name="S6" dataDxfId="92"/>
-    <tableColumn id="8" xr3:uid="{59937D66-C814-42EC-A281-7F9615B9AC54}" name="Total" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{EABB3472-FB4D-420C-9C6B-D5FBAEE8D4FF}" name="S1" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{362B0664-EECB-41EA-8E6D-BC83B9D56EFC}" name="S2" dataDxfId="110"/>
+    <tableColumn id="4" xr3:uid="{6AAC6F6B-16ED-403D-9C2D-403BD383643D}" name="S3" dataDxfId="109"/>
+    <tableColumn id="5" xr3:uid="{AD2D3DC2-A063-43E3-8F4D-72B5648D83E8}" name="S4" dataDxfId="108"/>
+    <tableColumn id="6" xr3:uid="{1ACA20C8-E74E-4AE0-9617-8D84870DB044}" name="S5" dataDxfId="107"/>
+    <tableColumn id="7" xr3:uid="{5FFF2E6B-00A8-47E0-8FF6-2C25AA61CD2E}" name="S6" dataDxfId="106"/>
+    <tableColumn id="8" xr3:uid="{59937D66-C814-42EC-A281-7F9615B9AC54}" name="Total" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -717,13 +762,13 @@
   <autoFilter ref="M147:T154" xr:uid="{2891661D-836E-47DB-BD40-F3A27A090E4F}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5ED748F3-0EF7-490E-9255-D93E2E8A38B3}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{A96E6DCE-0CD4-444C-AC15-B039A4AD73D3}" name="S1" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{A38F3CDE-3B3B-46A2-8F23-68228377ED85}" name="S2" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{8B8B1AD0-037F-4F96-A7E6-AD0731A1A674}" name="S3" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{C2CC595E-C7DA-4A76-917C-24B06D46A036}" name="S4" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{68190FF9-32AD-4425-9D62-C708869AA72B}" name="S5" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{FA329009-A789-402C-A1BE-8BA2289036EA}" name="S6" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{F099B37D-2BC9-4533-80BD-70060862C629}" name="Total" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{A96E6DCE-0CD4-444C-AC15-B039A4AD73D3}" name="S1" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{A38F3CDE-3B3B-46A2-8F23-68228377ED85}" name="S2" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{8B8B1AD0-037F-4F96-A7E6-AD0731A1A674}" name="S3" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{C2CC595E-C7DA-4A76-917C-24B06D46A036}" name="S4" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{68190FF9-32AD-4425-9D62-C708869AA72B}" name="S5" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{FA329009-A789-402C-A1BE-8BA2289036EA}" name="S6" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{F099B37D-2BC9-4533-80BD-70060862C629}" name="Total" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -734,13 +779,13 @@
   <autoFilter ref="AA9:AH16" xr:uid="{20E3359C-A163-4D07-9B73-3FE6F5470B48}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9D844AAF-0CDD-4431-955C-97AB5934E28C}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{C6418D28-1657-4D0C-9B1B-EFDBC441468D}" name="S1" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{5AD084BF-33BD-4934-ABFB-0D84D5716194}" name="S2" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{53F5A0F2-3C27-49EF-B38F-8AB6AFFF4585}" name="S3" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{AEFCE6A1-82A7-4762-8A87-8D7EE290BEF8}" name="S4" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{C005E345-92BC-4E8E-9ACC-1B22BB62D299}" name="S5" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{1CCACC3C-ED33-4844-B76F-F79AE1FC676C}" name="S6" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{5ED8CE44-AA0C-409B-812F-F763BC573AE3}" name="Total" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{C6418D28-1657-4D0C-9B1B-EFDBC441468D}" name="S1" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{5AD084BF-33BD-4934-ABFB-0D84D5716194}" name="S2" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{53F5A0F2-3C27-49EF-B38F-8AB6AFFF4585}" name="S3" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{AEFCE6A1-82A7-4762-8A87-8D7EE290BEF8}" name="S4" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{C005E345-92BC-4E8E-9ACC-1B22BB62D299}" name="S5" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{1CCACC3C-ED33-4844-B76F-F79AE1FC676C}" name="S6" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{5ED8CE44-AA0C-409B-812F-F763BC573AE3}" name="Total" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -751,13 +796,13 @@
   <autoFilter ref="AA23:AH30" xr:uid="{6B2C2460-94FC-4FB2-B838-01558F80A0D9}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{42188820-7181-4146-8D9B-483A6841AD2B}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{F875B116-BDC1-4F83-909D-624F36B983BA}" name="S1" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{683F8336-33FB-490C-927E-9EF0BB58C272}" name="S2" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{9B94A0E2-3731-4ECB-93CE-EA29BF8F0FB8}" name="S3" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{43398B5B-74D8-401A-A3DB-BBE6A00516D1}" name="S4" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{28F6192D-A9EF-4A04-987C-F9B382230D36}" name="S5" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{57B2B5DA-BD8D-44B0-A99C-DDC5309B66C8}" name="S6" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{EE9281C4-C299-4F06-9DE0-BAC560DC340D}" name="Total" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{F875B116-BDC1-4F83-909D-624F36B983BA}" name="S1" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{683F8336-33FB-490C-927E-9EF0BB58C272}" name="S2" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{9B94A0E2-3731-4ECB-93CE-EA29BF8F0FB8}" name="S3" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{43398B5B-74D8-401A-A3DB-BBE6A00516D1}" name="S4" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{28F6192D-A9EF-4A04-987C-F9B382230D36}" name="S5" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{57B2B5DA-BD8D-44B0-A99C-DDC5309B66C8}" name="S6" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{EE9281C4-C299-4F06-9DE0-BAC560DC340D}" name="Total" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -768,13 +813,13 @@
   <autoFilter ref="AA40:AH47" xr:uid="{9014955E-1965-4C9A-A9DC-52D322018E9C}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{85E8EEDB-E008-4D1E-84BA-7DAFD9B3B91A}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{9BAD68DC-D763-4EE6-8E7F-CF3BCBB288AB}" name="S1" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{F326866F-0A2F-4DAE-B81A-22A042D880AB}" name="S2" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{C91B65B3-A7A1-443E-8824-F147FE1A78D3}" name="S3" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{75D3802F-681F-4C3E-A022-2A048AF821C2}" name="S4" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{EBB82DA4-8866-4F55-9021-87127839AD21}" name="S5" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{72E3FD25-D43A-4384-9CC5-2793827655E1}" name="S6" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{340E3E17-7D6E-477A-BCA8-6436048088BC}" name="Total" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{9BAD68DC-D763-4EE6-8E7F-CF3BCBB288AB}" name="S1" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{F326866F-0A2F-4DAE-B81A-22A042D880AB}" name="S2" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{C91B65B3-A7A1-443E-8824-F147FE1A78D3}" name="S3" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{75D3802F-681F-4C3E-A022-2A048AF821C2}" name="S4" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{EBB82DA4-8866-4F55-9021-87127839AD21}" name="S5" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{72E3FD25-D43A-4384-9CC5-2793827655E1}" name="S6" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{340E3E17-7D6E-477A-BCA8-6436048088BC}" name="Total" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -785,13 +830,47 @@
   <autoFilter ref="AA54:AH61" xr:uid="{86B4AE62-98EF-4BDD-A78A-F87936C846E5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{FF1A5694-D41B-4A7A-AA69-CBB5EE0C4B7B}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{0C4C9F88-B7DD-4351-8C71-782E9D04C6F2}" name="S1" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{D7790C6F-74E4-4EBC-B244-F62780858E7C}" name="S2" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{32DA1EDD-693D-4ABB-A925-5FFE72CED6F5}" name="S3" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{5C9EA794-90CA-4009-980D-8CB10E63E5B4}" name="S4" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{2547B789-108B-4EB1-902A-4248C1F2E3AC}" name="S5" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{A6B77A2A-9DAA-492F-9584-428DCF062F04}" name="S6" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{CADDCCE0-1DD5-4109-9FA0-A0D19ECD12A9}" name="Total" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{0C4C9F88-B7DD-4351-8C71-782E9D04C6F2}" name="S1" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{D7790C6F-74E4-4EBC-B244-F62780858E7C}" name="S2" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{32DA1EDD-693D-4ABB-A925-5FFE72CED6F5}" name="S3" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{5C9EA794-90CA-4009-980D-8CB10E63E5B4}" name="S4" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{2547B789-108B-4EB1-902A-4248C1F2E3AC}" name="S5" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{A6B77A2A-9DAA-492F-9584-428DCF062F04}" name="S6" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{CADDCCE0-1DD5-4109-9FA0-A0D19ECD12A9}" name="Total" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{33B7A1DF-04CF-4188-8895-C497DE057B78}" name="Tabelle14121416" displayName="Tabelle14121416" ref="AA71:AH78" totalsRowShown="0">
+  <autoFilter ref="AA71:AH78" xr:uid="{BC4EBD0B-BD33-487C-8A1C-6DC244BEF9A5}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{C291C5E0-A57A-49FE-9A3C-EB26519E9FA0}" name="Analysis"/>
+    <tableColumn id="2" xr3:uid="{59D9B17D-5628-447F-A2DF-9CE9C3EEADB5}" name="S1" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{4141CBA9-9E1C-488E-B23D-12BFCC6982D7}" name="S2" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{74411D26-01B5-4918-B3FE-407A83F88764}" name="S3" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{BA7FF53B-526B-425D-9E9A-CA78118B689C}" name="S4" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{A4AD019F-5CB8-4EB8-9A72-3430AABAB4C9}" name="S5" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{C28CA15E-C51A-4275-9CE3-EF5909E727E4}" name="S6" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{977A5EA4-D8C2-4A8C-B69C-EB7DC70BAD1A}" name="Total" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{227BBFB7-D629-4AD4-98DA-5F2813E954F7}" name="Tabelle135131517" displayName="Tabelle135131517" ref="AA85:AH92" totalsRowShown="0">
+  <autoFilter ref="AA85:AH92" xr:uid="{701EFE6D-343B-4A16-8186-4717329795E9}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{C461D4E7-A17E-4CE2-8BA7-9461F5D21D40}" name="Analysis"/>
+    <tableColumn id="2" xr3:uid="{5B7B0F75-5C30-4477-91A1-8D37C1A9BFAC}" name="S1" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{D5AFA13C-AE10-4AB9-82E4-B9B18EF1A703}" name="S2" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{EF59A065-AA08-4782-AB9A-7693364A053B}" name="S3" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{E5D25AFF-5500-4AB9-B819-FF0F2E9B8995}" name="S4" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{64141ECF-BE07-4D18-9262-1B867AFE8D3F}" name="S5" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{2B8C867B-2973-4F94-9984-45040B80AE04}" name="S6" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{4128D960-E4CB-46EF-8239-5806C9DF4FD8}" name="Total" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -802,13 +881,13 @@
   <autoFilter ref="M23:T30" xr:uid="{9F3FFC4E-8857-417C-879B-7E46756E6ACB}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{6C7A2137-FE16-4D18-B3E5-47340E52F2D5}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{EDDA7831-D99A-413F-AA04-C00A206D6D34}" name="S1" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{3CB5E796-20A3-4C92-9FC5-590D66DC5593}" name="S2" dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{3D106F77-8448-4063-87F7-7B7BE008B2F2}" name="S3" dataDxfId="88"/>
-    <tableColumn id="5" xr3:uid="{A891D787-2819-425A-9CE0-E8145AC0C05B}" name="S4" dataDxfId="87"/>
-    <tableColumn id="6" xr3:uid="{C6263B6C-6BFC-46DD-94D3-5EDB5A4EAF2F}" name="S5" dataDxfId="86"/>
-    <tableColumn id="7" xr3:uid="{AAC57713-C8ED-436C-B744-473CD5CFAB13}" name="S6" dataDxfId="85"/>
-    <tableColumn id="8" xr3:uid="{31F74DD7-5067-4854-B832-9EFA7B4543EA}" name="Total" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{EDDA7831-D99A-413F-AA04-C00A206D6D34}" name="S1" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{3CB5E796-20A3-4C92-9FC5-590D66DC5593}" name="S2" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{3D106F77-8448-4063-87F7-7B7BE008B2F2}" name="S3" dataDxfId="102"/>
+    <tableColumn id="5" xr3:uid="{A891D787-2819-425A-9CE0-E8145AC0C05B}" name="S4" dataDxfId="101"/>
+    <tableColumn id="6" xr3:uid="{C6263B6C-6BFC-46DD-94D3-5EDB5A4EAF2F}" name="S5" dataDxfId="100"/>
+    <tableColumn id="7" xr3:uid="{AAC57713-C8ED-436C-B744-473CD5CFAB13}" name="S6" dataDxfId="99"/>
+    <tableColumn id="8" xr3:uid="{31F74DD7-5067-4854-B832-9EFA7B4543EA}" name="Total" dataDxfId="98"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -819,13 +898,13 @@
   <autoFilter ref="M40:T47" xr:uid="{E16230B5-F45F-4647-925B-5EE18F895F9C}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9D1375EE-0D83-4727-B0F9-FE752E8A0CBC}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{C37D03EB-F7B2-4349-B2CC-726DB4010C90}" name="S1" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{7037993D-3D73-4283-A3B4-93C5B4E6E202}" name="S2" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{7ADA14D4-6575-4C8D-A7EA-C47F389375CE}" name="S3" dataDxfId="81"/>
-    <tableColumn id="5" xr3:uid="{5429F400-2F0F-4356-AC4A-9C65390A88EF}" name="S4" dataDxfId="80"/>
-    <tableColumn id="6" xr3:uid="{65870CF8-359E-4FAC-947D-39633692A667}" name="S5" dataDxfId="79"/>
-    <tableColumn id="7" xr3:uid="{59753DB4-DBE6-466A-BCC2-D1C2D56D1A27}" name="S6" dataDxfId="78"/>
-    <tableColumn id="8" xr3:uid="{51BDBB4F-8359-4885-B4D7-DF406809ECB7}" name="Total" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{C37D03EB-F7B2-4349-B2CC-726DB4010C90}" name="S1" dataDxfId="97"/>
+    <tableColumn id="3" xr3:uid="{7037993D-3D73-4283-A3B4-93C5B4E6E202}" name="S2" dataDxfId="96"/>
+    <tableColumn id="4" xr3:uid="{7ADA14D4-6575-4C8D-A7EA-C47F389375CE}" name="S3" dataDxfId="95"/>
+    <tableColumn id="5" xr3:uid="{5429F400-2F0F-4356-AC4A-9C65390A88EF}" name="S4" dataDxfId="94"/>
+    <tableColumn id="6" xr3:uid="{65870CF8-359E-4FAC-947D-39633692A667}" name="S5" dataDxfId="93"/>
+    <tableColumn id="7" xr3:uid="{59753DB4-DBE6-466A-BCC2-D1C2D56D1A27}" name="S6" dataDxfId="92"/>
+    <tableColumn id="8" xr3:uid="{51BDBB4F-8359-4885-B4D7-DF406809ECB7}" name="Total" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -836,13 +915,13 @@
   <autoFilter ref="M54:T61" xr:uid="{B5EBC119-6892-4EFB-AB7E-F78E33D432A9}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0BB4E427-3492-4DCF-9D08-38551180E6EE}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{625D768D-2EA2-4E64-B741-35AF2819C1F7}" name="S1" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{2FA180EB-2936-481F-B1D1-4C1DA624FA57}" name="S2" dataDxfId="75"/>
-    <tableColumn id="4" xr3:uid="{7EDAFDAC-585A-4749-ABD8-DEBBA52F7B86}" name="S3" dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{3E05A679-5166-455F-9DE8-C76697485C01}" name="S4" dataDxfId="73"/>
-    <tableColumn id="6" xr3:uid="{9611ADE2-11EE-403F-8E25-5BF3FD83A7EE}" name="S5" dataDxfId="72"/>
-    <tableColumn id="7" xr3:uid="{4B5CC043-D947-410A-8D8E-B4B1EDA50E93}" name="S6" dataDxfId="71"/>
-    <tableColumn id="8" xr3:uid="{90BF4DC0-8F16-4F8E-AD7A-04145C27A52D}" name="Total" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{625D768D-2EA2-4E64-B741-35AF2819C1F7}" name="S1" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{2FA180EB-2936-481F-B1D1-4C1DA624FA57}" name="S2" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{7EDAFDAC-585A-4749-ABD8-DEBBA52F7B86}" name="S3" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{3E05A679-5166-455F-9DE8-C76697485C01}" name="S4" dataDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{9611ADE2-11EE-403F-8E25-5BF3FD83A7EE}" name="S5" dataDxfId="86"/>
+    <tableColumn id="7" xr3:uid="{4B5CC043-D947-410A-8D8E-B4B1EDA50E93}" name="S6" dataDxfId="85"/>
+    <tableColumn id="8" xr3:uid="{90BF4DC0-8F16-4F8E-AD7A-04145C27A52D}" name="Total" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -853,13 +932,13 @@
   <autoFilter ref="M71:T78" xr:uid="{51782671-9EEB-46B0-812D-DE4D14A213EE}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{AD5E4FB3-F32D-4B93-86CA-C7ECF985973B}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{32771DFC-FFFB-479C-8088-AA245ED9B201}" name="S1" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{850259B7-F6FC-40B4-94B0-436FE4A42169}" name="S2" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{D83AC1AB-1A0A-4527-925F-218D72D2227A}" name="S3" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{9AE7B8F5-E983-41B9-B1F4-4FC70710981E}" name="S4" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{BF918F35-6CDD-4DEE-956C-2A3434C345D0}" name="S5" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{8BF14E06-E1BE-45C5-B2AF-D712C65491A2}" name="S6" dataDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{386EE86E-EBB8-4A4D-B17D-421040C58630}" name="Total" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{32771DFC-FFFB-479C-8088-AA245ED9B201}" name="S1" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{850259B7-F6FC-40B4-94B0-436FE4A42169}" name="S2" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{D83AC1AB-1A0A-4527-925F-218D72D2227A}" name="S3" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{9AE7B8F5-E983-41B9-B1F4-4FC70710981E}" name="S4" dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{BF918F35-6CDD-4DEE-956C-2A3434C345D0}" name="S5" dataDxfId="79"/>
+    <tableColumn id="7" xr3:uid="{8BF14E06-E1BE-45C5-B2AF-D712C65491A2}" name="S6" dataDxfId="78"/>
+    <tableColumn id="8" xr3:uid="{386EE86E-EBB8-4A4D-B17D-421040C58630}" name="Total" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -870,13 +949,13 @@
   <autoFilter ref="M85:T92" xr:uid="{B8C55D2C-921B-49DD-AC76-772D4A43E64D}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{1B1BABD6-FD5C-41BB-948A-6FC0BCC11D24}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{DB6F9D20-C97E-480C-99B2-E87E4A9E1E0E}" name="S1" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{6D579111-6BD1-4C25-A59D-5752C6D1027B}" name="S2" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{971D35F8-9047-4D4E-B3A8-1050E4CBB9F7}" name="S3" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{12EA7A8D-ED74-4686-A548-2A70B019DDD4}" name="S4" dataDxfId="59"/>
-    <tableColumn id="6" xr3:uid="{1FE3C278-2C61-4E80-AD86-3FA5279E30B5}" name="S5" dataDxfId="58"/>
-    <tableColumn id="7" xr3:uid="{EE077AF3-1AB4-421C-B5DC-9511794D8F8E}" name="S6" dataDxfId="57"/>
-    <tableColumn id="8" xr3:uid="{4D81D46E-0FA9-4BFC-8316-8FE6191F7B12}" name="Total" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{DB6F9D20-C97E-480C-99B2-E87E4A9E1E0E}" name="S1" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{6D579111-6BD1-4C25-A59D-5752C6D1027B}" name="S2" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{971D35F8-9047-4D4E-B3A8-1050E4CBB9F7}" name="S3" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{12EA7A8D-ED74-4686-A548-2A70B019DDD4}" name="S4" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{1FE3C278-2C61-4E80-AD86-3FA5279E30B5}" name="S5" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{EE077AF3-1AB4-421C-B5DC-9511794D8F8E}" name="S6" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{4D81D46E-0FA9-4BFC-8316-8FE6191F7B12}" name="Total" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -887,13 +966,13 @@
   <autoFilter ref="M102:T109" xr:uid="{3B58D87F-510B-43F0-BC7D-8EF14E94029E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E6C46FA4-813C-4003-A6A1-34967D676206}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{C1B5C27C-40D8-4CE6-8300-D32B61DBD03E}" name="S1" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{822EBEC2-E9F3-433C-9D06-01D83E51B4EC}" name="S2" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{7E24F410-F931-4EB2-B8F2-71F614752416}" name="S3" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{6F4DDE75-12D5-4E09-BD4C-B84DBE3A1613}" name="S4" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{D1A7BB02-6526-44E4-BAC4-F951ACEB49E0}" name="S5" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{CA43AF65-8F45-41AF-809C-76D07CBDCA7B}" name="S6" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{AA305A43-F356-44F9-B1BE-8A8539A588B2}" name="Total" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{C1B5C27C-40D8-4CE6-8300-D32B61DBD03E}" name="S1" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{822EBEC2-E9F3-433C-9D06-01D83E51B4EC}" name="S2" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{7E24F410-F931-4EB2-B8F2-71F614752416}" name="S3" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{6F4DDE75-12D5-4E09-BD4C-B84DBE3A1613}" name="S4" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{D1A7BB02-6526-44E4-BAC4-F951ACEB49E0}" name="S5" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{CA43AF65-8F45-41AF-809C-76D07CBDCA7B}" name="S6" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{AA305A43-F356-44F9-B1BE-8A8539A588B2}" name="Total" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -904,13 +983,13 @@
   <autoFilter ref="M116:T123" xr:uid="{BBD41544-5CF6-451E-B19F-AA4B349E0FF5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F68E10CC-FD59-48C5-91A8-4F747980D2B8}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{091DCD40-AFF4-4A35-A51B-5CE995B27C5B}" name="S1" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{32F634D5-1211-4A7C-8411-0DC8BF7C0116}" name="S2" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{BE2DA717-3CEA-4B45-9D01-B2AF2CFBA155}" name="S3" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{820A1FC2-AB1F-424D-8760-928CAC5CEC89}" name="S4" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{7CDBF264-CA71-4555-AD13-B4F0B0EFF5CB}" name="S5" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{FD7873DE-5A47-42D5-BE83-3AC049767285}" name="S6" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{514BF621-1FB2-46A5-A883-5F156AE64F89}" name="Total" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{091DCD40-AFF4-4A35-A51B-5CE995B27C5B}" name="S1" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{32F634D5-1211-4A7C-8411-0DC8BF7C0116}" name="S2" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{BE2DA717-3CEA-4B45-9D01-B2AF2CFBA155}" name="S3" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{820A1FC2-AB1F-424D-8760-928CAC5CEC89}" name="S4" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{7CDBF264-CA71-4555-AD13-B4F0B0EFF5CB}" name="S5" dataDxfId="58"/>
+    <tableColumn id="7" xr3:uid="{FD7873DE-5A47-42D5-BE83-3AC049767285}" name="S6" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{514BF621-1FB2-46A5-A883-5F156AE64F89}" name="Total" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -921,13 +1000,13 @@
   <autoFilter ref="M133:T140" xr:uid="{FB41092D-F5FF-4971-9DDD-C9E03FD01631}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{6647CD1D-0845-4A23-9836-FBC960574DA7}" name="Analysis"/>
-    <tableColumn id="2" xr3:uid="{5BD82A11-F2EA-4903-B53D-DD982E06A315}" name="S1" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{424AE262-E0C8-44A2-B28D-3F028CA6231F}" name="S2" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{D576FA30-995E-46FE-8DB0-5798DAE28331}" name="S3" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{B630E084-8616-40E7-A93B-DA34C763EADC}" name="S4" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{04C38EE3-C04A-4AE3-B01D-D5CC7EEF4DE2}" name="S5" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{68C4544A-4832-4B5A-9EE3-E132B259AACC}" name="S6" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{71294977-C366-4F0A-B7E5-972975477A7D}" name="Total" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{5BD82A11-F2EA-4903-B53D-DD982E06A315}" name="S1" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{424AE262-E0C8-44A2-B28D-3F028CA6231F}" name="S2" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{D576FA30-995E-46FE-8DB0-5798DAE28331}" name="S3" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{B630E084-8616-40E7-A93B-DA34C763EADC}" name="S4" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{04C38EE3-C04A-4AE3-B01D-D5CC7EEF4DE2}" name="S5" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{68C4544A-4832-4B5A-9EE3-E132B259AACC}" name="S6" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{71294977-C366-4F0A-B7E5-972975477A7D}" name="Total" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1233,7 +1312,7 @@
   <dimension ref="B3:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1256,17 +1335,17 @@
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
       <c r="K3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="4">
         <f>B4*C4*8</f>
-        <v>2816</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
@@ -1274,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>176</v>
+        <v>264</v>
       </c>
       <c r="D4" s="1">
         <v>2.5000000000000001E-4</v>
@@ -1290,7 +1369,7 @@
       </c>
       <c r="L4" s="5">
         <f>L3/D4</f>
-        <v>11264000</v>
+        <v>16896000</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
@@ -1299,7 +1378,7 @@
       </c>
       <c r="L5" s="4">
         <f>L3*(1-(L4/E4))</f>
-        <v>2498.8057600000002</v>
+        <v>3510.3129600000002</v>
       </c>
     </row>
   </sheetData>
@@ -1315,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB25049-F719-48DC-B24C-CE81CB877780}">
   <dimension ref="B3:AK155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AL26" sqref="AL26"/>
+    <sheetView tabSelected="1" topLeftCell="S43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AE97" sqref="AE97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1419,7 +1498,7 @@
       <c r="AB4" s="12">
         <v>2</v>
       </c>
-      <c r="AC4" s="25">
+      <c r="AC4" s="24">
         <v>88</v>
       </c>
       <c r="AD4" s="12">
@@ -1429,10 +1508,10 @@
         <v>100000000</v>
       </c>
       <c r="AF4" s="11"/>
-      <c r="AG4" s="26">
+      <c r="AG4" s="25">
         <v>1328.70144</v>
       </c>
-      <c r="AH4" s="25" t="s">
+      <c r="AH4" s="24" t="s">
         <v>32</v>
       </c>
       <c r="AI4" s="11"/>
@@ -2074,7 +2153,7 @@
       <c r="N20" s="12">
         <v>2</v>
       </c>
-      <c r="O20" s="25">
+      <c r="O20" s="24">
         <v>88</v>
       </c>
       <c r="P20" s="12">
@@ -2084,10 +2163,10 @@
         <v>100000000</v>
       </c>
       <c r="R20" s="11"/>
-      <c r="S20" s="26">
+      <c r="S20" s="25">
         <v>1249.4028800000001</v>
       </c>
-      <c r="T20" s="25" t="s">
+      <c r="T20" s="24" t="s">
         <v>31</v>
       </c>
       <c r="U20" s="11"/>
@@ -2645,7 +2724,7 @@
       <c r="AB35" s="12">
         <v>2</v>
       </c>
-      <c r="AC35" s="25">
+      <c r="AC35" s="24">
         <v>176</v>
       </c>
       <c r="AD35" s="12">
@@ -2655,10 +2734,10 @@
         <v>100000000</v>
       </c>
       <c r="AF35" s="11"/>
-      <c r="AG35" s="26">
+      <c r="AG35" s="25">
         <v>2498.8057600000002</v>
       </c>
-      <c r="AH35" s="25" t="s">
+      <c r="AH35" s="24" t="s">
         <v>37</v>
       </c>
       <c r="AI35" s="11"/>
@@ -3287,7 +3366,7 @@
       <c r="N51" s="12">
         <v>2</v>
       </c>
-      <c r="O51" s="25">
+      <c r="O51" s="24">
         <v>176</v>
       </c>
       <c r="P51" s="12">
@@ -3297,10 +3376,10 @@
         <v>100000000</v>
       </c>
       <c r="R51" s="11"/>
-      <c r="S51" s="25">
+      <c r="S51" s="24">
         <v>2181.6115199999999</v>
       </c>
-      <c r="T51" s="25" t="s">
+      <c r="T51" s="24" t="s">
         <v>33</v>
       </c>
       <c r="U51" s="11"/>
@@ -3743,7 +3822,7 @@
       <c r="AJ62" s="19"/>
       <c r="AK62" s="21"/>
     </row>
-    <row r="65" spans="12:23" x14ac:dyDescent="0.3">
+    <row r="65" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L65" s="6"/>
       <c r="M65" s="7" t="s">
         <v>26</v>
@@ -3770,8 +3849,34 @@
       <c r="U65" s="7"/>
       <c r="V65" s="7"/>
       <c r="W65" s="9"/>
-    </row>
-    <row r="66" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z65" s="6"/>
+      <c r="AA65" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB65" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC65" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD65" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE65" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF65" s="7"/>
+      <c r="AG65" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH65" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI65" s="7"/>
+      <c r="AJ65" s="7"/>
+      <c r="AK65" s="9"/>
+    </row>
+    <row r="66" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L66" s="10"/>
       <c r="M66" s="11" t="s">
         <v>27</v>
@@ -3798,8 +3903,34 @@
       <c r="U66" s="11"/>
       <c r="V66" s="11"/>
       <c r="W66" s="14"/>
-    </row>
-    <row r="67" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z66" s="10"/>
+      <c r="AA66" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB66" s="12">
+        <v>2</v>
+      </c>
+      <c r="AC66" s="24">
+        <v>264</v>
+      </c>
+      <c r="AD66" s="12">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="AE66" s="13">
+        <v>100000000</v>
+      </c>
+      <c r="AF66" s="11"/>
+      <c r="AG66" s="25">
+        <v>3510.3129600000002</v>
+      </c>
+      <c r="AH66" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI66" s="11"/>
+      <c r="AJ66" s="11"/>
+      <c r="AK66" s="14"/>
+    </row>
+    <row r="67" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L67" s="10"/>
       <c r="M67" s="11"/>
       <c r="N67" s="11"/>
@@ -3812,8 +3943,20 @@
       <c r="U67" s="11"/>
       <c r="V67" s="11"/>
       <c r="W67" s="14"/>
-    </row>
-    <row r="68" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z67" s="10"/>
+      <c r="AA67" s="11"/>
+      <c r="AB67" s="11"/>
+      <c r="AC67" s="11"/>
+      <c r="AD67" s="11"/>
+      <c r="AE67" s="11"/>
+      <c r="AF67" s="11"/>
+      <c r="AG67" s="11"/>
+      <c r="AH67" s="11"/>
+      <c r="AI67" s="11"/>
+      <c r="AJ67" s="11"/>
+      <c r="AK67" s="14"/>
+    </row>
+    <row r="68" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L68" s="10"/>
       <c r="M68" s="11"/>
       <c r="N68" s="11"/>
@@ -3826,8 +3969,20 @@
       <c r="U68" s="11"/>
       <c r="V68" s="11"/>
       <c r="W68" s="14"/>
-    </row>
-    <row r="69" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z68" s="10"/>
+      <c r="AA68" s="11"/>
+      <c r="AB68" s="11"/>
+      <c r="AC68" s="11"/>
+      <c r="AD68" s="11"/>
+      <c r="AE68" s="11"/>
+      <c r="AF68" s="11"/>
+      <c r="AG68" s="11"/>
+      <c r="AH68" s="11"/>
+      <c r="AI68" s="11"/>
+      <c r="AJ68" s="11"/>
+      <c r="AK68" s="14"/>
+    </row>
+    <row r="69" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L69" s="10"/>
       <c r="M69" s="11"/>
       <c r="N69" s="11"/>
@@ -3840,8 +3995,20 @@
       <c r="U69" s="11"/>
       <c r="V69" s="11"/>
       <c r="W69" s="14"/>
-    </row>
-    <row r="70" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z69" s="10"/>
+      <c r="AA69" s="11"/>
+      <c r="AB69" s="11"/>
+      <c r="AC69" s="11"/>
+      <c r="AD69" s="11"/>
+      <c r="AE69" s="11"/>
+      <c r="AF69" s="11"/>
+      <c r="AG69" s="11"/>
+      <c r="AH69" s="11"/>
+      <c r="AI69" s="11"/>
+      <c r="AJ69" s="11"/>
+      <c r="AK69" s="14"/>
+    </row>
+    <row r="70" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L70" s="10"/>
       <c r="M70" s="11"/>
       <c r="N70" s="11"/>
@@ -3854,8 +4021,20 @@
       <c r="U70" s="11"/>
       <c r="V70" s="11"/>
       <c r="W70" s="14"/>
-    </row>
-    <row r="71" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z70" s="10"/>
+      <c r="AA70" s="11"/>
+      <c r="AB70" s="11"/>
+      <c r="AC70" s="11"/>
+      <c r="AD70" s="11"/>
+      <c r="AE70" s="11"/>
+      <c r="AF70" s="11"/>
+      <c r="AG70" s="11"/>
+      <c r="AH70" s="11"/>
+      <c r="AI70" s="11"/>
+      <c r="AJ70" s="11"/>
+      <c r="AK70" s="14"/>
+    </row>
+    <row r="71" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L71" s="10"/>
       <c r="M71" s="11" t="s">
         <v>15</v>
@@ -3884,8 +4063,36 @@
       <c r="U71" s="11"/>
       <c r="V71" s="11"/>
       <c r="W71" s="14"/>
-    </row>
-    <row r="72" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z71" s="10"/>
+      <c r="AA71" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB71" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC71" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD71" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE71" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF71" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG71" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH71" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI71" s="11"/>
+      <c r="AJ71" s="11"/>
+      <c r="AK71" s="14"/>
+    </row>
+    <row r="72" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L72" s="10"/>
       <c r="M72" s="11" t="s">
         <v>16</v>
@@ -3914,8 +4121,36 @@
       <c r="U72" s="11"/>
       <c r="V72" s="15"/>
       <c r="W72" s="14"/>
-    </row>
-    <row r="73" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z72" s="10"/>
+      <c r="AA72" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB72" s="15">
+        <v>2.3424824831999999E-3</v>
+      </c>
+      <c r="AC72" s="15">
+        <v>3.0910525439999998E-4</v>
+      </c>
+      <c r="AD72" s="15">
+        <v>3.6944424959999998E-4</v>
+      </c>
+      <c r="AE72" s="15">
+        <v>4.2978324479999997E-4</v>
+      </c>
+      <c r="AF72" s="15">
+        <v>4.9012223999999997E-4</v>
+      </c>
+      <c r="AG72" s="15">
+        <v>4.9526123519999998E-4</v>
+      </c>
+      <c r="AH72" s="15">
+        <v>2.3424824831999999E-3</v>
+      </c>
+      <c r="AI72" s="11"/>
+      <c r="AJ72" s="15"/>
+      <c r="AK72" s="14"/>
+    </row>
+    <row r="73" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L73" s="10"/>
       <c r="M73" s="11" t="s">
         <v>17</v>
@@ -3944,8 +4179,36 @@
       <c r="U73" s="11"/>
       <c r="V73" s="15"/>
       <c r="W73" s="14"/>
-    </row>
-    <row r="74" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z73" s="10"/>
+      <c r="AA73" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB73" s="15">
+        <v>2.208E-4</v>
+      </c>
+      <c r="AC73" s="15">
+        <v>2.208E-4</v>
+      </c>
+      <c r="AD73" s="15">
+        <v>2.208E-4</v>
+      </c>
+      <c r="AE73" s="15">
+        <v>2.208E-4</v>
+      </c>
+      <c r="AF73" s="15">
+        <v>2.208E-4</v>
+      </c>
+      <c r="AG73" s="15">
+        <v>1.6559999999999999E-4</v>
+      </c>
+      <c r="AH73" s="15">
+        <v>1.2696000000000001E-3</v>
+      </c>
+      <c r="AI73" s="11"/>
+      <c r="AJ73" s="15"/>
+      <c r="AK73" s="14"/>
+    </row>
+    <row r="74" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L74" s="16" t="s">
         <v>24</v>
       </c>
@@ -3976,8 +4239,38 @@
       <c r="U74" s="11"/>
       <c r="V74" s="15"/>
       <c r="W74" s="14"/>
-    </row>
-    <row r="75" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z74" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA74" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB74" s="15">
+        <v>2.4876625919999999E-4</v>
+      </c>
+      <c r="AC74" s="15">
+        <v>3.0910525439999998E-4</v>
+      </c>
+      <c r="AD74" s="15">
+        <v>3.6944424959999998E-4</v>
+      </c>
+      <c r="AE74" s="15">
+        <v>4.2047999999999999E-4</v>
+      </c>
+      <c r="AF74" s="15">
+        <v>4.2047999999999999E-4</v>
+      </c>
+      <c r="AG74" s="15">
+        <v>3.6528E-4</v>
+      </c>
+      <c r="AH74" s="15">
+        <v>2.1335557631999998E-3</v>
+      </c>
+      <c r="AI74" s="11"/>
+      <c r="AJ74" s="15"/>
+      <c r="AK74" s="14"/>
+    </row>
+    <row r="75" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L75" s="10"/>
       <c r="M75" s="11" t="s">
         <v>19</v>
@@ -3994,8 +4287,36 @@
       <c r="U75" s="11"/>
       <c r="V75" s="15"/>
       <c r="W75" s="14"/>
-    </row>
-    <row r="76" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z75" s="10"/>
+      <c r="AA75" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB75" s="15">
+        <v>2.208E-4</v>
+      </c>
+      <c r="AC75" s="15">
+        <v>2.208E-4</v>
+      </c>
+      <c r="AD75" s="15">
+        <v>2.208E-4</v>
+      </c>
+      <c r="AE75" s="15">
+        <v>2.208E-4</v>
+      </c>
+      <c r="AF75" s="15">
+        <v>2.208E-4</v>
+      </c>
+      <c r="AG75" s="15">
+        <v>1.6559999999999999E-4</v>
+      </c>
+      <c r="AH75" s="15">
+        <v>1.2696000000000001E-3</v>
+      </c>
+      <c r="AI75" s="11"/>
+      <c r="AJ75" s="15"/>
+      <c r="AK75" s="14"/>
+    </row>
+    <row r="76" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L76" s="10"/>
       <c r="M76" s="11" t="s">
         <v>20</v>
@@ -4012,8 +4333,24 @@
       <c r="U76" s="11"/>
       <c r="V76" s="15"/>
       <c r="W76" s="14"/>
-    </row>
-    <row r="77" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z76" s="10"/>
+      <c r="AA76" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB76" s="15"/>
+      <c r="AC76" s="15"/>
+      <c r="AD76" s="15"/>
+      <c r="AE76" s="15"/>
+      <c r="AF76" s="15"/>
+      <c r="AG76" s="15"/>
+      <c r="AH76" s="15">
+        <v>1.0863662592000001E-3</v>
+      </c>
+      <c r="AI76" s="11"/>
+      <c r="AJ76" s="15"/>
+      <c r="AK76" s="14"/>
+    </row>
+    <row r="77" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L77" s="10"/>
       <c r="M77" s="11" t="s">
         <v>21</v>
@@ -4030,8 +4367,24 @@
       <c r="U77" s="11"/>
       <c r="V77" s="15"/>
       <c r="W77" s="14"/>
-    </row>
-    <row r="78" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z77" s="10"/>
+      <c r="AA77" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB77" s="15"/>
+      <c r="AC77" s="15"/>
+      <c r="AD77" s="15"/>
+      <c r="AE77" s="15"/>
+      <c r="AF77" s="15"/>
+      <c r="AG77" s="15"/>
+      <c r="AH77" s="15">
+        <v>1.0863662592000001E-3</v>
+      </c>
+      <c r="AI77" s="11"/>
+      <c r="AJ77" s="15"/>
+      <c r="AK77" s="14"/>
+    </row>
+    <row r="78" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L78" s="10"/>
       <c r="M78" s="11" t="s">
         <v>22</v>
@@ -4048,8 +4401,24 @@
       <c r="U78" s="11"/>
       <c r="V78" s="15"/>
       <c r="W78" s="14"/>
-    </row>
-    <row r="79" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z78" s="10"/>
+      <c r="AA78" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB78" s="15"/>
+      <c r="AC78" s="15"/>
+      <c r="AD78" s="15"/>
+      <c r="AE78" s="15"/>
+      <c r="AF78" s="15"/>
+      <c r="AG78" s="15"/>
+      <c r="AH78" s="15">
+        <v>1.0863662591999901E-3</v>
+      </c>
+      <c r="AI78" s="11"/>
+      <c r="AJ78" s="15"/>
+      <c r="AK78" s="14"/>
+    </row>
+    <row r="79" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L79" s="10"/>
       <c r="M79" s="11"/>
       <c r="N79" s="11"/>
@@ -4062,8 +4431,20 @@
       <c r="U79" s="11"/>
       <c r="V79" s="11"/>
       <c r="W79" s="14"/>
-    </row>
-    <row r="80" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z79" s="10"/>
+      <c r="AA79" s="11"/>
+      <c r="AB79" s="11"/>
+      <c r="AC79" s="11"/>
+      <c r="AD79" s="11"/>
+      <c r="AE79" s="11"/>
+      <c r="AF79" s="11"/>
+      <c r="AG79" s="11"/>
+      <c r="AH79" s="11"/>
+      <c r="AI79" s="11"/>
+      <c r="AJ79" s="11"/>
+      <c r="AK79" s="14"/>
+    </row>
+    <row r="80" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L80" s="10"/>
       <c r="M80" s="11"/>
       <c r="N80" s="11"/>
@@ -4076,8 +4457,20 @@
       <c r="U80" s="11"/>
       <c r="V80" s="11"/>
       <c r="W80" s="14"/>
-    </row>
-    <row r="81" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z80" s="10"/>
+      <c r="AA80" s="11"/>
+      <c r="AB80" s="11"/>
+      <c r="AC80" s="11"/>
+      <c r="AD80" s="11"/>
+      <c r="AE80" s="11"/>
+      <c r="AF80" s="11"/>
+      <c r="AG80" s="11"/>
+      <c r="AH80" s="11"/>
+      <c r="AI80" s="11"/>
+      <c r="AJ80" s="11"/>
+      <c r="AK80" s="14"/>
+    </row>
+    <row r="81" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L81" s="10"/>
       <c r="M81" s="11" t="s">
         <v>25</v>
@@ -4104,8 +4497,34 @@
       <c r="U81" s="11"/>
       <c r="V81" s="11"/>
       <c r="W81" s="14"/>
-    </row>
-    <row r="82" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z81" s="10"/>
+      <c r="AA81" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB81" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC81" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD81" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE81" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF81" s="11"/>
+      <c r="AG81" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH81" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI81" s="11"/>
+      <c r="AJ81" s="11"/>
+      <c r="AK81" s="14"/>
+    </row>
+    <row r="82" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L82" s="10"/>
       <c r="M82" s="11" t="s">
         <v>28</v>
@@ -4113,7 +4532,7 @@
       <c r="N82" s="12">
         <v>2</v>
       </c>
-      <c r="O82" s="25">
+      <c r="O82" s="24">
         <v>264</v>
       </c>
       <c r="P82" s="12">
@@ -4123,17 +4542,43 @@
         <v>100000000</v>
       </c>
       <c r="R82" s="11"/>
-      <c r="S82" s="25">
+      <c r="S82" s="24">
         <v>2796.62592</v>
       </c>
-      <c r="T82" s="25" t="s">
+      <c r="T82" s="24" t="s">
         <v>34</v>
       </c>
       <c r="U82" s="11"/>
       <c r="V82" s="11"/>
       <c r="W82" s="14"/>
-    </row>
-    <row r="83" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z82" s="10"/>
+      <c r="AA82" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB82" s="12">
+        <v>2</v>
+      </c>
+      <c r="AC82" s="12">
+        <v>176</v>
+      </c>
+      <c r="AD82" s="12">
+        <v>1.25E-4</v>
+      </c>
+      <c r="AE82" s="13">
+        <v>100000000</v>
+      </c>
+      <c r="AF82" s="11"/>
+      <c r="AG82" s="22">
+        <v>2181.6115199999999</v>
+      </c>
+      <c r="AH82" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI82" s="11"/>
+      <c r="AJ82" s="11"/>
+      <c r="AK82" s="14"/>
+    </row>
+    <row r="83" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L83" s="10"/>
       <c r="M83" s="11"/>
       <c r="N83" s="11"/>
@@ -4146,8 +4591,20 @@
       <c r="U83" s="11"/>
       <c r="V83" s="11"/>
       <c r="W83" s="14"/>
-    </row>
-    <row r="84" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z83" s="10"/>
+      <c r="AA83" s="11"/>
+      <c r="AB83" s="11"/>
+      <c r="AC83" s="11"/>
+      <c r="AD83" s="11"/>
+      <c r="AE83" s="11"/>
+      <c r="AF83" s="11"/>
+      <c r="AG83" s="11"/>
+      <c r="AH83" s="11"/>
+      <c r="AI83" s="11"/>
+      <c r="AJ83" s="11"/>
+      <c r="AK83" s="14"/>
+    </row>
+    <row r="84" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L84" s="10"/>
       <c r="M84" s="11"/>
       <c r="N84" s="11"/>
@@ -4160,8 +4617,20 @@
       <c r="U84" s="11"/>
       <c r="V84" s="11"/>
       <c r="W84" s="14"/>
-    </row>
-    <row r="85" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z84" s="10"/>
+      <c r="AA84" s="11"/>
+      <c r="AB84" s="11"/>
+      <c r="AC84" s="11"/>
+      <c r="AD84" s="11"/>
+      <c r="AE84" s="11"/>
+      <c r="AF84" s="11"/>
+      <c r="AG84" s="11"/>
+      <c r="AH84" s="11"/>
+      <c r="AI84" s="11"/>
+      <c r="AJ84" s="11"/>
+      <c r="AK84" s="14"/>
+    </row>
+    <row r="85" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L85" s="10"/>
       <c r="M85" s="11" t="s">
         <v>15</v>
@@ -4190,8 +4659,36 @@
       <c r="U85" s="11"/>
       <c r="V85" s="11"/>
       <c r="W85" s="14"/>
-    </row>
-    <row r="86" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z85" s="10"/>
+      <c r="AA85" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB85" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC85" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD85" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE85" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF85" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG85" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH85" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI85" s="11"/>
+      <c r="AJ85" s="11"/>
+      <c r="AK85" s="14"/>
+    </row>
+    <row r="86" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L86" s="10"/>
       <c r="M86" s="11" t="s">
         <v>16</v>
@@ -4212,8 +4709,28 @@
       <c r="U86" s="11"/>
       <c r="V86" s="15"/>
       <c r="W86" s="14"/>
-    </row>
-    <row r="87" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z86" s="10"/>
+      <c r="AA86" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB86" s="15">
+        <v>2.1062446080000001E-4</v>
+      </c>
+      <c r="AC86" s="15">
+        <v>3.2178662400000001E-4</v>
+      </c>
+      <c r="AD86" s="15"/>
+      <c r="AE86" s="15"/>
+      <c r="AF86" s="15"/>
+      <c r="AG86" s="15"/>
+      <c r="AH86" s="15">
+        <v>5.3241108480000003E-4</v>
+      </c>
+      <c r="AI86" s="11"/>
+      <c r="AJ86" s="15"/>
+      <c r="AK86" s="14"/>
+    </row>
+    <row r="87" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L87" s="10"/>
       <c r="M87" s="11" t="s">
         <v>17</v>
@@ -4234,8 +4751,28 @@
       <c r="U87" s="11"/>
       <c r="V87" s="15"/>
       <c r="W87" s="14"/>
-    </row>
-    <row r="88" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z87" s="10"/>
+      <c r="AA87" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB87" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="AC87" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="AD87" s="15"/>
+      <c r="AE87" s="15"/>
+      <c r="AF87" s="15"/>
+      <c r="AG87" s="15"/>
+      <c r="AH87" s="15">
+        <v>3.5935999999999997E-4</v>
+      </c>
+      <c r="AI87" s="11"/>
+      <c r="AJ87" s="15"/>
+      <c r="AK87" s="14"/>
+    </row>
+    <row r="88" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L88" s="16" t="s">
         <v>0</v>
       </c>
@@ -4258,8 +4795,30 @@
       <c r="U88" s="11"/>
       <c r="V88" s="15"/>
       <c r="W88" s="14"/>
-    </row>
-    <row r="89" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z88" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA88" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB88" s="15">
+        <v>2.1062446080000001E-4</v>
+      </c>
+      <c r="AC88" s="15">
+        <v>3.2178662400000001E-4</v>
+      </c>
+      <c r="AD88" s="15"/>
+      <c r="AE88" s="15"/>
+      <c r="AF88" s="15"/>
+      <c r="AG88" s="15"/>
+      <c r="AH88" s="15">
+        <v>5.3241108480000003E-4</v>
+      </c>
+      <c r="AI88" s="11"/>
+      <c r="AJ88" s="15"/>
+      <c r="AK88" s="14"/>
+    </row>
+    <row r="89" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L89" s="10"/>
       <c r="M89" s="11" t="s">
         <v>19</v>
@@ -4280,8 +4839,28 @@
       <c r="U89" s="11"/>
       <c r="V89" s="15"/>
       <c r="W89" s="14"/>
-    </row>
-    <row r="90" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z89" s="10"/>
+      <c r="AA89" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB89" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="AC89" s="15">
+        <v>1.7967999999999999E-4</v>
+      </c>
+      <c r="AD89" s="15"/>
+      <c r="AE89" s="15"/>
+      <c r="AF89" s="15"/>
+      <c r="AG89" s="15"/>
+      <c r="AH89" s="15">
+        <v>3.5935999999999997E-4</v>
+      </c>
+      <c r="AI89" s="11"/>
+      <c r="AJ89" s="15"/>
+      <c r="AK89" s="14"/>
+    </row>
+    <row r="90" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L90" s="10"/>
       <c r="M90" s="11" t="s">
         <v>20</v>
@@ -4298,8 +4877,24 @@
       <c r="U90" s="11"/>
       <c r="V90" s="15"/>
       <c r="W90" s="14"/>
-    </row>
-    <row r="91" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z90" s="10"/>
+      <c r="AA90" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB90" s="15"/>
+      <c r="AC90" s="15"/>
+      <c r="AD90" s="15"/>
+      <c r="AE90" s="15"/>
+      <c r="AF90" s="15"/>
+      <c r="AG90" s="15"/>
+      <c r="AH90" s="15">
+        <v>3.339844608E-4</v>
+      </c>
+      <c r="AI90" s="11"/>
+      <c r="AJ90" s="15"/>
+      <c r="AK90" s="14"/>
+    </row>
+    <row r="91" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L91" s="10"/>
       <c r="M91" s="11" t="s">
         <v>21</v>
@@ -4316,8 +4911,24 @@
       <c r="U91" s="11"/>
       <c r="V91" s="15"/>
       <c r="W91" s="14"/>
-    </row>
-    <row r="92" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z91" s="10"/>
+      <c r="AA91" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB91" s="15"/>
+      <c r="AC91" s="15"/>
+      <c r="AD91" s="15"/>
+      <c r="AE91" s="15"/>
+      <c r="AF91" s="15"/>
+      <c r="AG91" s="15"/>
+      <c r="AH91" s="15">
+        <v>3.339844608E-4</v>
+      </c>
+      <c r="AI91" s="11"/>
+      <c r="AJ91" s="15"/>
+      <c r="AK91" s="14"/>
+    </row>
+    <row r="92" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L92" s="10"/>
       <c r="M92" s="11" t="s">
         <v>22</v>
@@ -4334,8 +4945,24 @@
       <c r="U92" s="11"/>
       <c r="V92" s="15"/>
       <c r="W92" s="14"/>
-    </row>
-    <row r="93" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z92" s="10"/>
+      <c r="AA92" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB92" s="15"/>
+      <c r="AC92" s="15"/>
+      <c r="AD92" s="15"/>
+      <c r="AE92" s="15"/>
+      <c r="AF92" s="15"/>
+      <c r="AG92" s="15"/>
+      <c r="AH92" s="15">
+        <v>3.339844608E-4</v>
+      </c>
+      <c r="AI92" s="11"/>
+      <c r="AJ92" s="15"/>
+      <c r="AK92" s="14"/>
+    </row>
+    <row r="93" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L93" s="18"/>
       <c r="M93" s="19"/>
       <c r="N93" s="19"/>
@@ -4348,8 +4975,20 @@
       <c r="U93" s="19"/>
       <c r="V93" s="19"/>
       <c r="W93" s="21"/>
-    </row>
-    <row r="96" spans="12:23" x14ac:dyDescent="0.3">
+      <c r="Z93" s="18"/>
+      <c r="AA93" s="19"/>
+      <c r="AB93" s="19"/>
+      <c r="AC93" s="19"/>
+      <c r="AD93" s="19"/>
+      <c r="AE93" s="19"/>
+      <c r="AF93" s="19"/>
+      <c r="AG93" s="19"/>
+      <c r="AH93" s="19"/>
+      <c r="AI93" s="19"/>
+      <c r="AJ93" s="19"/>
+      <c r="AK93" s="21"/>
+    </row>
+    <row r="96" spans="12:37" x14ac:dyDescent="0.3">
       <c r="L96" s="6"/>
       <c r="M96" s="7" t="s">
         <v>26</v>
@@ -4719,7 +5358,7 @@
       <c r="N113" s="12">
         <v>2</v>
       </c>
-      <c r="O113" s="25">
+      <c r="O113" s="24">
         <v>512</v>
       </c>
       <c r="P113" s="12">
@@ -4729,10 +5368,10 @@
         <v>100000000</v>
       </c>
       <c r="R113" s="11"/>
-      <c r="S113" s="25">
+      <c r="S113" s="24">
         <v>2823.2908799000002</v>
       </c>
-      <c r="T113" s="25" t="s">
+      <c r="T113" s="24" t="s">
         <v>35</v>
       </c>
       <c r="U113" s="11"/>
@@ -5337,7 +5976,7 @@
       <c r="N144" s="12">
         <v>2</v>
       </c>
-      <c r="O144" s="25">
+      <c r="O144" s="24">
         <v>780</v>
       </c>
       <c r="P144" s="12">
@@ -5347,10 +5986,10 @@
         <v>100000000</v>
       </c>
       <c r="R144" s="11"/>
-      <c r="S144" s="25">
+      <c r="S144" s="24">
         <v>19.968000000000501</v>
       </c>
-      <c r="T144" s="25" t="s">
+      <c r="T144" s="24" t="s">
         <v>36</v>
       </c>
       <c r="U144" s="11"/>
@@ -5576,7 +6215,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="14">
+  <tableParts count="16">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -5591,6 +6230,8 @@
     <tablePart r:id="rId13"/>
     <tablePart r:id="rId14"/>
     <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>